<commit_message>
plotting the two leads of the AHA database
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/AHA_database.xlsx
+++ b/R peak detection/beatdetection/AHA_database.xlsx
@@ -1,52 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofmora-my.sharepoint.com/personal/desilvawadk_19_uom_lk/Documents/Internship/ECG-beat-detection/R peak detection/beatdetection/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2BB1ED8477D5C18BE6CDCDCBC59025724C070037" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F80B7AB-D743-4EE0-8206-F648EBE52AAC}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="gfdug" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,21 +48,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -367,27 +409,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>8207</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>1248</v>
+      </c>
+      <c r="C1" t="n">
+        <v>1356</v>
+      </c>
+      <c r="D1" t="n">
+        <v>1244</v>
+      </c>
+      <c r="E1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" t="n">
+        <v>111</v>
+      </c>
+      <c r="G1" t="n">
+        <v>91.80811808118081</v>
+      </c>
+      <c r="H1" t="n">
+        <v>99.75942261427426</v>
+      </c>
+      <c r="I1" t="n">
+        <v>0.084070796460177</v>
+      </c>
+      <c r="J1" t="n">
+        <v>46.32402014732361</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>8209</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1972</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2025</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1971</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>53</v>
+      </c>
+      <c r="G2" t="n">
+        <v>97.38142292490119</v>
+      </c>
+      <c r="H2" t="n">
+        <v>100</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.02617283950617284</v>
+      </c>
+      <c r="J2" t="n">
+        <v>39.51032686233521</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed the threshold values for 250Hz sampling
Changed all three threshold values for the criterions and changed the R Peak checking window interval to 0.5s and 0.25s
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/AHA_database.xlsx
+++ b/R peak detection/beatdetection/AHA_database.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sgasu" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="C1" t="n">
         <v>1622</v>
@@ -456,7 +456,7 @@
         <v>1620</v>
       </c>
       <c r="E1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="n">
         <v>1</v>
@@ -465,13 +465,13 @@
         <v>99.93830968537939</v>
       </c>
       <c r="H1" t="n">
-        <v>99.75369458128078</v>
+        <v>99.81515711645102</v>
       </c>
       <c r="I1" t="n">
-        <v>0.003082614056720099</v>
+        <v>0.002466091245376079</v>
       </c>
       <c r="J1" t="n">
-        <v>57.12636828422546</v>
+        <v>92.78410625457764</v>
       </c>
     </row>
     <row r="2">
@@ -481,31 +481,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="C2" t="n">
         <v>2595</v>
       </c>
       <c r="D2" t="n">
-        <v>2594</v>
+        <v>2593</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>99.96144949884348</v>
       </c>
       <c r="H2" t="n">
         <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.0003853564547206166</v>
       </c>
       <c r="J2" t="n">
-        <v>44.51120710372925</v>
+        <v>85.88464260101318</v>
       </c>
     </row>
     <row r="3">
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>59.98539710044861</v>
+        <v>87.46213173866272</v>
       </c>
     </row>
     <row r="4">
@@ -549,31 +549,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2954</v>
+        <v>2956</v>
       </c>
       <c r="C4" t="n">
         <v>2974</v>
       </c>
       <c r="D4" t="n">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" t="n">
-        <v>99.26000672721158</v>
+        <v>99.22637066935755</v>
       </c>
       <c r="H4" t="n">
-        <v>99.93227226549271</v>
+        <v>99.83079526226734</v>
       </c>
       <c r="I4" t="n">
-        <v>0.008069939475453935</v>
+        <v>0.00941492938802959</v>
       </c>
       <c r="J4" t="n">
-        <v>62.39261889457703</v>
+        <v>120.8448188304901</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>100.2954154014587</v>
+        <v>90.32473945617676</v>
       </c>
     </row>
     <row r="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2122</v>
+        <v>2123</v>
       </c>
       <c r="C6" t="n">
         <v>2122</v>
@@ -626,7 +626,7 @@
         <v>2121</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -635,13 +635,13 @@
         <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>100</v>
+        <v>99.95287464655985</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>0.000471253534401508</v>
       </c>
       <c r="J6" t="n">
-        <v>79.23145008087158</v>
+        <v>102.7025241851807</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>69.70431470870972</v>
+        <v>78.43877506256104</v>
       </c>
     </row>
     <row r="8">
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>71.15496706962585</v>
+        <v>104.8826658725739</v>
       </c>
     </row>
     <row r="9">
@@ -719,31 +719,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3581</v>
+        <v>3582</v>
       </c>
       <c r="C9" t="n">
         <v>3582</v>
       </c>
       <c r="D9" t="n">
-        <v>3579</v>
+        <v>3580</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>99.94414967886065</v>
+        <v>99.97207483943032</v>
       </c>
       <c r="H9" t="n">
-        <v>99.97206703910615</v>
+        <v>99.97207483943032</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0008375209380234506</v>
+        <v>0.0005583472920156337</v>
       </c>
       <c r="J9" t="n">
-        <v>38.53868055343628</v>
+        <v>147.9974005222321</v>
       </c>
     </row>
     <row r="10">
@@ -753,7 +753,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2008</v>
+        <v>2026</v>
       </c>
       <c r="C10" t="n">
         <v>1997</v>
@@ -762,7 +762,7 @@
         <v>1991</v>
       </c>
       <c r="E10" t="n">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F10" t="n">
         <v>5</v>
@@ -771,13 +771,13 @@
         <v>99.74949899799599</v>
       </c>
       <c r="H10" t="n">
-        <v>99.20279023418037</v>
+        <v>98.32098765432099</v>
       </c>
       <c r="I10" t="n">
-        <v>0.01051577366049074</v>
+        <v>0.01952929394091137</v>
       </c>
       <c r="J10" t="n">
-        <v>99.93582034111023</v>
+        <v>173.7748024463654</v>
       </c>
     </row>
     <row r="11">
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>45.14150619506836</v>
+        <v>92.80263185501099</v>
       </c>
     </row>
     <row r="12">
@@ -821,31 +821,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2413</v>
+        <v>2415</v>
       </c>
       <c r="C12" t="n">
         <v>2414</v>
       </c>
       <c r="D12" t="n">
-        <v>2412</v>
+        <v>2413</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>99.95855781185247</v>
+        <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>100</v>
+        <v>99.95857497928749</v>
       </c>
       <c r="I12" t="n">
         <v>0.0004142502071251035</v>
       </c>
       <c r="J12" t="n">
-        <v>95.002445936203</v>
+        <v>132.6538851261139</v>
       </c>
     </row>
     <row r="13">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3415</v>
+        <v>3423</v>
       </c>
       <c r="C13" t="n">
         <v>3511</v>
@@ -864,7 +864,7 @@
         <v>3402</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F13" t="n">
         <v>108</v>
@@ -873,13 +873,13 @@
         <v>96.92307692307692</v>
       </c>
       <c r="H13" t="n">
-        <v>99.64850615114236</v>
+        <v>99.41554646405611</v>
       </c>
       <c r="I13" t="n">
-        <v>0.03417829678154372</v>
+        <v>0.0364568499003133</v>
       </c>
       <c r="J13" t="n">
-        <v>104.2177672386169</v>
+        <v>218.8199925422668</v>
       </c>
     </row>
     <row r="14">
@@ -889,7 +889,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="C14" t="n">
         <v>1628</v>
@@ -898,7 +898,7 @@
         <v>1627</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -907,13 +907,13 @@
         <v>100</v>
       </c>
       <c r="H14" t="n">
-        <v>99.69362745098039</v>
+        <v>99.75475168608216</v>
       </c>
       <c r="I14" t="n">
-        <v>0.003071253071253071</v>
+        <v>0.002457002457002457</v>
       </c>
       <c r="J14" t="n">
-        <v>80.66756176948547</v>
+        <v>105.687805891037</v>
       </c>
     </row>
     <row r="15">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="C15" t="n">
         <v>1613</v>
@@ -932,7 +932,7 @@
         <v>1612</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -941,13 +941,13 @@
         <v>100</v>
       </c>
       <c r="H15" t="n">
-        <v>100</v>
+        <v>99.93800371977682</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>0.0006199628022318661</v>
       </c>
       <c r="J15" t="n">
-        <v>112.3315939903259</v>
+        <v>124.9002187252045</v>
       </c>
     </row>
     <row r="16">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>104.3713936805725</v>
+        <v>136.8912932872772</v>
       </c>
     </row>
     <row r="17">
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2854</v>
+        <v>2855</v>
       </c>
       <c r="C17" t="n">
         <v>2854</v>
@@ -1000,7 +1000,7 @@
         <v>2853</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -1009,13 +1009,13 @@
         <v>100</v>
       </c>
       <c r="H17" t="n">
-        <v>100</v>
+        <v>99.96496145760337</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>0.000350385423966363</v>
       </c>
       <c r="J17" t="n">
-        <v>84.89576387405396</v>
+        <v>135.2376980781555</v>
       </c>
     </row>
     <row r="18">
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>112.4936456680298</v>
+        <v>146.0154478549957</v>
       </c>
     </row>
     <row r="19">
@@ -1059,7 +1059,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2536</v>
+        <v>2592</v>
       </c>
       <c r="C19" t="n">
         <v>2537</v>
@@ -1068,7 +1068,7 @@
         <v>2534</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="F19" t="n">
         <v>2</v>
@@ -1077,13 +1077,13 @@
         <v>99.9211356466877</v>
       </c>
       <c r="H19" t="n">
-        <v>99.96055226824457</v>
+        <v>97.80007719027402</v>
       </c>
       <c r="I19" t="n">
-        <v>0.001182499014584154</v>
+        <v>0.02325581395348837</v>
       </c>
       <c r="J19" t="n">
-        <v>180.8852071762085</v>
+        <v>221.7416796684265</v>
       </c>
     </row>
     <row r="20">
@@ -1093,31 +1093,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2174</v>
+        <v>2175</v>
       </c>
       <c r="C20" t="n">
         <v>2177</v>
       </c>
       <c r="D20" t="n">
-        <v>2172</v>
+        <v>2173</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20" t="n">
-        <v>99.81617647058823</v>
+        <v>99.86213235294117</v>
       </c>
       <c r="H20" t="n">
-        <v>99.95398067188219</v>
+        <v>99.95400183992641</v>
       </c>
       <c r="I20" t="n">
-        <v>0.002296738631143776</v>
+        <v>0.001837390904915021</v>
       </c>
       <c r="J20" t="n">
-        <v>172.1606252193451</v>
+        <v>216.0197570323944</v>
       </c>
     </row>
     <row r="21">
@@ -1133,25 +1133,25 @@
         <v>2943</v>
       </c>
       <c r="D21" t="n">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21" t="n">
-        <v>99.96600951733515</v>
+        <v>99.93201903467029</v>
       </c>
       <c r="H21" t="n">
-        <v>99.96600951733515</v>
+        <v>99.93201903467029</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0006795786612300374</v>
+        <v>0.001359157322460075</v>
       </c>
       <c r="J21" t="n">
-        <v>203.5486257076263</v>
+        <v>240.9267868995667</v>
       </c>
     </row>
     <row r="22">
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1952</v>
+        <v>1956</v>
       </c>
       <c r="C22" t="n">
         <v>1950</v>
@@ -1170,7 +1170,7 @@
         <v>1949</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1179,13 +1179,13 @@
         <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>99.89748846745259</v>
+        <v>99.69309462915601</v>
       </c>
       <c r="I22" t="n">
-        <v>0.001025641025641026</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="J22" t="n">
-        <v>131.9613223075867</v>
+        <v>145.673201084137</v>
       </c>
     </row>
     <row r="23">
@@ -1195,31 +1195,31 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1878</v>
+        <v>1889</v>
       </c>
       <c r="C23" t="n">
         <v>1878</v>
       </c>
       <c r="D23" t="n">
-        <v>1877</v>
+        <v>1871</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G23" t="n">
-        <v>100</v>
+        <v>99.6803409696324</v>
       </c>
       <c r="H23" t="n">
-        <v>100</v>
+        <v>99.09957627118644</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>0.01224707135250266</v>
       </c>
       <c r="J23" t="n">
-        <v>194.1588733196259</v>
+        <v>241.0386998653412</v>
       </c>
     </row>
     <row r="24">
@@ -1229,31 +1229,31 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="C24" t="n">
         <v>1784</v>
       </c>
       <c r="D24" t="n">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>99.94391475042065</v>
+        <v>99.88782950084128</v>
       </c>
       <c r="H24" t="n">
         <v>100</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0005605381165919282</v>
+        <v>0.001121076233183856</v>
       </c>
       <c r="J24" t="n">
-        <v>141.826144695282</v>
+        <v>159.7406003475189</v>
       </c>
     </row>
     <row r="25">
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>117.6158657073975</v>
+        <v>137.2374458312988</v>
       </c>
     </row>
     <row r="26">
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2324</v>
+        <v>2330</v>
       </c>
       <c r="C26" t="n">
         <v>2324</v>
@@ -1306,7 +1306,7 @@
         <v>2323</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1315,13 +1315,13 @@
         <v>100</v>
       </c>
       <c r="H26" t="n">
-        <v>100</v>
+        <v>99.74237870330614</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>0.002581755593803787</v>
       </c>
       <c r="J26" t="n">
-        <v>169.5841147899628</v>
+        <v>212.4686231613159</v>
       </c>
     </row>
     <row r="27">
@@ -1331,7 +1331,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2424</v>
+        <v>2425</v>
       </c>
       <c r="C27" t="n">
         <v>2424</v>
@@ -1340,7 +1340,7 @@
         <v>2423</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1349,13 +1349,13 @@
         <v>100</v>
       </c>
       <c r="H27" t="n">
-        <v>100</v>
+        <v>99.95874587458746</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>0.0004125412541254125</v>
       </c>
       <c r="J27" t="n">
-        <v>213.6410274505615</v>
+        <v>227.0689141750336</v>
       </c>
     </row>
     <row r="28">
@@ -1389,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>256.3792386054993</v>
+        <v>257.8162310123444</v>
       </c>
     </row>
     <row r="29">
@@ -1399,31 +1399,31 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2449</v>
+        <v>2459</v>
       </c>
       <c r="C29" t="n">
         <v>2472</v>
       </c>
       <c r="D29" t="n">
-        <v>2448</v>
+        <v>2450</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F29" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G29" t="n">
-        <v>99.0692027519223</v>
+        <v>99.15014164305948</v>
       </c>
       <c r="H29" t="n">
-        <v>100</v>
+        <v>99.67453213995118</v>
       </c>
       <c r="I29" t="n">
-        <v>0.009304207119741101</v>
+        <v>0.01173139158576052</v>
       </c>
       <c r="J29" t="n">
-        <v>149.4029595851898</v>
+        <v>173.8208084106445</v>
       </c>
     </row>
     <row r="30">
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>170.4144566059113</v>
+        <v>183.9332089424133</v>
       </c>
     </row>
     <row r="31">
@@ -1467,31 +1467,31 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2366</v>
+        <v>2371</v>
       </c>
       <c r="C31" t="n">
         <v>2376</v>
       </c>
       <c r="D31" t="n">
-        <v>2365</v>
+        <v>2366</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G31" t="n">
-        <v>99.57894736842105</v>
+        <v>99.62105263157895</v>
       </c>
       <c r="H31" t="n">
-        <v>100</v>
+        <v>99.83122362869199</v>
       </c>
       <c r="I31" t="n">
-        <v>0.004208754208754209</v>
+        <v>0.005471380471380472</v>
       </c>
       <c r="J31" t="n">
-        <v>143.0126583576202</v>
+        <v>162.4402174949646</v>
       </c>
     </row>
     <row r="32">
@@ -1525,7 +1525,7 @@
         <v>0.0003872966692486445</v>
       </c>
       <c r="J32" t="n">
-        <v>232.4607458114624</v>
+        <v>249.9720501899719</v>
       </c>
     </row>
     <row r="33">
@@ -1541,25 +1541,25 @@
         <v>2258</v>
       </c>
       <c r="D33" t="n">
-        <v>2257</v>
+        <v>2253</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G33" t="n">
-        <v>100</v>
+        <v>99.8227735932654</v>
       </c>
       <c r="H33" t="n">
-        <v>100</v>
+        <v>99.8227735932654</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>0.00354295837023915</v>
       </c>
       <c r="J33" t="n">
-        <v>132.0851335525513</v>
+        <v>153.5061819553375</v>
       </c>
     </row>
     <row r="34">
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1453</v>
+        <v>1456</v>
       </c>
       <c r="C34" t="n">
         <v>1452</v>
@@ -1578,7 +1578,7 @@
         <v>1451</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1587,13 +1587,13 @@
         <v>100</v>
       </c>
       <c r="H34" t="n">
-        <v>99.93112947658402</v>
+        <v>99.72508591065292</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0006887052341597796</v>
+        <v>0.002754820936639119</v>
       </c>
       <c r="J34" t="n">
-        <v>219.3314127922058</v>
+        <v>236.7128043174744</v>
       </c>
     </row>
     <row r="35">
@@ -1603,31 +1603,31 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1944</v>
+        <v>1947</v>
       </c>
       <c r="C35" t="n">
         <v>1947</v>
       </c>
       <c r="D35" t="n">
-        <v>1943</v>
+        <v>1946</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>99.84583761562179</v>
+        <v>100</v>
       </c>
       <c r="H35" t="n">
         <v>100</v>
       </c>
       <c r="I35" t="n">
-        <v>0.001540832049306626</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>146.004891872406</v>
+        <v>157.3932671546936</v>
       </c>
     </row>
     <row r="36">
@@ -1637,31 +1637,31 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3520</v>
+        <v>3524</v>
       </c>
       <c r="C36" t="n">
         <v>3520</v>
       </c>
       <c r="D36" t="n">
-        <v>3490</v>
+        <v>3504</v>
       </c>
       <c r="E36" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F36" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="G36" t="n">
-        <v>99.17590224495595</v>
+        <v>99.57374254049446</v>
       </c>
       <c r="H36" t="n">
-        <v>99.17590224495595</v>
+        <v>99.46068691456145</v>
       </c>
       <c r="I36" t="n">
-        <v>0.01647727272727273</v>
+        <v>0.009659090909090909</v>
       </c>
       <c r="J36" t="n">
-        <v>146.4537315368652</v>
+        <v>284.1411597728729</v>
       </c>
     </row>
     <row r="37">
@@ -1671,31 +1671,31 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1879</v>
+        <v>1882</v>
       </c>
       <c r="C37" t="n">
         <v>1878</v>
       </c>
       <c r="D37" t="n">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="E37" t="n">
+        <v>5</v>
+      </c>
+      <c r="F37" t="n">
         <v>1</v>
       </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
       <c r="G37" t="n">
-        <v>100</v>
+        <v>99.94672349493874</v>
       </c>
       <c r="H37" t="n">
-        <v>99.94675186368477</v>
+        <v>99.73418394471027</v>
       </c>
       <c r="I37" t="n">
-        <v>0.0005324813631522897</v>
+        <v>0.003194888178913738</v>
       </c>
       <c r="J37" t="n">
-        <v>196.2306437492371</v>
+        <v>228.9701895713806</v>
       </c>
     </row>
     <row r="38">
@@ -1729,7 +1729,7 @@
         <v>0.002530577815267819</v>
       </c>
       <c r="J38" t="n">
-        <v>245.413859128952</v>
+        <v>284.8226659297943</v>
       </c>
     </row>
     <row r="39">
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>119.5019459724426</v>
+        <v>136.9302062988281</v>
       </c>
     </row>
     <row r="40">
@@ -1773,31 +1773,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2184</v>
+        <v>2243</v>
       </c>
       <c r="C40" t="n">
         <v>2257</v>
       </c>
       <c r="D40" t="n">
-        <v>2182</v>
+        <v>2241</v>
       </c>
       <c r="E40" t="n">
         <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="G40" t="n">
-        <v>96.71985815602837</v>
+        <v>99.33510638297872</v>
       </c>
       <c r="H40" t="n">
-        <v>99.9541914796152</v>
+        <v>99.95539696699376</v>
       </c>
       <c r="I40" t="n">
-        <v>0.03322995126273815</v>
+        <v>0.007089056269384138</v>
       </c>
       <c r="J40" t="n">
-        <v>108.9764442443848</v>
+        <v>123.6139595508575</v>
       </c>
     </row>
     <row r="41">
@@ -1807,31 +1807,31 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2350</v>
+        <v>2351</v>
       </c>
       <c r="C41" t="n">
         <v>2351</v>
       </c>
       <c r="D41" t="n">
-        <v>2349</v>
+        <v>2319</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="G41" t="n">
-        <v>99.95744680851064</v>
+        <v>98.68085106382979</v>
       </c>
       <c r="H41" t="n">
-        <v>100</v>
+        <v>98.68085106382979</v>
       </c>
       <c r="I41" t="n">
-        <v>0.0004253509145044662</v>
+        <v>0.0263717566992769</v>
       </c>
       <c r="J41" t="n">
-        <v>248.7543003559113</v>
+        <v>277.9519579410553</v>
       </c>
     </row>
     <row r="42">
@@ -1865,7 +1865,7 @@
         <v>0.0004212299915754001</v>
       </c>
       <c r="J42" t="n">
-        <v>183.7958388328552</v>
+        <v>218.5389811992645</v>
       </c>
     </row>
     <row r="43">
@@ -1899,7 +1899,7 @@
         <v>0.0004372540445999126</v>
       </c>
       <c r="J43" t="n">
-        <v>229.5102982521057</v>
+        <v>271.5392079353333</v>
       </c>
     </row>
     <row r="44">
@@ -1915,25 +1915,25 @@
         <v>1806</v>
       </c>
       <c r="D44" t="n">
-        <v>1805</v>
+        <v>1790</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G44" t="n">
-        <v>100</v>
+        <v>99.16897506925208</v>
       </c>
       <c r="H44" t="n">
-        <v>100</v>
+        <v>99.16897506925208</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>0.01661129568106312</v>
       </c>
       <c r="J44" t="n">
-        <v>217.8969798088074</v>
+        <v>232.0619854927063</v>
       </c>
     </row>
     <row r="45">
@@ -1943,31 +1943,31 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2067</v>
+        <v>2070</v>
       </c>
       <c r="C45" t="n">
         <v>2068</v>
       </c>
       <c r="D45" t="n">
-        <v>2066</v>
+        <v>2067</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>99.95162070633769</v>
+        <v>100</v>
       </c>
       <c r="H45" t="n">
-        <v>100</v>
+        <v>99.90333494441759</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0004835589941972921</v>
+        <v>0.0009671179883945841</v>
       </c>
       <c r="J45" t="n">
-        <v>227.9730706214905</v>
+        <v>286.9822735786438</v>
       </c>
     </row>
     <row r="46">
@@ -1977,31 +1977,31 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2922</v>
+        <v>2913</v>
       </c>
       <c r="C46" t="n">
         <v>2923</v>
       </c>
       <c r="D46" t="n">
-        <v>2921</v>
+        <v>2911</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G46" t="n">
-        <v>99.96577686516085</v>
+        <v>99.62354551676934</v>
       </c>
       <c r="H46" t="n">
-        <v>100</v>
+        <v>99.96565934065934</v>
       </c>
       <c r="I46" t="n">
-        <v>0.0003421142661648991</v>
+        <v>0.004105371193978789</v>
       </c>
       <c r="J46" t="n">
-        <v>247.1438779830933</v>
+        <v>304.0650587081909</v>
       </c>
     </row>
     <row r="47">
@@ -2011,31 +2011,31 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1845</v>
+        <v>1863</v>
       </c>
       <c r="C47" t="n">
         <v>1845</v>
       </c>
       <c r="D47" t="n">
-        <v>1842</v>
+        <v>1834</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="F47" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G47" t="n">
-        <v>99.89154013015184</v>
+        <v>99.45770065075922</v>
       </c>
       <c r="H47" t="n">
-        <v>99.89154013015184</v>
+        <v>98.49624060150376</v>
       </c>
       <c r="I47" t="n">
-        <v>0.002168021680216802</v>
+        <v>0.02059620596205962</v>
       </c>
       <c r="J47" t="n">
-        <v>251.8318390846252</v>
+        <v>295.8240525722504</v>
       </c>
     </row>
     <row r="48">
@@ -2069,7 +2069,7 @@
         <v>0.0009242144177449168</v>
       </c>
       <c r="J48" t="n">
-        <v>232.6140594482422</v>
+        <v>255.9696805477142</v>
       </c>
     </row>
     <row r="49">
@@ -2103,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>290.3382065296173</v>
+        <v>326.4495222568512</v>
       </c>
     </row>
     <row r="50">
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>442.078052520752</v>
+        <v>465.9692249298096</v>
       </c>
     </row>
     <row r="51">
@@ -2171,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>340.8398251533508</v>
+        <v>358.5515220165253</v>
       </c>
     </row>
     <row r="52">
@@ -2181,31 +2181,31 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2695</v>
+        <v>2696</v>
       </c>
       <c r="C52" t="n">
         <v>2698</v>
       </c>
       <c r="D52" t="n">
-        <v>2694</v>
+        <v>2684</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F52" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G52" t="n">
-        <v>99.88876529477197</v>
+        <v>99.51798294401186</v>
       </c>
       <c r="H52" t="n">
-        <v>100</v>
+        <v>99.59183673469387</v>
       </c>
       <c r="I52" t="n">
-        <v>0.001111934766493699</v>
+        <v>0.008895478131949592</v>
       </c>
       <c r="J52" t="n">
-        <v>339.1537983417511</v>
+        <v>367.5740327835083</v>
       </c>
     </row>
     <row r="53">
@@ -2215,7 +2215,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2251</v>
+        <v>2254</v>
       </c>
       <c r="C53" t="n">
         <v>2251</v>
@@ -2224,7 +2224,7 @@
         <v>2250</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -2233,13 +2233,13 @@
         <v>100</v>
       </c>
       <c r="H53" t="n">
-        <v>100</v>
+        <v>99.86684420772303</v>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>0.001332741003998223</v>
       </c>
       <c r="J53" t="n">
-        <v>332.6028652191162</v>
+        <v>363.5812191963196</v>
       </c>
     </row>
     <row r="54">
@@ -2249,31 +2249,31 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2294</v>
+        <v>2299</v>
       </c>
       <c r="C54" t="n">
         <v>2294</v>
       </c>
       <c r="D54" t="n">
-        <v>2293</v>
+        <v>2267</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G54" t="n">
-        <v>100</v>
+        <v>98.86611426079372</v>
       </c>
       <c r="H54" t="n">
-        <v>100</v>
+        <v>98.65100087032202</v>
       </c>
       <c r="I54" t="n">
-        <v>0</v>
+        <v>0.02484742807323452</v>
       </c>
       <c r="J54" t="n">
-        <v>439.0658259391785</v>
+        <v>474.1692237854004</v>
       </c>
     </row>
     <row r="55">
@@ -2283,31 +2283,31 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>2780</v>
+        <v>2779</v>
       </c>
       <c r="C55" t="n">
         <v>2785</v>
       </c>
       <c r="D55" t="n">
-        <v>2776</v>
+        <v>2777</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G55" t="n">
-        <v>99.71264367816092</v>
+        <v>99.7485632183908</v>
       </c>
       <c r="H55" t="n">
-        <v>99.8920474991004</v>
+        <v>99.96400287976962</v>
       </c>
       <c r="I55" t="n">
-        <v>0.003949730700179534</v>
+        <v>0.002872531418312388</v>
       </c>
       <c r="J55" t="n">
-        <v>161.3858320713043</v>
+        <v>182.9815897941589</v>
       </c>
     </row>
     <row r="56">
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>326.9828114509583</v>
+        <v>349.4402720928192</v>
       </c>
     </row>
     <row r="57">
@@ -2357,25 +2357,25 @@
         <v>2359</v>
       </c>
       <c r="D57" t="n">
-        <v>2358</v>
+        <v>2357</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" t="n">
-        <v>100</v>
+        <v>99.95759117896523</v>
       </c>
       <c r="H57" t="n">
-        <v>100</v>
+        <v>99.95759117896523</v>
       </c>
       <c r="I57" t="n">
-        <v>0</v>
+        <v>0.000847816871555744</v>
       </c>
       <c r="J57" t="n">
-        <v>193.0121486186981</v>
+        <v>227.7234578132629</v>
       </c>
     </row>
     <row r="58">
@@ -2385,7 +2385,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>2505</v>
+        <v>2502</v>
       </c>
       <c r="C58" t="n">
         <v>2500</v>
@@ -2394,7 +2394,7 @@
         <v>2499</v>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -2403,13 +2403,13 @@
         <v>100</v>
       </c>
       <c r="H58" t="n">
-        <v>99.80031948881789</v>
+        <v>99.92003198720512</v>
       </c>
       <c r="I58" t="n">
-        <v>0.002</v>
+        <v>0.0008</v>
       </c>
       <c r="J58" t="n">
-        <v>411.6667761802673</v>
+        <v>442.980672121048</v>
       </c>
     </row>
     <row r="59">
@@ -2419,31 +2419,31 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>3289</v>
+        <v>3294</v>
       </c>
       <c r="C59" t="n">
         <v>3289</v>
       </c>
       <c r="D59" t="n">
-        <v>3288</v>
+        <v>3283</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G59" t="n">
-        <v>100</v>
+        <v>99.84793187347933</v>
       </c>
       <c r="H59" t="n">
-        <v>100</v>
+        <v>99.69632553902217</v>
       </c>
       <c r="I59" t="n">
-        <v>0</v>
+        <v>0.004560656734569778</v>
       </c>
       <c r="J59" t="n">
-        <v>224.4549751281738</v>
+        <v>333.7351341247559</v>
       </c>
     </row>
     <row r="60">
@@ -2453,31 +2453,31 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>3154</v>
+        <v>3163</v>
       </c>
       <c r="C60" t="n">
         <v>3164</v>
       </c>
       <c r="D60" t="n">
-        <v>3153</v>
+        <v>3158</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G60" t="n">
-        <v>99.68384445147012</v>
+        <v>99.84192222573506</v>
       </c>
       <c r="H60" t="n">
-        <v>100</v>
+        <v>99.87349778621126</v>
       </c>
       <c r="I60" t="n">
-        <v>0.00316055625790139</v>
+        <v>0.002844500632111252</v>
       </c>
       <c r="J60" t="n">
-        <v>234.5104565620422</v>
+        <v>327.6184418201447</v>
       </c>
     </row>
     <row r="61">
@@ -2511,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>432.3569734096527</v>
+        <v>479.7675290107727</v>
       </c>
     </row>
     <row r="62">
@@ -2521,7 +2521,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2533</v>
+        <v>2534</v>
       </c>
       <c r="C62" t="n">
         <v>2533</v>
@@ -2530,7 +2530,7 @@
         <v>2531</v>
       </c>
       <c r="E62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
         <v>1</v>
@@ -2539,13 +2539,13 @@
         <v>99.96050552922591</v>
       </c>
       <c r="H62" t="n">
-        <v>99.96050552922591</v>
+        <v>99.92104224240032</v>
       </c>
       <c r="I62" t="n">
-        <v>0.0007895775759968417</v>
+        <v>0.001184366363995263</v>
       </c>
       <c r="J62" t="n">
-        <v>205.7845056056976</v>
+        <v>246.7846231460571</v>
       </c>
     </row>
     <row r="63">
@@ -2555,31 +2555,31 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="C63" t="n">
         <v>1927</v>
       </c>
       <c r="D63" t="n">
-        <v>1918</v>
+        <v>1919</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G63" t="n">
-        <v>99.5846313603323</v>
+        <v>99.63655244029076</v>
       </c>
       <c r="H63" t="n">
         <v>100</v>
       </c>
       <c r="I63" t="n">
-        <v>0.004151530877010898</v>
+        <v>0.003632589517384536</v>
       </c>
       <c r="J63" t="n">
-        <v>197.7857949733734</v>
+        <v>216.4848577976227</v>
       </c>
     </row>
     <row r="64">
@@ -2589,31 +2589,31 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2434</v>
+        <v>2437</v>
       </c>
       <c r="C64" t="n">
         <v>2437</v>
       </c>
       <c r="D64" t="n">
-        <v>2425</v>
+        <v>2434</v>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F64" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G64" t="n">
-        <v>99.54844006568145</v>
+        <v>99.91789819376027</v>
       </c>
       <c r="H64" t="n">
-        <v>99.67118783394986</v>
+        <v>99.91789819376027</v>
       </c>
       <c r="I64" t="n">
-        <v>0.007796471070988921</v>
+        <v>0.00164136233073451</v>
       </c>
       <c r="J64" t="n">
-        <v>354.5041198730469</v>
+        <v>380.8764493465424</v>
       </c>
     </row>
     <row r="65">
@@ -2623,31 +2623,31 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>3105</v>
+        <v>3107</v>
       </c>
       <c r="C65" t="n">
         <v>3109</v>
       </c>
       <c r="D65" t="n">
-        <v>3104</v>
+        <v>3099</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F65" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G65" t="n">
-        <v>99.87129987129987</v>
+        <v>99.7104247104247</v>
       </c>
       <c r="H65" t="n">
-        <v>100</v>
+        <v>99.77462974887315</v>
       </c>
       <c r="I65" t="n">
-        <v>0.001286587327114828</v>
+        <v>0.005146349308459312</v>
       </c>
       <c r="J65" t="n">
-        <v>400.4975786209106</v>
+        <v>460.5091700553894</v>
       </c>
     </row>
     <row r="66">
@@ -2657,7 +2657,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2337</v>
+        <v>2338</v>
       </c>
       <c r="C66" t="n">
         <v>2340</v>
@@ -2666,7 +2666,7 @@
         <v>2336</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" t="n">
         <v>3</v>
@@ -2675,13 +2675,13 @@
         <v>99.87174005985464</v>
       </c>
       <c r="H66" t="n">
-        <v>100</v>
+        <v>99.95721009841678</v>
       </c>
       <c r="I66" t="n">
-        <v>0.001282051282051282</v>
+        <v>0.001709401709401709</v>
       </c>
       <c r="J66" t="n">
-        <v>248.4117677211761</v>
+        <v>308.5487623214722</v>
       </c>
     </row>
     <row r="67">
@@ -2715,7 +2715,7 @@
         <v>0.0006389776357827476</v>
       </c>
       <c r="J67" t="n">
-        <v>258.4243924617767</v>
+        <v>282.1427466869354</v>
       </c>
     </row>
     <row r="68">
@@ -2725,31 +2725,31 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2899</v>
+        <v>2908</v>
       </c>
       <c r="C68" t="n">
         <v>2897</v>
       </c>
       <c r="D68" t="n">
-        <v>2861</v>
+        <v>2874</v>
       </c>
       <c r="E68" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F68" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G68" t="n">
-        <v>98.79143646408839</v>
+        <v>99.24033149171271</v>
       </c>
       <c r="H68" t="n">
-        <v>98.7232574189096</v>
+        <v>98.86480908152735</v>
       </c>
       <c r="I68" t="n">
-        <v>0.02485329651363479</v>
+        <v>0.01898515705902658</v>
       </c>
       <c r="J68" t="n">
-        <v>349.5400116443634</v>
+        <v>470.2379167079926</v>
       </c>
     </row>
     <row r="69">
@@ -2759,31 +2759,31 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="C69" t="n">
         <v>1753</v>
       </c>
       <c r="D69" t="n">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
       </c>
       <c r="F69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G69" t="n">
-        <v>99.60045662100457</v>
+        <v>99.65753424657534</v>
       </c>
       <c r="H69" t="n">
-        <v>99.94272623138602</v>
+        <v>99.94275901545507</v>
       </c>
       <c r="I69" t="n">
-        <v>0.004563605248146035</v>
+        <v>0.003993154592127781</v>
       </c>
       <c r="J69" t="n">
-        <v>347.7069363594055</v>
+        <v>375.9237840175629</v>
       </c>
     </row>
     <row r="70">
@@ -2793,31 +2793,31 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="C70" t="n">
         <v>1459</v>
       </c>
       <c r="D70" t="n">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
       </c>
       <c r="F70" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G70" t="n">
-        <v>99.58847736625515</v>
+        <v>99.65706447187928</v>
       </c>
       <c r="H70" t="n">
-        <v>99.93117687543014</v>
+        <v>99.93122420907841</v>
       </c>
       <c r="I70" t="n">
-        <v>0.004797806716929404</v>
+        <v>0.00411240575736806</v>
       </c>
       <c r="J70" t="n">
-        <v>433.9890723228455</v>
+        <v>475.0378057956696</v>
       </c>
     </row>
     <row r="71">
@@ -2827,31 +2827,31 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1750</v>
+        <v>1762</v>
       </c>
       <c r="C71" t="n">
         <v>1787</v>
       </c>
       <c r="D71" t="n">
-        <v>1745</v>
+        <v>1755</v>
       </c>
       <c r="E71" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F71" t="n">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G71" t="n">
-        <v>97.64969222160045</v>
+        <v>98.20928931169558</v>
       </c>
       <c r="H71" t="n">
-        <v>99.77129788450543</v>
+        <v>99.65928449744463</v>
       </c>
       <c r="I71" t="n">
-        <v>0.02574146614437605</v>
+        <v>0.021264689423615</v>
       </c>
       <c r="J71" t="n">
-        <v>176.9270191192627</v>
+        <v>203.6996734142303</v>
       </c>
     </row>
     <row r="72">
@@ -2861,31 +2861,31 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>1523</v>
+        <v>1546</v>
       </c>
       <c r="C72" t="n">
         <v>1567</v>
       </c>
       <c r="D72" t="n">
-        <v>1522</v>
+        <v>1542</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="G72" t="n">
-        <v>97.19029374201789</v>
+        <v>98.46743295019157</v>
       </c>
       <c r="H72" t="n">
-        <v>100</v>
+        <v>99.80582524271844</v>
       </c>
       <c r="I72" t="n">
-        <v>0.02807913209955329</v>
+        <v>0.01723037651563497</v>
       </c>
       <c r="J72" t="n">
-        <v>338.6903302669525</v>
+        <v>416.5431251525879</v>
       </c>
     </row>
     <row r="73">
@@ -2895,7 +2895,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="C73" t="n">
         <v>920</v>
@@ -2904,7 +2904,7 @@
         <v>908</v>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
         <v>11</v>
@@ -2913,13 +2913,13 @@
         <v>98.80304678998912</v>
       </c>
       <c r="H73" t="n">
-        <v>99.78021978021978</v>
+        <v>99.67069154774973</v>
       </c>
       <c r="I73" t="n">
-        <v>0.0141304347826087</v>
+        <v>0.01521739130434783</v>
       </c>
       <c r="J73" t="n">
-        <v>265.6977455615997</v>
+        <v>306.2742254734039</v>
       </c>
     </row>
     <row r="74">
@@ -2929,7 +2929,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="C74" t="n">
         <v>1143</v>
@@ -2938,7 +2938,7 @@
         <v>1121</v>
       </c>
       <c r="E74" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F74" t="n">
         <v>21</v>
@@ -2947,13 +2947,13 @@
         <v>98.16112084063047</v>
       </c>
       <c r="H74" t="n">
-        <v>96.88850475367329</v>
+        <v>97.14038128249567</v>
       </c>
       <c r="I74" t="n">
-        <v>0.04986876640419947</v>
+        <v>0.04724409448818898</v>
       </c>
       <c r="J74" t="n">
-        <v>209.1126613616943</v>
+        <v>272.3200597763062</v>
       </c>
     </row>
     <row r="75">
@@ -2963,31 +2963,31 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1279</v>
+        <v>1336</v>
       </c>
       <c r="C75" t="n">
         <v>1356</v>
       </c>
       <c r="D75" t="n">
-        <v>1273</v>
+        <v>1311</v>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F75" t="n">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="G75" t="n">
-        <v>93.94833948339483</v>
+        <v>96.75276752767527</v>
       </c>
       <c r="H75" t="n">
-        <v>99.60876369327073</v>
+        <v>98.20224719101124</v>
       </c>
       <c r="I75" t="n">
-        <v>0.06415929203539823</v>
+        <v>0.05014749262536873</v>
       </c>
       <c r="J75" t="n">
-        <v>447.4528653621674</v>
+        <v>551.5230448246002</v>
       </c>
     </row>
     <row r="76">
@@ -2997,31 +2997,31 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C76" t="n">
         <v>543</v>
       </c>
       <c r="D76" t="n">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G76" t="n">
-        <v>98.33948339483395</v>
+        <v>98.8929889298893</v>
       </c>
       <c r="H76" t="n">
         <v>100</v>
       </c>
       <c r="I76" t="n">
-        <v>0.01657458563535912</v>
+        <v>0.01104972375690608</v>
       </c>
       <c r="J76" t="n">
-        <v>391.500287771225</v>
+        <v>441.5104689598083</v>
       </c>
     </row>
     <row r="77">
@@ -3031,31 +3031,31 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>1923</v>
+        <v>1938</v>
       </c>
       <c r="C77" t="n">
         <v>2025</v>
       </c>
       <c r="D77" t="n">
-        <v>1922</v>
+        <v>1937</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="G77" t="n">
-        <v>94.96047430830039</v>
+        <v>95.70158102766798</v>
       </c>
       <c r="H77" t="n">
         <v>100</v>
       </c>
       <c r="I77" t="n">
-        <v>0.05037037037037037</v>
+        <v>0.04296296296296296</v>
       </c>
       <c r="J77" t="n">
-        <v>241.3798811435699</v>
+        <v>260.8916940689087</v>
       </c>
     </row>
     <row r="78">
@@ -3065,31 +3065,31 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="C78" t="n">
         <v>2145</v>
       </c>
       <c r="D78" t="n">
-        <v>2143</v>
+        <v>2141</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G78" t="n">
-        <v>99.95335820895522</v>
+        <v>99.86007462686567</v>
       </c>
       <c r="H78" t="n">
-        <v>100</v>
+        <v>99.95331465919701</v>
       </c>
       <c r="I78" t="n">
-        <v>0.0004662004662004662</v>
+        <v>0.001864801864801865</v>
       </c>
       <c r="J78" t="n">
-        <v>502.8298606872559</v>
+        <v>530.2923488616943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove baseline using two cascaded median filters
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/AHA_database.xlsx
+++ b/R peak detection/beatdetection/AHA_database.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sgasu" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="gygcgc" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1624</v>
+        <v>1630</v>
       </c>
       <c r="C1" t="n">
         <v>1622</v>
@@ -456,7 +456,7 @@
         <v>1620</v>
       </c>
       <c r="E1" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F1" t="n">
         <v>1</v>
@@ -465,13 +465,13 @@
         <v>99.93830968537939</v>
       </c>
       <c r="H1" t="n">
-        <v>99.81515711645102</v>
+        <v>99.4475138121547</v>
       </c>
       <c r="I1" t="n">
-        <v>0.002466091245376079</v>
+        <v>0.006165228113440197</v>
       </c>
       <c r="J1" t="n">
-        <v>92.78410625457764</v>
+        <v>62.67790913581848</v>
       </c>
     </row>
     <row r="2">
@@ -505,7 +505,7 @@
         <v>0.0003853564547206166</v>
       </c>
       <c r="J2" t="n">
-        <v>85.88464260101318</v>
+        <v>66.2179114818573</v>
       </c>
     </row>
     <row r="3">
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>87.46213173866272</v>
+        <v>60.37194752693176</v>
       </c>
     </row>
     <row r="4">
@@ -549,31 +549,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2956</v>
+        <v>2957</v>
       </c>
       <c r="C4" t="n">
         <v>2974</v>
       </c>
       <c r="D4" t="n">
-        <v>2950</v>
+        <v>2953</v>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" t="n">
-        <v>99.22637066935755</v>
+        <v>99.32727884291961</v>
       </c>
       <c r="H4" t="n">
-        <v>99.83079526226734</v>
+        <v>99.89851150202978</v>
       </c>
       <c r="I4" t="n">
-        <v>0.00941492938802959</v>
+        <v>0.00773369199731002</v>
       </c>
       <c r="J4" t="n">
-        <v>120.8448188304901</v>
+        <v>64.86515617370605</v>
       </c>
     </row>
     <row r="5">
@@ -583,31 +583,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2554</v>
+        <v>2473</v>
       </c>
       <c r="C5" t="n">
         <v>2554</v>
       </c>
       <c r="D5" t="n">
-        <v>2553</v>
+        <v>2472</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="G5" t="n">
-        <v>100</v>
+        <v>96.82726204465335</v>
       </c>
       <c r="H5" t="n">
         <v>100</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>0.0317149569303054</v>
       </c>
       <c r="J5" t="n">
-        <v>90.32473945617676</v>
+        <v>56.96660089492798</v>
       </c>
     </row>
     <row r="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="C6" t="n">
         <v>2122</v>
@@ -626,7 +626,7 @@
         <v>2121</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -635,13 +635,13 @@
         <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>99.95287464655985</v>
+        <v>100</v>
       </c>
       <c r="I6" t="n">
-        <v>0.000471253534401508</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>102.7025241851807</v>
+        <v>59.69064903259277</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>78.43877506256104</v>
+        <v>53.69886684417725</v>
       </c>
     </row>
     <row r="8">
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>104.8826658725739</v>
+        <v>62.91601657867432</v>
       </c>
     </row>
     <row r="9">
@@ -719,7 +719,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3582</v>
+        <v>3581</v>
       </c>
       <c r="C9" t="n">
         <v>3582</v>
@@ -728,7 +728,7 @@
         <v>3580</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -737,13 +737,13 @@
         <v>99.97207483943032</v>
       </c>
       <c r="H9" t="n">
-        <v>99.97207483943032</v>
+        <v>100</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0005583472920156337</v>
+        <v>0.0002791736460078169</v>
       </c>
       <c r="J9" t="n">
-        <v>147.9974005222321</v>
+        <v>80.72808980941772</v>
       </c>
     </row>
     <row r="10">
@@ -753,31 +753,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2026</v>
+        <v>2080</v>
       </c>
       <c r="C10" t="n">
         <v>1997</v>
       </c>
       <c r="D10" t="n">
-        <v>1991</v>
+        <v>1994</v>
       </c>
       <c r="E10" t="n">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="F10" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>99.74949899799599</v>
+        <v>99.8997995991984</v>
       </c>
       <c r="H10" t="n">
-        <v>98.32098765432099</v>
+        <v>95.9114959114959</v>
       </c>
       <c r="I10" t="n">
-        <v>0.01952929394091137</v>
+        <v>0.04356534802203305</v>
       </c>
       <c r="J10" t="n">
-        <v>173.7748024463654</v>
+        <v>82.19165658950806</v>
       </c>
     </row>
     <row r="11">
@@ -793,25 +793,25 @@
         <v>2875</v>
       </c>
       <c r="D11" t="n">
-        <v>2874</v>
+        <v>2867</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G11" t="n">
-        <v>100</v>
+        <v>99.75643702157272</v>
       </c>
       <c r="H11" t="n">
-        <v>100</v>
+        <v>99.75643702157272</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>0.004869565217391304</v>
       </c>
       <c r="J11" t="n">
-        <v>92.80263185501099</v>
+        <v>48.26282835006714</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="C12" t="n">
         <v>2414</v>
@@ -830,7 +830,7 @@
         <v>2413</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -839,13 +839,13 @@
         <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>99.95857497928749</v>
+        <v>100</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0004142502071251035</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>132.6538851261139</v>
+        <v>58.46115565299988</v>
       </c>
     </row>
     <row r="13">
@@ -855,31 +855,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3423</v>
+        <v>3444</v>
       </c>
       <c r="C13" t="n">
         <v>3511</v>
       </c>
       <c r="D13" t="n">
-        <v>3402</v>
+        <v>3412</v>
       </c>
       <c r="E13" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F13" t="n">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G13" t="n">
-        <v>96.92307692307692</v>
+        <v>97.20797720797721</v>
       </c>
       <c r="H13" t="n">
-        <v>99.41554646405611</v>
+        <v>99.09962242230613</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0364568499003133</v>
+        <v>0.0367416690401595</v>
       </c>
       <c r="J13" t="n">
-        <v>218.8199925422668</v>
+        <v>92.56618070602417</v>
       </c>
     </row>
     <row r="14">
@@ -913,7 +913,7 @@
         <v>0.002457002457002457</v>
       </c>
       <c r="J14" t="n">
-        <v>105.687805891037</v>
+        <v>47.75854253768921</v>
       </c>
     </row>
     <row r="15">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="C15" t="n">
         <v>1613</v>
@@ -932,7 +932,7 @@
         <v>1612</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -941,13 +941,13 @@
         <v>100</v>
       </c>
       <c r="H15" t="n">
-        <v>99.93800371977682</v>
+        <v>99.87608426270137</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0006199628022318661</v>
+        <v>0.001239925604463732</v>
       </c>
       <c r="J15" t="n">
-        <v>124.9002187252045</v>
+        <v>55.35753440856934</v>
       </c>
     </row>
     <row r="16">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>136.8912932872772</v>
+        <v>57.25705170631409</v>
       </c>
     </row>
     <row r="17">
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="C17" t="n">
         <v>2854</v>
@@ -1000,7 +1000,7 @@
         <v>2853</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -1009,13 +1009,13 @@
         <v>100</v>
       </c>
       <c r="H17" t="n">
-        <v>99.96496145760337</v>
+        <v>100</v>
       </c>
       <c r="I17" t="n">
-        <v>0.000350385423966363</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>135.2376980781555</v>
+        <v>56.73311519622803</v>
       </c>
     </row>
     <row r="18">
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>146.0154478549957</v>
+        <v>51.73887252807617</v>
       </c>
     </row>
     <row r="19">
@@ -1059,7 +1059,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2592</v>
+        <v>2579</v>
       </c>
       <c r="C19" t="n">
         <v>2537</v>
@@ -1068,7 +1068,7 @@
         <v>2534</v>
       </c>
       <c r="E19" t="n">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F19" t="n">
         <v>2</v>
@@ -1077,13 +1077,13 @@
         <v>99.9211356466877</v>
       </c>
       <c r="H19" t="n">
-        <v>97.80007719027402</v>
+        <v>98.29325058184639</v>
       </c>
       <c r="I19" t="n">
-        <v>0.02325581395348837</v>
+        <v>0.01813165155695703</v>
       </c>
       <c r="J19" t="n">
-        <v>221.7416796684265</v>
+        <v>59.73395538330078</v>
       </c>
     </row>
     <row r="20">
@@ -1117,7 +1117,7 @@
         <v>0.001837390904915021</v>
       </c>
       <c r="J20" t="n">
-        <v>216.0197570323944</v>
+        <v>62.7965726852417</v>
       </c>
     </row>
     <row r="21">
@@ -1127,31 +1127,31 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2943</v>
+        <v>2944</v>
       </c>
       <c r="C21" t="n">
         <v>2943</v>
       </c>
       <c r="D21" t="n">
-        <v>2940</v>
+        <v>2938</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G21" t="n">
-        <v>99.93201903467029</v>
+        <v>99.86403806934058</v>
       </c>
       <c r="H21" t="n">
-        <v>99.93201903467029</v>
+        <v>99.83010533469249</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001359157322460075</v>
+        <v>0.003058103975535168</v>
       </c>
       <c r="J21" t="n">
-        <v>240.9267868995667</v>
+        <v>60.8289201259613</v>
       </c>
     </row>
     <row r="22">
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1956</v>
+        <v>1959</v>
       </c>
       <c r="C22" t="n">
         <v>1950</v>
@@ -1170,7 +1170,7 @@
         <v>1949</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1179,13 +1179,13 @@
         <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>99.69309462915601</v>
+        <v>99.54034729315629</v>
       </c>
       <c r="I22" t="n">
-        <v>0.003076923076923077</v>
+        <v>0.004615384615384616</v>
       </c>
       <c r="J22" t="n">
-        <v>145.673201084137</v>
+        <v>50.91852688789368</v>
       </c>
     </row>
     <row r="23">
@@ -1195,7 +1195,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1889</v>
+        <v>1878</v>
       </c>
       <c r="C23" t="n">
         <v>1878</v>
@@ -1204,7 +1204,7 @@
         <v>1871</v>
       </c>
       <c r="E23" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
         <v>6</v>
@@ -1213,13 +1213,13 @@
         <v>99.6803409696324</v>
       </c>
       <c r="H23" t="n">
-        <v>99.09957627118644</v>
+        <v>99.6803409696324</v>
       </c>
       <c r="I23" t="n">
-        <v>0.01224707135250266</v>
+        <v>0.006389776357827476</v>
       </c>
       <c r="J23" t="n">
-        <v>241.0386998653412</v>
+        <v>69.2003128528595</v>
       </c>
     </row>
     <row r="24">
@@ -1253,7 +1253,7 @@
         <v>0.001121076233183856</v>
       </c>
       <c r="J24" t="n">
-        <v>159.7406003475189</v>
+        <v>56.52787446975708</v>
       </c>
     </row>
     <row r="25">
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>137.2374458312988</v>
+        <v>46.54709959030151</v>
       </c>
     </row>
     <row r="26">
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2330</v>
+        <v>2328</v>
       </c>
       <c r="C26" t="n">
         <v>2324</v>
@@ -1306,7 +1306,7 @@
         <v>2323</v>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1315,13 +1315,13 @@
         <v>100</v>
       </c>
       <c r="H26" t="n">
-        <v>99.74237870330614</v>
+        <v>99.82810485603781</v>
       </c>
       <c r="I26" t="n">
-        <v>0.002581755593803787</v>
+        <v>0.001721170395869191</v>
       </c>
       <c r="J26" t="n">
-        <v>212.4686231613159</v>
+        <v>62.1968777179718</v>
       </c>
     </row>
     <row r="27">
@@ -1355,7 +1355,7 @@
         <v>0.0004125412541254125</v>
       </c>
       <c r="J27" t="n">
-        <v>227.0689141750336</v>
+        <v>55.56084966659546</v>
       </c>
     </row>
     <row r="28">
@@ -1389,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>257.8162310123444</v>
+        <v>56.7192907333374</v>
       </c>
     </row>
     <row r="29">
@@ -1399,31 +1399,31 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2459</v>
+        <v>2454</v>
       </c>
       <c r="C29" t="n">
         <v>2472</v>
       </c>
       <c r="D29" t="n">
-        <v>2450</v>
+        <v>2447</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F29" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G29" t="n">
-        <v>99.15014164305948</v>
+        <v>99.0287333063537</v>
       </c>
       <c r="H29" t="n">
-        <v>99.67453213995118</v>
+        <v>99.75540154912352</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01173139158576052</v>
+        <v>0.01213592233009709</v>
       </c>
       <c r="J29" t="n">
-        <v>173.8208084106445</v>
+        <v>47.90150046348572</v>
       </c>
     </row>
     <row r="30">
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>183.9332089424133</v>
+        <v>49.90666246414185</v>
       </c>
     </row>
     <row r="31">
@@ -1467,31 +1467,31 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2371</v>
+        <v>2369</v>
       </c>
       <c r="C31" t="n">
         <v>2376</v>
       </c>
       <c r="D31" t="n">
-        <v>2366</v>
+        <v>2367</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" t="n">
-        <v>99.62105263157895</v>
+        <v>99.66315789473684</v>
       </c>
       <c r="H31" t="n">
-        <v>99.83122362869199</v>
+        <v>99.95777027027027</v>
       </c>
       <c r="I31" t="n">
-        <v>0.005471380471380472</v>
+        <v>0.003787878787878788</v>
       </c>
       <c r="J31" t="n">
-        <v>162.4402174949646</v>
+        <v>47.74468374252319</v>
       </c>
     </row>
     <row r="32">
@@ -1525,7 +1525,7 @@
         <v>0.0003872966692486445</v>
       </c>
       <c r="J32" t="n">
-        <v>249.9720501899719</v>
+        <v>59.15033054351807</v>
       </c>
     </row>
     <row r="33">
@@ -1541,25 +1541,25 @@
         <v>2258</v>
       </c>
       <c r="D33" t="n">
-        <v>2253</v>
+        <v>2254</v>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G33" t="n">
-        <v>99.8227735932654</v>
+        <v>99.86708019494905</v>
       </c>
       <c r="H33" t="n">
-        <v>99.8227735932654</v>
+        <v>99.86708019494905</v>
       </c>
       <c r="I33" t="n">
-        <v>0.00354295837023915</v>
+        <v>0.002657218777679362</v>
       </c>
       <c r="J33" t="n">
-        <v>153.5061819553375</v>
+        <v>45.13383817672729</v>
       </c>
     </row>
     <row r="34">
@@ -1569,31 +1569,31 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1456</v>
+        <v>1444</v>
       </c>
       <c r="C34" t="n">
         <v>1452</v>
       </c>
       <c r="D34" t="n">
-        <v>1451</v>
+        <v>1443</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G34" t="n">
-        <v>100</v>
+        <v>99.4486560992419</v>
       </c>
       <c r="H34" t="n">
-        <v>99.72508591065292</v>
+        <v>100</v>
       </c>
       <c r="I34" t="n">
-        <v>0.002754820936639119</v>
+        <v>0.005509641873278237</v>
       </c>
       <c r="J34" t="n">
-        <v>236.7128043174744</v>
+        <v>58.11594462394714</v>
       </c>
     </row>
     <row r="35">
@@ -1603,31 +1603,31 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1947</v>
+        <v>1940</v>
       </c>
       <c r="C35" t="n">
         <v>1947</v>
       </c>
       <c r="D35" t="n">
-        <v>1946</v>
+        <v>1938</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G35" t="n">
-        <v>100</v>
+        <v>99.58890030832477</v>
       </c>
       <c r="H35" t="n">
-        <v>100</v>
+        <v>99.94842702423929</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>0.004622496147919877</v>
       </c>
       <c r="J35" t="n">
-        <v>157.3932671546936</v>
+        <v>45.50319528579712</v>
       </c>
     </row>
     <row r="36">
@@ -1637,31 +1637,31 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3524</v>
+        <v>3527</v>
       </c>
       <c r="C36" t="n">
         <v>3520</v>
       </c>
       <c r="D36" t="n">
-        <v>3504</v>
+        <v>3515</v>
       </c>
       <c r="E36" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F36" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G36" t="n">
-        <v>99.57374254049446</v>
+        <v>99.88633134413186</v>
       </c>
       <c r="H36" t="n">
-        <v>99.46068691456145</v>
+        <v>99.68803176403857</v>
       </c>
       <c r="I36" t="n">
-        <v>0.009659090909090909</v>
+        <v>0.004261363636363636</v>
       </c>
       <c r="J36" t="n">
-        <v>284.1411597728729</v>
+        <v>85.39648604393005</v>
       </c>
     </row>
     <row r="37">
@@ -1671,31 +1671,31 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1882</v>
+        <v>1887</v>
       </c>
       <c r="C37" t="n">
         <v>1878</v>
       </c>
       <c r="D37" t="n">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>99.94672349493874</v>
+        <v>100</v>
       </c>
       <c r="H37" t="n">
-        <v>99.73418394471027</v>
+        <v>99.52279957582185</v>
       </c>
       <c r="I37" t="n">
-        <v>0.003194888178913738</v>
+        <v>0.004792332268370607</v>
       </c>
       <c r="J37" t="n">
-        <v>228.9701895713806</v>
+        <v>53.20688462257385</v>
       </c>
     </row>
     <row r="38">
@@ -1705,31 +1705,31 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2369</v>
+        <v>2367</v>
       </c>
       <c r="C38" t="n">
         <v>2371</v>
       </c>
       <c r="D38" t="n">
-        <v>2366</v>
+        <v>2362</v>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F38" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G38" t="n">
-        <v>99.83122362869199</v>
+        <v>99.66244725738396</v>
       </c>
       <c r="H38" t="n">
-        <v>99.91554054054055</v>
+        <v>99.83093829247676</v>
       </c>
       <c r="I38" t="n">
-        <v>0.002530577815267819</v>
+        <v>0.005061155630535639</v>
       </c>
       <c r="J38" t="n">
-        <v>284.8226659297943</v>
+        <v>63.9724907875061</v>
       </c>
     </row>
     <row r="39">
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>136.9302062988281</v>
+        <v>47.29521489143372</v>
       </c>
     </row>
     <row r="40">
@@ -1773,31 +1773,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2243</v>
+        <v>2247</v>
       </c>
       <c r="C40" t="n">
         <v>2257</v>
       </c>
       <c r="D40" t="n">
-        <v>2241</v>
+        <v>2245</v>
       </c>
       <c r="E40" t="n">
         <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G40" t="n">
-        <v>99.33510638297872</v>
+        <v>99.51241134751773</v>
       </c>
       <c r="H40" t="n">
-        <v>99.95539696699376</v>
+        <v>99.95547640249332</v>
       </c>
       <c r="I40" t="n">
-        <v>0.007089056269384138</v>
+        <v>0.005316792202038104</v>
       </c>
       <c r="J40" t="n">
-        <v>123.6139595508575</v>
+        <v>45.28063583374023</v>
       </c>
     </row>
     <row r="41">
@@ -1807,31 +1807,31 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2351</v>
+        <v>2341</v>
       </c>
       <c r="C41" t="n">
         <v>2351</v>
       </c>
       <c r="D41" t="n">
-        <v>2319</v>
+        <v>2340</v>
       </c>
       <c r="E41" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G41" t="n">
-        <v>98.68085106382979</v>
+        <v>99.57446808510639</v>
       </c>
       <c r="H41" t="n">
-        <v>98.68085106382979</v>
+        <v>100</v>
       </c>
       <c r="I41" t="n">
-        <v>0.0263717566992769</v>
+        <v>0.004253509145044662</v>
       </c>
       <c r="J41" t="n">
-        <v>277.9519579410553</v>
+        <v>61.5987548828125</v>
       </c>
     </row>
     <row r="42">
@@ -1865,7 +1865,7 @@
         <v>0.0004212299915754001</v>
       </c>
       <c r="J42" t="n">
-        <v>218.5389811992645</v>
+        <v>49.960857629776</v>
       </c>
     </row>
     <row r="43">
@@ -1899,7 +1899,7 @@
         <v>0.0004372540445999126</v>
       </c>
       <c r="J43" t="n">
-        <v>271.5392079353333</v>
+        <v>58.5847852230072</v>
       </c>
     </row>
     <row r="44">
@@ -1915,25 +1915,25 @@
         <v>1806</v>
       </c>
       <c r="D44" t="n">
-        <v>1790</v>
+        <v>1805</v>
       </c>
       <c r="E44" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>99.16897506925208</v>
+        <v>100</v>
       </c>
       <c r="H44" t="n">
-        <v>99.16897506925208</v>
+        <v>100</v>
       </c>
       <c r="I44" t="n">
-        <v>0.01661129568106312</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>232.0619854927063</v>
+        <v>52.38355231285095</v>
       </c>
     </row>
     <row r="45">
@@ -1943,7 +1943,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2070</v>
+        <v>2078</v>
       </c>
       <c r="C45" t="n">
         <v>2068</v>
@@ -1952,7 +1952,7 @@
         <v>2067</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1961,13 +1961,13 @@
         <v>100</v>
       </c>
       <c r="H45" t="n">
-        <v>99.90333494441759</v>
+        <v>99.51853635050554</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0009671179883945841</v>
+        <v>0.004835589941972921</v>
       </c>
       <c r="J45" t="n">
-        <v>286.9822735786438</v>
+        <v>61.90393447875977</v>
       </c>
     </row>
     <row r="46">
@@ -1977,7 +1977,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="C46" t="n">
         <v>2923</v>
@@ -1986,7 +1986,7 @@
         <v>2911</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
         <v>11</v>
@@ -1995,13 +1995,13 @@
         <v>99.62354551676934</v>
       </c>
       <c r="H46" t="n">
-        <v>99.96565934065934</v>
+        <v>100</v>
       </c>
       <c r="I46" t="n">
-        <v>0.004105371193978789</v>
+        <v>0.00376325692781389</v>
       </c>
       <c r="J46" t="n">
-        <v>304.0650587081909</v>
+        <v>63.3736572265625</v>
       </c>
     </row>
     <row r="47">
@@ -2011,31 +2011,31 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1863</v>
+        <v>1848</v>
       </c>
       <c r="C47" t="n">
         <v>1845</v>
       </c>
       <c r="D47" t="n">
-        <v>1834</v>
+        <v>1817</v>
       </c>
       <c r="E47" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F47" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G47" t="n">
-        <v>99.45770065075922</v>
+        <v>98.53579175704989</v>
       </c>
       <c r="H47" t="n">
-        <v>98.49624060150376</v>
+        <v>98.3757444504602</v>
       </c>
       <c r="I47" t="n">
-        <v>0.02059620596205962</v>
+        <v>0.03089430894308943</v>
       </c>
       <c r="J47" t="n">
-        <v>295.8240525722504</v>
+        <v>54.64325356483459</v>
       </c>
     </row>
     <row r="48">
@@ -2051,25 +2051,25 @@
         <v>2164</v>
       </c>
       <c r="D48" t="n">
-        <v>2162</v>
+        <v>2163</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>99.95376791493297</v>
+        <v>100</v>
       </c>
       <c r="H48" t="n">
-        <v>99.95376791493297</v>
+        <v>100</v>
       </c>
       <c r="I48" t="n">
-        <v>0.0009242144177449168</v>
+        <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>255.9696805477142</v>
+        <v>57.44101595878601</v>
       </c>
     </row>
     <row r="49">
@@ -2079,31 +2079,31 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C49" t="n">
         <v>2017</v>
       </c>
       <c r="D49" t="n">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" t="n">
-        <v>100</v>
+        <v>99.95039682539682</v>
       </c>
       <c r="H49" t="n">
         <v>100</v>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>0.0004957858205255329</v>
       </c>
       <c r="J49" t="n">
-        <v>326.4495222568512</v>
+        <v>62.5575053691864</v>
       </c>
     </row>
     <row r="50">
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>465.9692249298096</v>
+        <v>57.86803817749023</v>
       </c>
     </row>
     <row r="51">
@@ -2171,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>358.5515220165253</v>
+        <v>56.69511032104492</v>
       </c>
     </row>
     <row r="52">
@@ -2181,31 +2181,31 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2696</v>
+        <v>2687</v>
       </c>
       <c r="C52" t="n">
         <v>2698</v>
       </c>
       <c r="D52" t="n">
-        <v>2684</v>
+        <v>2685</v>
       </c>
       <c r="E52" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G52" t="n">
-        <v>99.51798294401186</v>
+        <v>99.55506117908787</v>
       </c>
       <c r="H52" t="n">
-        <v>99.59183673469387</v>
+        <v>99.96276991809383</v>
       </c>
       <c r="I52" t="n">
-        <v>0.008895478131949592</v>
+        <v>0.004818383988139363</v>
       </c>
       <c r="J52" t="n">
-        <v>367.5740327835083</v>
+        <v>52.16977000236511</v>
       </c>
     </row>
     <row r="53">
@@ -2215,7 +2215,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2254</v>
+        <v>2251</v>
       </c>
       <c r="C53" t="n">
         <v>2251</v>
@@ -2224,7 +2224,7 @@
         <v>2250</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -2233,13 +2233,13 @@
         <v>100</v>
       </c>
       <c r="H53" t="n">
-        <v>99.86684420772303</v>
+        <v>100</v>
       </c>
       <c r="I53" t="n">
-        <v>0.001332741003998223</v>
+        <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>363.5812191963196</v>
+        <v>58.77567720413208</v>
       </c>
     </row>
     <row r="54">
@@ -2249,31 +2249,31 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2299</v>
+        <v>2295</v>
       </c>
       <c r="C54" t="n">
         <v>2294</v>
       </c>
       <c r="D54" t="n">
-        <v>2267</v>
+        <v>2291</v>
       </c>
       <c r="E54" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="F54" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="G54" t="n">
-        <v>98.86611426079372</v>
+        <v>99.91277802006105</v>
       </c>
       <c r="H54" t="n">
-        <v>98.65100087032202</v>
+        <v>99.86922406277245</v>
       </c>
       <c r="I54" t="n">
-        <v>0.02484742807323452</v>
+        <v>0.002179598953792502</v>
       </c>
       <c r="J54" t="n">
-        <v>474.1692237854004</v>
+        <v>62.4241087436676</v>
       </c>
     </row>
     <row r="55">
@@ -2289,25 +2289,25 @@
         <v>2785</v>
       </c>
       <c r="D55" t="n">
-        <v>2777</v>
+        <v>2778</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G55" t="n">
-        <v>99.7485632183908</v>
+        <v>99.78448275862068</v>
       </c>
       <c r="H55" t="n">
-        <v>99.96400287976962</v>
+        <v>100</v>
       </c>
       <c r="I55" t="n">
-        <v>0.002872531418312388</v>
+        <v>0.002154398563734291</v>
       </c>
       <c r="J55" t="n">
-        <v>182.9815897941589</v>
+        <v>45.6457211971283</v>
       </c>
     </row>
     <row r="56">
@@ -2317,31 +2317,31 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>2044</v>
+        <v>2042</v>
       </c>
       <c r="C56" t="n">
         <v>2044</v>
       </c>
       <c r="D56" t="n">
-        <v>2043</v>
+        <v>2039</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G56" t="n">
-        <v>100</v>
+        <v>99.80420949583946</v>
       </c>
       <c r="H56" t="n">
-        <v>100</v>
+        <v>99.90200881920627</v>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>0.002935420743639922</v>
       </c>
       <c r="J56" t="n">
-        <v>349.4402720928192</v>
+        <v>52.88484120368958</v>
       </c>
     </row>
     <row r="57">
@@ -2357,25 +2357,25 @@
         <v>2359</v>
       </c>
       <c r="D57" t="n">
-        <v>2357</v>
+        <v>2358</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>99.95759117896523</v>
+        <v>100</v>
       </c>
       <c r="H57" t="n">
-        <v>99.95759117896523</v>
+        <v>100</v>
       </c>
       <c r="I57" t="n">
-        <v>0.000847816871555744</v>
+        <v>0</v>
       </c>
       <c r="J57" t="n">
-        <v>227.7234578132629</v>
+        <v>45.55906987190247</v>
       </c>
     </row>
     <row r="58">
@@ -2385,31 +2385,31 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>2502</v>
+        <v>2495</v>
       </c>
       <c r="C58" t="n">
         <v>2500</v>
       </c>
       <c r="D58" t="n">
-        <v>2499</v>
+        <v>2493</v>
       </c>
       <c r="E58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G58" t="n">
-        <v>100</v>
+        <v>99.75990396158464</v>
       </c>
       <c r="H58" t="n">
-        <v>99.92003198720512</v>
+        <v>99.95990376904571</v>
       </c>
       <c r="I58" t="n">
-        <v>0.0008</v>
+        <v>0.0028</v>
       </c>
       <c r="J58" t="n">
-        <v>442.980672121048</v>
+        <v>56.66622734069824</v>
       </c>
     </row>
     <row r="59">
@@ -2419,31 +2419,31 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>3294</v>
+        <v>3290</v>
       </c>
       <c r="C59" t="n">
         <v>3289</v>
       </c>
       <c r="D59" t="n">
-        <v>3283</v>
+        <v>3286</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F59" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G59" t="n">
-        <v>99.84793187347933</v>
+        <v>99.93917274939173</v>
       </c>
       <c r="H59" t="n">
-        <v>99.69632553902217</v>
+        <v>99.9087868653086</v>
       </c>
       <c r="I59" t="n">
-        <v>0.004560656734569778</v>
+        <v>0.001520218911523259</v>
       </c>
       <c r="J59" t="n">
-        <v>333.7351341247559</v>
+        <v>84.75144481658936</v>
       </c>
     </row>
     <row r="60">
@@ -2453,31 +2453,31 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>3163</v>
+        <v>3157</v>
       </c>
       <c r="C60" t="n">
         <v>3164</v>
       </c>
       <c r="D60" t="n">
-        <v>3158</v>
+        <v>3156</v>
       </c>
       <c r="E60" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G60" t="n">
-        <v>99.84192222573506</v>
+        <v>99.77869111602908</v>
       </c>
       <c r="H60" t="n">
-        <v>99.87349778621126</v>
+        <v>100</v>
       </c>
       <c r="I60" t="n">
-        <v>0.002844500632111252</v>
+        <v>0.002212389380530973</v>
       </c>
       <c r="J60" t="n">
-        <v>327.6184418201447</v>
+        <v>61.18451523780823</v>
       </c>
     </row>
     <row r="61">
@@ -2511,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>479.7675290107727</v>
+        <v>68.66913318634033</v>
       </c>
     </row>
     <row r="62">
@@ -2545,7 +2545,7 @@
         <v>0.001184366363995263</v>
       </c>
       <c r="J62" t="n">
-        <v>246.7846231460571</v>
+        <v>54.58682751655579</v>
       </c>
     </row>
     <row r="63">
@@ -2555,31 +2555,31 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1920</v>
+        <v>1923</v>
       </c>
       <c r="C63" t="n">
         <v>1927</v>
       </c>
       <c r="D63" t="n">
-        <v>1919</v>
+        <v>1922</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G63" t="n">
-        <v>99.63655244029076</v>
+        <v>99.79231568016614</v>
       </c>
       <c r="H63" t="n">
         <v>100</v>
       </c>
       <c r="I63" t="n">
-        <v>0.003632589517384536</v>
+        <v>0.002075765438505449</v>
       </c>
       <c r="J63" t="n">
-        <v>216.4848577976227</v>
+        <v>46.70656681060791</v>
       </c>
     </row>
     <row r="64">
@@ -2589,31 +2589,31 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>2437</v>
+        <v>2445</v>
       </c>
       <c r="C64" t="n">
         <v>2437</v>
       </c>
       <c r="D64" t="n">
-        <v>2434</v>
+        <v>2426</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F64" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G64" t="n">
-        <v>99.91789819376027</v>
+        <v>99.58949096880131</v>
       </c>
       <c r="H64" t="n">
-        <v>99.91789819376027</v>
+        <v>99.26350245499182</v>
       </c>
       <c r="I64" t="n">
-        <v>0.00164136233073451</v>
+        <v>0.01148953631514157</v>
       </c>
       <c r="J64" t="n">
-        <v>380.8764493465424</v>
+        <v>55.50897455215454</v>
       </c>
     </row>
     <row r="65">
@@ -2623,31 +2623,31 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>3107</v>
+        <v>3109</v>
       </c>
       <c r="C65" t="n">
         <v>3109</v>
       </c>
       <c r="D65" t="n">
-        <v>3099</v>
+        <v>3107</v>
       </c>
       <c r="E65" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F65" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G65" t="n">
-        <v>99.7104247104247</v>
+        <v>99.96782496782497</v>
       </c>
       <c r="H65" t="n">
-        <v>99.77462974887315</v>
+        <v>99.96782496782497</v>
       </c>
       <c r="I65" t="n">
-        <v>0.005146349308459312</v>
+        <v>0.000643293663557414</v>
       </c>
       <c r="J65" t="n">
-        <v>460.5091700553894</v>
+        <v>99.00425601005554</v>
       </c>
     </row>
     <row r="66">
@@ -2657,31 +2657,31 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2338</v>
+        <v>2342</v>
       </c>
       <c r="C66" t="n">
         <v>2340</v>
       </c>
       <c r="D66" t="n">
-        <v>2336</v>
+        <v>2328</v>
       </c>
       <c r="E66" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F66" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G66" t="n">
-        <v>99.87174005985464</v>
+        <v>99.52971355280035</v>
       </c>
       <c r="H66" t="n">
-        <v>99.95721009841678</v>
+        <v>99.44468175993165</v>
       </c>
       <c r="I66" t="n">
-        <v>0.001709401709401709</v>
+        <v>0.01025641025641026</v>
       </c>
       <c r="J66" t="n">
-        <v>308.5487623214722</v>
+        <v>61.87328124046326</v>
       </c>
     </row>
     <row r="67">
@@ -2715,7 +2715,7 @@
         <v>0.0006389776357827476</v>
       </c>
       <c r="J67" t="n">
-        <v>282.1427466869354</v>
+        <v>52.98287630081177</v>
       </c>
     </row>
     <row r="68">
@@ -2725,31 +2725,31 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2908</v>
+        <v>2180</v>
       </c>
       <c r="C68" t="n">
         <v>2897</v>
       </c>
       <c r="D68" t="n">
-        <v>2874</v>
+        <v>2167</v>
       </c>
       <c r="E68" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="F68" t="n">
-        <v>22</v>
+        <v>729</v>
       </c>
       <c r="G68" t="n">
-        <v>99.24033149171271</v>
+        <v>74.82734806629834</v>
       </c>
       <c r="H68" t="n">
-        <v>98.86480908152735</v>
+        <v>99.44928866452501</v>
       </c>
       <c r="I68" t="n">
-        <v>0.01898515705902658</v>
+        <v>0.2557818432861581</v>
       </c>
       <c r="J68" t="n">
-        <v>470.2379167079926</v>
+        <v>62.44965243339539</v>
       </c>
     </row>
     <row r="69">
@@ -2759,31 +2759,31 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1748</v>
+        <v>1751</v>
       </c>
       <c r="C69" t="n">
         <v>1753</v>
       </c>
       <c r="D69" t="n">
-        <v>1746</v>
+        <v>1749</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
       </c>
       <c r="F69" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G69" t="n">
-        <v>99.65753424657534</v>
+        <v>99.82876712328768</v>
       </c>
       <c r="H69" t="n">
-        <v>99.94275901545507</v>
+        <v>99.94285714285714</v>
       </c>
       <c r="I69" t="n">
-        <v>0.003993154592127781</v>
+        <v>0.002281802624073018</v>
       </c>
       <c r="J69" t="n">
-        <v>375.9237840175629</v>
+        <v>55.60299038887024</v>
       </c>
     </row>
     <row r="70">
@@ -2793,31 +2793,31 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="C70" t="n">
         <v>1459</v>
       </c>
       <c r="D70" t="n">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G70" t="n">
-        <v>99.65706447187928</v>
+        <v>99.38271604938272</v>
       </c>
       <c r="H70" t="n">
-        <v>99.93122420907841</v>
+        <v>100</v>
       </c>
       <c r="I70" t="n">
-        <v>0.00411240575736806</v>
+        <v>0.00616860863605209</v>
       </c>
       <c r="J70" t="n">
-        <v>475.0378057956696</v>
+        <v>71.0113320350647</v>
       </c>
     </row>
     <row r="71">
@@ -2827,31 +2827,31 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1762</v>
+        <v>1758</v>
       </c>
       <c r="C71" t="n">
         <v>1787</v>
       </c>
       <c r="D71" t="n">
-        <v>1755</v>
+        <v>1749</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F71" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G71" t="n">
-        <v>98.20928931169558</v>
+        <v>97.8735310576385</v>
       </c>
       <c r="H71" t="n">
-        <v>99.65928449744463</v>
+        <v>99.54467842914057</v>
       </c>
       <c r="I71" t="n">
-        <v>0.021264689423615</v>
+        <v>0.02574146614437605</v>
       </c>
       <c r="J71" t="n">
-        <v>203.6996734142303</v>
+        <v>53.20101070404053</v>
       </c>
     </row>
     <row r="72">
@@ -2861,31 +2861,31 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>1546</v>
+        <v>1560</v>
       </c>
       <c r="C72" t="n">
         <v>1567</v>
       </c>
       <c r="D72" t="n">
-        <v>1542</v>
+        <v>1558</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F72" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G72" t="n">
-        <v>98.46743295019157</v>
+        <v>99.48914431673052</v>
       </c>
       <c r="H72" t="n">
-        <v>99.80582524271844</v>
+        <v>99.93585631815266</v>
       </c>
       <c r="I72" t="n">
-        <v>0.01723037651563497</v>
+        <v>0.00574345883854499</v>
       </c>
       <c r="J72" t="n">
-        <v>416.5431251525879</v>
+        <v>73.6719069480896</v>
       </c>
     </row>
     <row r="73">
@@ -2895,31 +2895,31 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C73" t="n">
         <v>920</v>
       </c>
       <c r="D73" t="n">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F73" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G73" t="n">
-        <v>98.80304678998912</v>
+        <v>98.5854189336235</v>
       </c>
       <c r="H73" t="n">
-        <v>99.67069154774973</v>
+        <v>99.56043956043956</v>
       </c>
       <c r="I73" t="n">
-        <v>0.01521739130434783</v>
+        <v>0.01847826086956522</v>
       </c>
       <c r="J73" t="n">
-        <v>306.2742254734039</v>
+        <v>61.24680233001709</v>
       </c>
     </row>
     <row r="74">
@@ -2929,31 +2929,31 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1155</v>
+        <v>1145</v>
       </c>
       <c r="C74" t="n">
         <v>1143</v>
       </c>
       <c r="D74" t="n">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="E74" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F74" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G74" t="n">
-        <v>98.16112084063047</v>
+        <v>97.63572679509632</v>
       </c>
       <c r="H74" t="n">
-        <v>97.14038128249567</v>
+        <v>97.46503496503496</v>
       </c>
       <c r="I74" t="n">
-        <v>0.04724409448818898</v>
+        <v>0.04899387576552931</v>
       </c>
       <c r="J74" t="n">
-        <v>272.3200597763062</v>
+        <v>63.34862208366394</v>
       </c>
     </row>
     <row r="75">
@@ -2963,31 +2963,31 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1336</v>
+        <v>1311</v>
       </c>
       <c r="C75" t="n">
         <v>1356</v>
       </c>
       <c r="D75" t="n">
-        <v>1311</v>
+        <v>1294</v>
       </c>
       <c r="E75" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F75" t="n">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="G75" t="n">
-        <v>96.75276752767527</v>
+        <v>95.49815498154982</v>
       </c>
       <c r="H75" t="n">
-        <v>98.20224719101124</v>
+        <v>98.77862595419847</v>
       </c>
       <c r="I75" t="n">
-        <v>0.05014749262536873</v>
+        <v>0.05678466076696165</v>
       </c>
       <c r="J75" t="n">
-        <v>551.5230448246002</v>
+        <v>85.42148947715759</v>
       </c>
     </row>
     <row r="76">
@@ -2997,31 +2997,31 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C76" t="n">
         <v>543</v>
       </c>
       <c r="D76" t="n">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G76" t="n">
-        <v>98.8929889298893</v>
+        <v>98.52398523985239</v>
       </c>
       <c r="H76" t="n">
         <v>100</v>
       </c>
       <c r="I76" t="n">
-        <v>0.01104972375690608</v>
+        <v>0.0147329650092081</v>
       </c>
       <c r="J76" t="n">
-        <v>441.5104689598083</v>
+        <v>68.30287003517151</v>
       </c>
     </row>
     <row r="77">
@@ -3055,7 +3055,7 @@
         <v>0.04296296296296296</v>
       </c>
       <c r="J77" t="n">
-        <v>260.8916940689087</v>
+        <v>54.18106770515442</v>
       </c>
     </row>
     <row r="78">
@@ -3071,25 +3071,25 @@
         <v>2145</v>
       </c>
       <c r="D78" t="n">
-        <v>2141</v>
+        <v>2142</v>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G78" t="n">
-        <v>99.86007462686567</v>
+        <v>99.90671641791045</v>
       </c>
       <c r="H78" t="n">
-        <v>99.95331465919701</v>
+        <v>100</v>
       </c>
       <c r="I78" t="n">
-        <v>0.001864801864801865</v>
+        <v>0.0009324009324009324</v>
       </c>
       <c r="J78" t="n">
-        <v>530.2923488616943</v>
+        <v>69.41012048721313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the first criterions values
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/AHA_database.xlsx
+++ b/R peak detection/beatdetection/AHA_database.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="vdgydgfe" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sahcjhdc" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,31 +447,31 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1636</v>
+        <v>1646</v>
       </c>
       <c r="C1" t="n">
         <v>1622</v>
       </c>
       <c r="D1" t="n">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="E1" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" t="n">
-        <v>99.93830968537939</v>
+        <v>100</v>
       </c>
       <c r="H1" t="n">
-        <v>99.08256880733946</v>
+        <v>98.54103343465046</v>
       </c>
       <c r="I1" t="n">
-        <v>0.009864364981504316</v>
+        <v>0.01479654747225647</v>
       </c>
       <c r="J1" t="n">
-        <v>53.132976770401</v>
+        <v>52.27596759796143</v>
       </c>
     </row>
     <row r="2">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2595</v>
+        <v>2597</v>
       </c>
       <c r="C2" t="n">
         <v>2595</v>
@@ -490,7 +490,7 @@
         <v>2594</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -499,13 +499,13 @@
         <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>99.92295839753467</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.0007707129094412332</v>
       </c>
       <c r="J2" t="n">
-        <v>39.7284562587738</v>
+        <v>37.44754314422607</v>
       </c>
     </row>
     <row r="3">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2181</v>
+        <v>2183</v>
       </c>
       <c r="C3" t="n">
         <v>2181</v>
@@ -524,7 +524,7 @@
         <v>2180</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -533,13 +533,13 @@
         <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>100</v>
+        <v>99.9083409715857</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.0009170105456212746</v>
       </c>
       <c r="J3" t="n">
-        <v>45.55912399291992</v>
+        <v>44.58232259750366</v>
       </c>
     </row>
     <row r="4">
@@ -549,31 +549,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2943</v>
+        <v>2944</v>
       </c>
       <c r="C4" t="n">
         <v>2974</v>
       </c>
       <c r="D4" t="n">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G4" t="n">
-        <v>98.92364614867138</v>
+        <v>98.89001009081736</v>
       </c>
       <c r="H4" t="n">
-        <v>99.96600951733515</v>
+        <v>99.8980632008155</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01109616677874916</v>
+        <v>0.0121049092131809</v>
       </c>
       <c r="J4" t="n">
-        <v>38.57578897476196</v>
+        <v>38.54309749603271</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>47.92852783203125</v>
+        <v>44.170729637146</v>
       </c>
     </row>
     <row r="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2122</v>
+        <v>2123</v>
       </c>
       <c r="C6" t="n">
         <v>2122</v>
@@ -626,7 +626,7 @@
         <v>2121</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -635,13 +635,13 @@
         <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>100</v>
+        <v>99.95287464655985</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>0.000471253534401508</v>
       </c>
       <c r="J6" t="n">
-        <v>44.39997386932373</v>
+        <v>42.25898385047913</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>42.72305607795715</v>
+        <v>41.91249537467957</v>
       </c>
     </row>
     <row r="8">
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>40.63794755935669</v>
+        <v>39.8234691619873</v>
       </c>
     </row>
     <row r="9">
@@ -719,31 +719,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3583</v>
+        <v>3584</v>
       </c>
       <c r="C9" t="n">
         <v>3582</v>
       </c>
       <c r="D9" t="n">
-        <v>3580</v>
+        <v>3581</v>
       </c>
       <c r="E9" t="n">
         <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>99.97207483943032</v>
+        <v>100</v>
       </c>
       <c r="H9" t="n">
-        <v>99.94416527079844</v>
+        <v>99.94418085403294</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0008375209380234506</v>
+        <v>0.0005583472920156337</v>
       </c>
       <c r="J9" t="n">
-        <v>49.82845020294189</v>
+        <v>30.35046863555908</v>
       </c>
     </row>
     <row r="10">
@@ -753,31 +753,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2043</v>
+        <v>2076</v>
       </c>
       <c r="C10" t="n">
         <v>1997</v>
       </c>
       <c r="D10" t="n">
-        <v>1987</v>
+        <v>1991</v>
       </c>
       <c r="E10" t="n">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="F10" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G10" t="n">
-        <v>99.54909819639279</v>
+        <v>99.74949899799599</v>
       </c>
       <c r="H10" t="n">
-        <v>97.30656219392752</v>
+        <v>95.95180722891567</v>
       </c>
       <c r="I10" t="n">
-        <v>0.03204807210816224</v>
+        <v>0.04456685027541312</v>
       </c>
       <c r="J10" t="n">
-        <v>52.44508409500122</v>
+        <v>49.65616512298584</v>
       </c>
     </row>
     <row r="11">
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>33.45886707305908</v>
+        <v>31.62161588668823</v>
       </c>
     </row>
     <row r="12">
@@ -845,7 +845,7 @@
         <v>0.0004142502071251035</v>
       </c>
       <c r="J12" t="n">
-        <v>42.92843580245972</v>
+        <v>42.17319846153259</v>
       </c>
     </row>
     <row r="13">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1632</v>
+        <v>1640</v>
       </c>
       <c r="C13" t="n">
         <v>1628</v>
@@ -864,7 +864,7 @@
         <v>1627</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -873,13 +873,13 @@
         <v>100</v>
       </c>
       <c r="H13" t="n">
-        <v>99.75475168608216</v>
+        <v>99.26784624771201</v>
       </c>
       <c r="I13" t="n">
-        <v>0.002457002457002457</v>
+        <v>0.007371007371007371</v>
       </c>
       <c r="J13" t="n">
-        <v>39.96148109436035</v>
+        <v>39.75209832191467</v>
       </c>
     </row>
     <row r="14">
@@ -913,7 +913,7 @@
         <v>0.0006199628022318661</v>
       </c>
       <c r="J14" t="n">
-        <v>49.09306263923645</v>
+        <v>48.3426558971405</v>
       </c>
     </row>
     <row r="15">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>42.58173489570618</v>
+        <v>35.24733471870422</v>
       </c>
     </row>
     <row r="16">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>38.49989485740662</v>
+        <v>36.98453426361084</v>
       </c>
     </row>
     <row r="17">
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>41.38833498954773</v>
+        <v>38.85833930969238</v>
       </c>
     </row>
     <row r="18">
@@ -1025,31 +1025,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2539</v>
+        <v>2543</v>
       </c>
       <c r="C18" t="n">
         <v>2537</v>
       </c>
       <c r="D18" t="n">
-        <v>2533</v>
+        <v>2534</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18" t="n">
-        <v>99.88170347003154</v>
+        <v>99.9211356466877</v>
       </c>
       <c r="H18" t="n">
-        <v>99.80299448384555</v>
+        <v>99.6852871754524</v>
       </c>
       <c r="I18" t="n">
-        <v>0.003153330705557745</v>
+        <v>0.003941663381947182</v>
       </c>
       <c r="J18" t="n">
-        <v>51.23068714141846</v>
+        <v>49.43160891532898</v>
       </c>
     </row>
     <row r="19">
@@ -1083,7 +1083,7 @@
         <v>0.002296738631143776</v>
       </c>
       <c r="J19" t="n">
-        <v>47.28110456466675</v>
+        <v>45.50825595855713</v>
       </c>
     </row>
     <row r="20">
@@ -1099,25 +1099,25 @@
         <v>2943</v>
       </c>
       <c r="D20" t="n">
-        <v>2941</v>
+        <v>2942</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>99.96600951733515</v>
+        <v>100</v>
       </c>
       <c r="H20" t="n">
-        <v>99.96600951733515</v>
+        <v>100</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0006795786612300374</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>43.43896412849426</v>
+        <v>42.40396881103516</v>
       </c>
     </row>
     <row r="21">
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1954</v>
+        <v>1955</v>
       </c>
       <c r="C21" t="n">
         <v>1950</v>
@@ -1136,7 +1136,7 @@
         <v>1949</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -1145,13 +1145,13 @@
         <v>100</v>
       </c>
       <c r="H21" t="n">
-        <v>99.79518689196108</v>
+        <v>99.74411463664278</v>
       </c>
       <c r="I21" t="n">
-        <v>0.002051282051282051</v>
+        <v>0.002564102564102564</v>
       </c>
       <c r="J21" t="n">
-        <v>41.88124299049377</v>
+        <v>41.40494346618652</v>
       </c>
     </row>
     <row r="22">
@@ -1167,25 +1167,25 @@
         <v>1878</v>
       </c>
       <c r="D22" t="n">
-        <v>1875</v>
+        <v>1877</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>99.89344698987746</v>
+        <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>99.89344698987746</v>
+        <v>100</v>
       </c>
       <c r="I22" t="n">
-        <v>0.002129925452609159</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>51.17532539367676</v>
+        <v>49.15558266639709</v>
       </c>
     </row>
     <row r="23">
@@ -1219,7 +1219,7 @@
         <v>0.001121076233183856</v>
       </c>
       <c r="J23" t="n">
-        <v>43.67114114761353</v>
+        <v>43.26976871490479</v>
       </c>
     </row>
     <row r="24">
@@ -1235,25 +1235,25 @@
         <v>3245</v>
       </c>
       <c r="D24" t="n">
-        <v>3243</v>
+        <v>3244</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>99.9691738594328</v>
+        <v>100</v>
       </c>
       <c r="H24" t="n">
-        <v>99.9691738594328</v>
+        <v>100</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0006163328197226503</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>35.35506272315979</v>
+        <v>33.49357557296753</v>
       </c>
     </row>
     <row r="25">
@@ -1269,25 +1269,25 @@
         <v>2324</v>
       </c>
       <c r="D25" t="n">
-        <v>2308</v>
+        <v>2322</v>
       </c>
       <c r="E25" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>99.35428325441239</v>
+        <v>99.95695221696083</v>
       </c>
       <c r="H25" t="n">
-        <v>99.39707149009475</v>
+        <v>100</v>
       </c>
       <c r="I25" t="n">
-        <v>0.01247848537005163</v>
+        <v>0.0004302925989672978</v>
       </c>
       <c r="J25" t="n">
-        <v>46.46960091590881</v>
+        <v>43.17362904548645</v>
       </c>
     </row>
     <row r="26">
@@ -1321,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>43.79783964157104</v>
+        <v>43.25995492935181</v>
       </c>
     </row>
     <row r="27">
@@ -1331,7 +1331,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2586</v>
+        <v>2587</v>
       </c>
       <c r="C27" t="n">
         <v>2584</v>
@@ -1340,7 +1340,7 @@
         <v>2583</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1349,13 +1349,13 @@
         <v>100</v>
       </c>
       <c r="H27" t="n">
-        <v>99.92263056092844</v>
+        <v>99.88399071925754</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0007739938080495357</v>
+        <v>0.001160990712074303</v>
       </c>
       <c r="J27" t="n">
-        <v>43.88408231735229</v>
+        <v>42.09691071510315</v>
       </c>
     </row>
     <row r="28">
@@ -1365,31 +1365,31 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2449</v>
+        <v>2451</v>
       </c>
       <c r="C28" t="n">
         <v>2472</v>
       </c>
       <c r="D28" t="n">
-        <v>2443</v>
+        <v>2448</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G28" t="n">
-        <v>98.86685552407933</v>
+        <v>99.0692027519223</v>
       </c>
       <c r="H28" t="n">
-        <v>99.79575163398692</v>
+        <v>99.91836734693878</v>
       </c>
       <c r="I28" t="n">
-        <v>0.0133495145631068</v>
+        <v>0.01011326860841424</v>
       </c>
       <c r="J28" t="n">
-        <v>37.47303247451782</v>
+        <v>36.36382722854614</v>
       </c>
     </row>
     <row r="29">
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>42.88022089004517</v>
+        <v>42.59109139442444</v>
       </c>
     </row>
     <row r="30">
@@ -1433,31 +1433,31 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2367</v>
+        <v>2368</v>
       </c>
       <c r="C30" t="n">
         <v>2376</v>
       </c>
       <c r="D30" t="n">
-        <v>2365</v>
+        <v>2366</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30" t="n">
-        <v>99.57894736842105</v>
+        <v>99.62105263157895</v>
       </c>
       <c r="H30" t="n">
-        <v>99.95773457311918</v>
+        <v>99.95775242923531</v>
       </c>
       <c r="I30" t="n">
-        <v>0.004629629629629629</v>
+        <v>0.004208754208754209</v>
       </c>
       <c r="J30" t="n">
-        <v>41.97994041442871</v>
+        <v>39.60499286651611</v>
       </c>
     </row>
     <row r="31">
@@ -1467,31 +1467,31 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2581</v>
+        <v>2582</v>
       </c>
       <c r="C31" t="n">
         <v>2582</v>
       </c>
       <c r="D31" t="n">
-        <v>2580</v>
+        <v>2581</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>99.96125532739248</v>
+        <v>100</v>
       </c>
       <c r="H31" t="n">
         <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0003872966692486445</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>46.69895267486572</v>
+        <v>42.3595449924469</v>
       </c>
     </row>
     <row r="32">
@@ -1501,31 +1501,31 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2258</v>
+        <v>2259</v>
       </c>
       <c r="C32" t="n">
         <v>2258</v>
       </c>
       <c r="D32" t="n">
-        <v>2253</v>
+        <v>2257</v>
       </c>
       <c r="E32" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>99.8227735932654</v>
+        <v>100</v>
       </c>
       <c r="H32" t="n">
-        <v>99.8227735932654</v>
+        <v>99.95571302037202</v>
       </c>
       <c r="I32" t="n">
-        <v>0.00354295837023915</v>
+        <v>0.0004428697962798937</v>
       </c>
       <c r="J32" t="n">
-        <v>37.5033061504364</v>
+        <v>36.50954580307007</v>
       </c>
     </row>
     <row r="33">
@@ -1535,31 +1535,31 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1452</v>
+        <v>1457</v>
       </c>
       <c r="C33" t="n">
         <v>1452</v>
       </c>
       <c r="D33" t="n">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G33" t="n">
-        <v>99.58649207443143</v>
+        <v>99.65541006202619</v>
       </c>
       <c r="H33" t="n">
-        <v>99.58649207443143</v>
+        <v>99.31318681318682</v>
       </c>
       <c r="I33" t="n">
-        <v>0.008264462809917356</v>
+        <v>0.01033057851239669</v>
       </c>
       <c r="J33" t="n">
-        <v>51.62883234024048</v>
+        <v>49.96272349357605</v>
       </c>
     </row>
     <row r="34">
@@ -1569,31 +1569,31 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1946</v>
+        <v>1941</v>
       </c>
       <c r="C34" t="n">
         <v>1947</v>
       </c>
       <c r="D34" t="n">
-        <v>1945</v>
+        <v>1940</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G34" t="n">
-        <v>99.9486125385406</v>
+        <v>99.69167523124358</v>
       </c>
       <c r="H34" t="n">
         <v>100</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0005136106831022085</v>
+        <v>0.003081664098613251</v>
       </c>
       <c r="J34" t="n">
-        <v>39.41153311729431</v>
+        <v>40.64520740509033</v>
       </c>
     </row>
     <row r="35">
@@ -1603,31 +1603,31 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3520</v>
+        <v>3521</v>
       </c>
       <c r="C35" t="n">
         <v>3520</v>
       </c>
       <c r="D35" t="n">
-        <v>3517</v>
+        <v>3519</v>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>99.94316567206593</v>
+        <v>100</v>
       </c>
       <c r="H35" t="n">
-        <v>99.94316567206593</v>
+        <v>99.97159090909091</v>
       </c>
       <c r="I35" t="n">
-        <v>0.001136363636363636</v>
+        <v>0.0002840909090909091</v>
       </c>
       <c r="J35" t="n">
-        <v>45.72541284561157</v>
+        <v>32.74433255195618</v>
       </c>
     </row>
     <row r="36">
@@ -1637,7 +1637,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1882</v>
+        <v>1886</v>
       </c>
       <c r="C36" t="n">
         <v>1878</v>
@@ -1646,7 +1646,7 @@
         <v>1877</v>
       </c>
       <c r="E36" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1655,13 +1655,13 @@
         <v>100</v>
       </c>
       <c r="H36" t="n">
-        <v>99.7873471557682</v>
+        <v>99.57559681697613</v>
       </c>
       <c r="I36" t="n">
-        <v>0.002129925452609159</v>
+        <v>0.004259850905218318</v>
       </c>
       <c r="J36" t="n">
-        <v>41.95764207839966</v>
+        <v>41.56852269172668</v>
       </c>
     </row>
     <row r="37">
@@ -1677,25 +1677,25 @@
         <v>2371</v>
       </c>
       <c r="D37" t="n">
-        <v>2365</v>
+        <v>2367</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G37" t="n">
-        <v>99.78902953586498</v>
+        <v>99.87341772151899</v>
       </c>
       <c r="H37" t="n">
-        <v>99.91550485847064</v>
+        <v>100</v>
       </c>
       <c r="I37" t="n">
-        <v>0.002952340784479123</v>
+        <v>0.00126528890763391</v>
       </c>
       <c r="J37" t="n">
-        <v>50.67544746398926</v>
+        <v>44.75942325592041</v>
       </c>
     </row>
     <row r="38">
@@ -1705,31 +1705,31 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2906</v>
+        <v>2907</v>
       </c>
       <c r="C38" t="n">
         <v>2907</v>
       </c>
       <c r="D38" t="n">
-        <v>2905</v>
+        <v>2906</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>99.96558843771507</v>
+        <v>100</v>
       </c>
       <c r="H38" t="n">
         <v>100</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0003439972480220158</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>35.34384179115295</v>
+        <v>33.52435040473938</v>
       </c>
     </row>
     <row r="39">
@@ -1739,31 +1739,31 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2126</v>
+        <v>2204</v>
       </c>
       <c r="C39" t="n">
         <v>2257</v>
       </c>
       <c r="D39" t="n">
-        <v>2125</v>
+        <v>2202</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="G39" t="n">
-        <v>94.19326241134752</v>
+        <v>97.6063829787234</v>
       </c>
       <c r="H39" t="n">
-        <v>100</v>
+        <v>99.95460735360872</v>
       </c>
       <c r="I39" t="n">
-        <v>0.05804164820558263</v>
+        <v>0.02436863092600797</v>
       </c>
       <c r="J39" t="n">
-        <v>36.34434533119202</v>
+        <v>34.6678581237793</v>
       </c>
     </row>
     <row r="40">
@@ -1779,25 +1779,25 @@
         <v>2351</v>
       </c>
       <c r="D40" t="n">
-        <v>2272</v>
+        <v>2350</v>
       </c>
       <c r="E40" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>96.68085106382979</v>
+        <v>100</v>
       </c>
       <c r="H40" t="n">
-        <v>96.68085106382979</v>
+        <v>100</v>
       </c>
       <c r="I40" t="n">
-        <v>0.06635474266269673</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>42.92795062065125</v>
+        <v>42.31657028198242</v>
       </c>
     </row>
     <row r="41">
@@ -1831,7 +1831,7 @@
         <v>0.0004212299915754001</v>
       </c>
       <c r="J41" t="n">
-        <v>38.71389985084534</v>
+        <v>36.85695815086365</v>
       </c>
     </row>
     <row r="42">
@@ -1841,31 +1841,31 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>2286</v>
+        <v>2287</v>
       </c>
       <c r="C42" t="n">
         <v>2287</v>
       </c>
       <c r="D42" t="n">
-        <v>2285</v>
+        <v>2286</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>99.95625546806649</v>
+        <v>100</v>
       </c>
       <c r="H42" t="n">
         <v>100</v>
       </c>
       <c r="I42" t="n">
-        <v>0.0004372540445999126</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>45.30891060829163</v>
+        <v>39.94545125961304</v>
       </c>
     </row>
     <row r="43">
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>43.83182573318481</v>
+        <v>43.2958071231842</v>
       </c>
     </row>
     <row r="44">
@@ -1909,7 +1909,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2068</v>
+        <v>2078</v>
       </c>
       <c r="C44" t="n">
         <v>2068</v>
@@ -1918,7 +1918,7 @@
         <v>2066</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -1927,13 +1927,13 @@
         <v>99.95162070633769</v>
       </c>
       <c r="H44" t="n">
-        <v>99.95162070633769</v>
+        <v>99.4703899855561</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0009671179883945841</v>
+        <v>0.005802707930367505</v>
       </c>
       <c r="J44" t="n">
-        <v>42.22286629676819</v>
+        <v>41.93298411369324</v>
       </c>
     </row>
     <row r="45">
@@ -1943,31 +1943,31 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2914</v>
+        <v>2922</v>
       </c>
       <c r="C45" t="n">
         <v>2923</v>
       </c>
       <c r="D45" t="n">
-        <v>2913</v>
+        <v>2921</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G45" t="n">
-        <v>99.69199178644764</v>
+        <v>99.96577686516085</v>
       </c>
       <c r="H45" t="n">
         <v>100</v>
       </c>
       <c r="I45" t="n">
-        <v>0.003079028395484092</v>
+        <v>0.0003421142661648991</v>
       </c>
       <c r="J45" t="n">
-        <v>41.07178282737732</v>
+        <v>37.44164514541626</v>
       </c>
     </row>
     <row r="46">
@@ -1983,25 +1983,25 @@
         <v>1845</v>
       </c>
       <c r="D46" t="n">
-        <v>1833</v>
+        <v>1844</v>
       </c>
       <c r="E46" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>99.40347071583514</v>
+        <v>100</v>
       </c>
       <c r="H46" t="n">
-        <v>99.40347071583514</v>
+        <v>100</v>
       </c>
       <c r="I46" t="n">
-        <v>0.01192411924119241</v>
+        <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>46.75041842460632</v>
+        <v>44.58977437019348</v>
       </c>
     </row>
     <row r="47">
@@ -2011,7 +2011,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2164</v>
+        <v>2166</v>
       </c>
       <c r="C47" t="n">
         <v>2164</v>
@@ -2020,7 +2020,7 @@
         <v>2163</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -2029,13 +2029,13 @@
         <v>100</v>
       </c>
       <c r="H47" t="n">
-        <v>100</v>
+        <v>99.90762124711317</v>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>0.0009242144177449168</v>
       </c>
       <c r="J47" t="n">
-        <v>41.17143487930298</v>
+        <v>39.75320172309875</v>
       </c>
     </row>
     <row r="48">
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2048</v>
+        <v>2155</v>
       </c>
       <c r="C48" t="n">
         <v>2017</v>
@@ -2054,7 +2054,7 @@
         <v>2016</v>
       </c>
       <c r="E48" t="n">
-        <v>31</v>
+        <v>138</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -2063,13 +2063,13 @@
         <v>100</v>
       </c>
       <c r="H48" t="n">
-        <v>98.48558866634099</v>
+        <v>93.59331476323119</v>
       </c>
       <c r="I48" t="n">
-        <v>0.01536936043629152</v>
+        <v>0.06841844323252355</v>
       </c>
       <c r="J48" t="n">
-        <v>49.63862681388855</v>
+        <v>32.54594302177429</v>
       </c>
     </row>
     <row r="49">
@@ -2103,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>46.51400136947632</v>
+        <v>45.51438045501709</v>
       </c>
     </row>
     <row r="50">
@@ -2137,7 +2137,7 @@
         <v>0.004608294930875576</v>
       </c>
       <c r="J50" t="n">
-        <v>47.91498255729675</v>
+        <v>46.73506903648376</v>
       </c>
     </row>
     <row r="51">
@@ -2153,25 +2153,25 @@
         <v>2698</v>
       </c>
       <c r="D51" t="n">
-        <v>2680</v>
+        <v>2696</v>
       </c>
       <c r="E51" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>99.36967000370782</v>
+        <v>99.96292176492399</v>
       </c>
       <c r="H51" t="n">
-        <v>99.40652818991099</v>
+        <v>100</v>
       </c>
       <c r="I51" t="n">
-        <v>0.01223128243143069</v>
+        <v>0.0003706449221645663</v>
       </c>
       <c r="J51" t="n">
-        <v>41.67695331573486</v>
+        <v>40.9460244178772</v>
       </c>
     </row>
     <row r="52">
@@ -2181,31 +2181,31 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2250</v>
+        <v>2251</v>
       </c>
       <c r="C52" t="n">
         <v>2251</v>
       </c>
       <c r="D52" t="n">
-        <v>2249</v>
+        <v>2250</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>99.95555555555555</v>
+        <v>100</v>
       </c>
       <c r="H52" t="n">
         <v>100</v>
       </c>
       <c r="I52" t="n">
-        <v>0.000444247001332741</v>
+        <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>44.780024766922</v>
+        <v>43.46905112266541</v>
       </c>
     </row>
     <row r="53">
@@ -2221,25 +2221,25 @@
         <v>2294</v>
       </c>
       <c r="D53" t="n">
-        <v>2286</v>
+        <v>2293</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>99.6947230702137</v>
+        <v>100</v>
       </c>
       <c r="H53" t="n">
-        <v>99.6947230702137</v>
+        <v>100</v>
       </c>
       <c r="I53" t="n">
-        <v>0.006102877070619006</v>
+        <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>48.28517436981201</v>
+        <v>45.77689003944397</v>
       </c>
     </row>
     <row r="54">
@@ -2249,31 +2249,31 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2779</v>
+        <v>2777</v>
       </c>
       <c r="C54" t="n">
         <v>2785</v>
       </c>
       <c r="D54" t="n">
-        <v>2719</v>
+        <v>2776</v>
       </c>
       <c r="E54" t="n">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="G54" t="n">
-        <v>97.66522988505747</v>
+        <v>99.71264367816092</v>
       </c>
       <c r="H54" t="n">
-        <v>97.87616990640748</v>
+        <v>100</v>
       </c>
       <c r="I54" t="n">
-        <v>0.04452423698384201</v>
+        <v>0.002872531418312388</v>
       </c>
       <c r="J54" t="n">
-        <v>33.60817241668701</v>
+        <v>32.6847288608551</v>
       </c>
     </row>
     <row r="55">
@@ -2307,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>44.33131980895996</v>
+        <v>44.11378479003906</v>
       </c>
     </row>
     <row r="56">
@@ -2323,25 +2323,25 @@
         <v>2359</v>
       </c>
       <c r="D56" t="n">
-        <v>2357</v>
+        <v>2358</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>99.95759117896523</v>
+        <v>100</v>
       </c>
       <c r="H56" t="n">
-        <v>99.95759117896523</v>
+        <v>100</v>
       </c>
       <c r="I56" t="n">
-        <v>0.000847816871555744</v>
+        <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>36.6710844039917</v>
+        <v>35.52968215942383</v>
       </c>
     </row>
     <row r="57">
@@ -2357,25 +2357,25 @@
         <v>2500</v>
       </c>
       <c r="D57" t="n">
-        <v>2490</v>
+        <v>2499</v>
       </c>
       <c r="E57" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F57" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>99.63985594237695</v>
+        <v>100</v>
       </c>
       <c r="H57" t="n">
-        <v>99.59999999999999</v>
+        <v>99.95999999999999</v>
       </c>
       <c r="I57" t="n">
-        <v>0.0076</v>
+        <v>0.0004</v>
       </c>
       <c r="J57" t="n">
-        <v>45.32866668701172</v>
+        <v>43.56386017799377</v>
       </c>
     </row>
     <row r="58">
@@ -2385,31 +2385,31 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>3288</v>
+        <v>3289</v>
       </c>
       <c r="C58" t="n">
         <v>3289</v>
       </c>
       <c r="D58" t="n">
-        <v>3287</v>
+        <v>3288</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>99.96958637469587</v>
+        <v>100</v>
       </c>
       <c r="H58" t="n">
         <v>100</v>
       </c>
       <c r="I58" t="n">
-        <v>0.0003040437823046519</v>
+        <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>38.3699095249176</v>
+        <v>35.19466376304626</v>
       </c>
     </row>
     <row r="59">
@@ -2419,31 +2419,31 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>3156</v>
+        <v>3157</v>
       </c>
       <c r="C59" t="n">
         <v>3164</v>
       </c>
       <c r="D59" t="n">
-        <v>3150</v>
+        <v>3156</v>
       </c>
       <c r="E59" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G59" t="n">
-        <v>99.58899778691116</v>
+        <v>99.77869111602908</v>
       </c>
       <c r="H59" t="n">
-        <v>99.84152139461173</v>
+        <v>100</v>
       </c>
       <c r="I59" t="n">
-        <v>0.005689001264222503</v>
+        <v>0.002212389380530973</v>
       </c>
       <c r="J59" t="n">
-        <v>40.85526466369629</v>
+        <v>34.22929835319519</v>
       </c>
     </row>
     <row r="60">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>49.21147418022156</v>
+        <v>47.20427298545837</v>
       </c>
     </row>
     <row r="61">
@@ -2487,31 +2487,31 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2533</v>
+        <v>2535</v>
       </c>
       <c r="C61" t="n">
         <v>2533</v>
       </c>
       <c r="D61" t="n">
-        <v>2531</v>
+        <v>2532</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>99.96050552922591</v>
+        <v>100</v>
       </c>
       <c r="H61" t="n">
-        <v>99.96050552922591</v>
+        <v>99.92107340173638</v>
       </c>
       <c r="I61" t="n">
         <v>0.0007895775759968417</v>
       </c>
       <c r="J61" t="n">
-        <v>36.27220129966736</v>
+        <v>34.87859582901001</v>
       </c>
     </row>
     <row r="62">
@@ -2521,31 +2521,31 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>1921</v>
+        <v>1927</v>
       </c>
       <c r="C62" t="n">
         <v>1927</v>
       </c>
       <c r="D62" t="n">
-        <v>1920</v>
+        <v>1924</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F62" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G62" t="n">
-        <v>99.68847352024922</v>
+        <v>99.89615784008308</v>
       </c>
       <c r="H62" t="n">
-        <v>100</v>
+        <v>99.89615784008308</v>
       </c>
       <c r="I62" t="n">
-        <v>0.003113648157758173</v>
+        <v>0.002075765438505449</v>
       </c>
       <c r="J62" t="n">
-        <v>36.93985533714294</v>
+        <v>36.22535061836243</v>
       </c>
     </row>
     <row r="63">
@@ -2555,31 +2555,31 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2436</v>
+        <v>2442</v>
       </c>
       <c r="C63" t="n">
         <v>2437</v>
       </c>
       <c r="D63" t="n">
-        <v>2430</v>
+        <v>2431</v>
       </c>
       <c r="E63" t="n">
+        <v>10</v>
+      </c>
+      <c r="F63" t="n">
         <v>5</v>
       </c>
-      <c r="F63" t="n">
-        <v>6</v>
-      </c>
       <c r="G63" t="n">
-        <v>99.75369458128078</v>
+        <v>99.79474548440065</v>
       </c>
       <c r="H63" t="n">
-        <v>99.79466119096509</v>
+        <v>99.59033183121672</v>
       </c>
       <c r="I63" t="n">
-        <v>0.004513746409519901</v>
+        <v>0.006155108740254411</v>
       </c>
       <c r="J63" t="n">
-        <v>42.44726395606995</v>
+        <v>42.51649332046509</v>
       </c>
     </row>
     <row r="64">
@@ -2589,31 +2589,31 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>3049</v>
+        <v>3109</v>
       </c>
       <c r="C64" t="n">
         <v>3109</v>
       </c>
       <c r="D64" t="n">
-        <v>3048</v>
+        <v>3108</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>98.06949806949807</v>
+        <v>100</v>
       </c>
       <c r="H64" t="n">
         <v>100</v>
       </c>
       <c r="I64" t="n">
-        <v>0.01929880990672242</v>
+        <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>54.35197806358337</v>
+        <v>41.51781320571899</v>
       </c>
     </row>
     <row r="65">
@@ -2623,31 +2623,31 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2339</v>
+        <v>2345</v>
       </c>
       <c r="C65" t="n">
         <v>2340</v>
       </c>
       <c r="D65" t="n">
-        <v>2336</v>
+        <v>2338</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F65" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G65" t="n">
-        <v>99.87174005985464</v>
+        <v>99.95724668661822</v>
       </c>
       <c r="H65" t="n">
-        <v>99.91445680068435</v>
+        <v>99.74402730375427</v>
       </c>
       <c r="I65" t="n">
-        <v>0.002136752136752137</v>
+        <v>0.002991452991452992</v>
       </c>
       <c r="J65" t="n">
-        <v>39.66250681877136</v>
+        <v>38.65426015853882</v>
       </c>
     </row>
     <row r="66">
@@ -2657,31 +2657,31 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="C66" t="n">
         <v>1565</v>
       </c>
       <c r="D66" t="n">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>99.93606138107417</v>
+        <v>100</v>
       </c>
       <c r="H66" t="n">
         <v>100</v>
       </c>
       <c r="I66" t="n">
-        <v>0.0006389776357827476</v>
+        <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>42.3455638885498</v>
+        <v>41.5362913608551</v>
       </c>
     </row>
     <row r="67">
@@ -2691,31 +2691,31 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="C67" t="n">
         <v>2897</v>
       </c>
       <c r="D67" t="n">
-        <v>2680</v>
+        <v>2896</v>
       </c>
       <c r="E67" t="n">
-        <v>217</v>
+        <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>216</v>
+        <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>92.54143646408839</v>
+        <v>100</v>
       </c>
       <c r="H67" t="n">
-        <v>92.50949257852952</v>
+        <v>100</v>
       </c>
       <c r="I67" t="n">
-        <v>0.1494649637556092</v>
+        <v>0</v>
       </c>
       <c r="J67" t="n">
-        <v>48.20941090583801</v>
+        <v>42.67780494689941</v>
       </c>
     </row>
     <row r="68">
@@ -2725,31 +2725,31 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1749</v>
+        <v>1754</v>
       </c>
       <c r="C68" t="n">
         <v>1753</v>
       </c>
       <c r="D68" t="n">
-        <v>1748</v>
+        <v>1751</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F68" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G68" t="n">
-        <v>99.77168949771689</v>
+        <v>99.94292237442923</v>
       </c>
       <c r="H68" t="n">
-        <v>100</v>
+        <v>99.88590986879635</v>
       </c>
       <c r="I68" t="n">
-        <v>0.002281802624073018</v>
+        <v>0.001711351968054763</v>
       </c>
       <c r="J68" t="n">
-        <v>45.47977447509766</v>
+        <v>44.7093551158905</v>
       </c>
     </row>
     <row r="69">
@@ -2783,7 +2783,7 @@
         <v>0.002741603838245374</v>
       </c>
       <c r="J69" t="n">
-        <v>48.22821068763733</v>
+        <v>47.57292461395264</v>
       </c>
     </row>
     <row r="70">
@@ -2793,31 +2793,31 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1755</v>
+        <v>1771</v>
       </c>
       <c r="C70" t="n">
         <v>1787</v>
       </c>
       <c r="D70" t="n">
-        <v>1750</v>
+        <v>1765</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F70" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G70" t="n">
-        <v>97.92949076664802</v>
+        <v>98.76888640179071</v>
       </c>
       <c r="H70" t="n">
-        <v>99.77194982896238</v>
+        <v>99.71751412429379</v>
       </c>
       <c r="I70" t="n">
-        <v>0.02294348069390039</v>
+        <v>0.01510912143256855</v>
       </c>
       <c r="J70" t="n">
-        <v>36.31299090385437</v>
+        <v>35.72090625762939</v>
       </c>
     </row>
     <row r="71">
@@ -2827,31 +2827,31 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1534</v>
+        <v>1551</v>
       </c>
       <c r="C71" t="n">
         <v>1567</v>
       </c>
       <c r="D71" t="n">
-        <v>1531</v>
+        <v>1550</v>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G71" t="n">
-        <v>97.76500638569604</v>
+        <v>98.97828863346105</v>
       </c>
       <c r="H71" t="n">
-        <v>99.86953685583822</v>
+        <v>100</v>
       </c>
       <c r="I71" t="n">
-        <v>0.02361199744735163</v>
+        <v>0.01021059349074665</v>
       </c>
       <c r="J71" t="n">
-        <v>49.01823663711548</v>
+        <v>36.45135927200317</v>
       </c>
     </row>
     <row r="72">
@@ -2861,31 +2861,31 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="C72" t="n">
         <v>920</v>
       </c>
       <c r="D72" t="n">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="E72" t="n">
         <v>1</v>
       </c>
       <c r="F72" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G72" t="n">
-        <v>98.69423286180631</v>
+        <v>99.56474428726877</v>
       </c>
       <c r="H72" t="n">
-        <v>99.8898678414097</v>
+        <v>99.89082969432314</v>
       </c>
       <c r="I72" t="n">
-        <v>0.0141304347826087</v>
+        <v>0.005434782608695652</v>
       </c>
       <c r="J72" t="n">
-        <v>46.75248098373413</v>
+        <v>44.91983652114868</v>
       </c>
     </row>
     <row r="73">
@@ -2895,31 +2895,31 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1151</v>
+        <v>1171</v>
       </c>
       <c r="C73" t="n">
         <v>1143</v>
       </c>
       <c r="D73" t="n">
-        <v>1120</v>
+        <v>1126</v>
       </c>
       <c r="E73" t="n">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F73" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G73" t="n">
-        <v>98.07355516637477</v>
+        <v>98.59894921190893</v>
       </c>
       <c r="H73" t="n">
-        <v>97.39130434782609</v>
+        <v>96.23931623931624</v>
       </c>
       <c r="I73" t="n">
-        <v>0.04549431321084865</v>
+        <v>0.05249343832020997</v>
       </c>
       <c r="J73" t="n">
-        <v>41.81941366195679</v>
+        <v>39.71299982070923</v>
       </c>
     </row>
     <row r="74">
@@ -2929,31 +2929,31 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1332</v>
+        <v>1342</v>
       </c>
       <c r="C74" t="n">
         <v>1356</v>
       </c>
       <c r="D74" t="n">
-        <v>1315</v>
+        <v>1325</v>
       </c>
       <c r="E74" t="n">
         <v>16</v>
       </c>
       <c r="F74" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G74" t="n">
-        <v>97.0479704797048</v>
+        <v>97.7859778597786</v>
       </c>
       <c r="H74" t="n">
-        <v>98.79789631855748</v>
+        <v>98.806860551827</v>
       </c>
       <c r="I74" t="n">
-        <v>0.04129793510324484</v>
+        <v>0.03392330383480826</v>
       </c>
       <c r="J74" t="n">
-        <v>52.64056539535522</v>
+        <v>41.83043575286865</v>
       </c>
     </row>
     <row r="75">
@@ -2963,31 +2963,31 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C75" t="n">
         <v>543</v>
       </c>
       <c r="D75" t="n">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G75" t="n">
-        <v>99.2619926199262</v>
+        <v>99.07749077490774</v>
       </c>
       <c r="H75" t="n">
         <v>100</v>
       </c>
       <c r="I75" t="n">
-        <v>0.007366482504604052</v>
+        <v>0.009208103130755065</v>
       </c>
       <c r="J75" t="n">
-        <v>48.8492751121521</v>
+        <v>45.27727079391479</v>
       </c>
     </row>
     <row r="76">
@@ -2997,31 +2997,31 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1943</v>
+        <v>1974</v>
       </c>
       <c r="C76" t="n">
         <v>2025</v>
       </c>
       <c r="D76" t="n">
-        <v>1942</v>
+        <v>1973</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="G76" t="n">
-        <v>95.94861660079052</v>
+        <v>97.4802371541502</v>
       </c>
       <c r="H76" t="n">
         <v>100</v>
       </c>
       <c r="I76" t="n">
-        <v>0.04049382716049383</v>
+        <v>0.02518518518518519</v>
       </c>
       <c r="J76" t="n">
-        <v>42.21176767349243</v>
+        <v>38.05605459213257</v>
       </c>
     </row>
     <row r="77">
@@ -3031,31 +3031,31 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>2142</v>
+        <v>2144</v>
       </c>
       <c r="C77" t="n">
         <v>2145</v>
       </c>
       <c r="D77" t="n">
-        <v>2136</v>
+        <v>2143</v>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G77" t="n">
-        <v>99.6268656716418</v>
+        <v>99.95335820895522</v>
       </c>
       <c r="H77" t="n">
-        <v>99.76646426903316</v>
+        <v>100</v>
       </c>
       <c r="I77" t="n">
-        <v>0.006060606060606061</v>
+        <v>0.0004662004662004662</v>
       </c>
       <c r="J77" t="n">
-        <v>48.48971939086914</v>
+        <v>41.29235649108887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the first R peak window to 0.3*fs
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/AHA_database.xlsx
+++ b/R peak detection/beatdetection/AHA_database.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sahcjhdc" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="gscgwuc" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1646</v>
+        <v>1643</v>
       </c>
       <c r="C1" t="n">
         <v>1622</v>
@@ -456,7 +456,7 @@
         <v>1621</v>
       </c>
       <c r="E1" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F1" t="n">
         <v>0</v>
@@ -465,13 +465,13 @@
         <v>100</v>
       </c>
       <c r="H1" t="n">
-        <v>98.54103343465046</v>
+        <v>98.721071863581</v>
       </c>
       <c r="I1" t="n">
-        <v>0.01479654747225647</v>
+        <v>0.01294697903822441</v>
       </c>
       <c r="J1" t="n">
-        <v>52.27596759796143</v>
+        <v>52.9605758190155</v>
       </c>
     </row>
     <row r="2">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="C2" t="n">
         <v>2595</v>
@@ -490,7 +490,7 @@
         <v>2594</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -499,13 +499,13 @@
         <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>99.92295839753467</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0007707129094412332</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>37.44754314422607</v>
+        <v>36.99648785591125</v>
       </c>
     </row>
     <row r="3">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="C3" t="n">
         <v>2181</v>
@@ -524,7 +524,7 @@
         <v>2180</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -533,13 +533,13 @@
         <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>99.9083409715857</v>
+        <v>99.95414947271894</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0009170105456212746</v>
+        <v>0.0004585052728106373</v>
       </c>
       <c r="J3" t="n">
-        <v>44.58232259750366</v>
+        <v>44.56078028678894</v>
       </c>
     </row>
     <row r="4">
@@ -549,31 +549,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2944</v>
+        <v>2939</v>
       </c>
       <c r="C4" t="n">
         <v>2974</v>
       </c>
       <c r="D4" t="n">
-        <v>2940</v>
+        <v>2936</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G4" t="n">
-        <v>98.89001009081736</v>
+        <v>98.75546585940128</v>
       </c>
       <c r="H4" t="n">
-        <v>99.8980632008155</v>
+        <v>99.93192648059905</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0121049092131809</v>
+        <v>0.01311365164761264</v>
       </c>
       <c r="J4" t="n">
-        <v>38.54309749603271</v>
+        <v>38.42226243019104</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>44.170729637146</v>
+        <v>44.00360679626465</v>
       </c>
     </row>
     <row r="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="C6" t="n">
         <v>2122</v>
@@ -626,7 +626,7 @@
         <v>2121</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -635,13 +635,13 @@
         <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>99.95287464655985</v>
+        <v>100</v>
       </c>
       <c r="I6" t="n">
-        <v>0.000471253534401508</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>42.25898385047913</v>
+        <v>42.20387578010559</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>41.91249537467957</v>
+        <v>42.274169921875</v>
       </c>
     </row>
     <row r="8">
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>39.8234691619873</v>
+        <v>40.643310546875</v>
       </c>
     </row>
     <row r="9">
@@ -719,7 +719,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="C9" t="n">
         <v>3582</v>
@@ -728,7 +728,7 @@
         <v>3581</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -737,13 +737,13 @@
         <v>100</v>
       </c>
       <c r="H9" t="n">
-        <v>99.94418085403294</v>
+        <v>99.97208263539922</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0005583472920156337</v>
+        <v>0.0002791736460078169</v>
       </c>
       <c r="J9" t="n">
-        <v>30.35046863555908</v>
+        <v>31.53788757324219</v>
       </c>
     </row>
     <row r="10">
@@ -753,7 +753,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2076</v>
+        <v>2045</v>
       </c>
       <c r="C10" t="n">
         <v>1997</v>
@@ -762,7 +762,7 @@
         <v>1991</v>
       </c>
       <c r="E10" t="n">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="F10" t="n">
         <v>5</v>
@@ -771,13 +771,13 @@
         <v>99.74949899799599</v>
       </c>
       <c r="H10" t="n">
-        <v>95.95180722891567</v>
+        <v>97.40704500978474</v>
       </c>
       <c r="I10" t="n">
-        <v>0.04456685027541312</v>
+        <v>0.02904356534802203</v>
       </c>
       <c r="J10" t="n">
-        <v>49.65616512298584</v>
+        <v>48.92391967773438</v>
       </c>
     </row>
     <row r="11">
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>31.62161588668823</v>
+        <v>32.3477954864502</v>
       </c>
     </row>
     <row r="12">
@@ -845,7 +845,7 @@
         <v>0.0004142502071251035</v>
       </c>
       <c r="J12" t="n">
-        <v>42.17319846153259</v>
+        <v>42.63553929328918</v>
       </c>
     </row>
     <row r="13">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="C13" t="n">
         <v>1628</v>
@@ -864,7 +864,7 @@
         <v>1627</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -873,13 +873,13 @@
         <v>100</v>
       </c>
       <c r="H13" t="n">
-        <v>99.26784624771201</v>
+        <v>99.38912645082468</v>
       </c>
       <c r="I13" t="n">
-        <v>0.007371007371007371</v>
+        <v>0.006142506142506142</v>
       </c>
       <c r="J13" t="n">
-        <v>39.75209832191467</v>
+        <v>40.82839941978455</v>
       </c>
     </row>
     <row r="14">
@@ -913,7 +913,7 @@
         <v>0.0006199628022318661</v>
       </c>
       <c r="J14" t="n">
-        <v>48.3426558971405</v>
+        <v>49.46972990036011</v>
       </c>
     </row>
     <row r="15">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>35.24733471870422</v>
+        <v>35.96109127998352</v>
       </c>
     </row>
     <row r="16">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>36.98453426361084</v>
+        <v>38.06334471702576</v>
       </c>
     </row>
     <row r="17">
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>38.85833930969238</v>
+        <v>40.34566068649292</v>
       </c>
     </row>
     <row r="18">
@@ -1025,31 +1025,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2543</v>
+        <v>2536</v>
       </c>
       <c r="C18" t="n">
         <v>2537</v>
       </c>
       <c r="D18" t="n">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" t="n">
-        <v>99.9211356466877</v>
+        <v>99.88170347003154</v>
       </c>
       <c r="H18" t="n">
-        <v>99.6852871754524</v>
+        <v>99.92110453648915</v>
       </c>
       <c r="I18" t="n">
-        <v>0.003941663381947182</v>
+        <v>0.001970831690973591</v>
       </c>
       <c r="J18" t="n">
-        <v>49.43160891532898</v>
+        <v>50.3194305896759</v>
       </c>
     </row>
     <row r="19">
@@ -1059,31 +1059,31 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2174</v>
+        <v>2172</v>
       </c>
       <c r="C19" t="n">
         <v>2177</v>
       </c>
       <c r="D19" t="n">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G19" t="n">
-        <v>99.81617647058823</v>
+        <v>99.77022058823529</v>
       </c>
       <c r="H19" t="n">
-        <v>99.95398067188219</v>
+        <v>100</v>
       </c>
       <c r="I19" t="n">
         <v>0.002296738631143776</v>
       </c>
       <c r="J19" t="n">
-        <v>45.50825595855713</v>
+        <v>46.8381724357605</v>
       </c>
     </row>
     <row r="20">
@@ -1117,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>42.40396881103516</v>
+        <v>43.31258606910706</v>
       </c>
     </row>
     <row r="21">
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="C21" t="n">
         <v>1950</v>
@@ -1136,7 +1136,7 @@
         <v>1949</v>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -1145,13 +1145,13 @@
         <v>100</v>
       </c>
       <c r="H21" t="n">
-        <v>99.74411463664278</v>
+        <v>99.89748846745259</v>
       </c>
       <c r="I21" t="n">
-        <v>0.002564102564102564</v>
+        <v>0.001025641025641026</v>
       </c>
       <c r="J21" t="n">
-        <v>41.40494346618652</v>
+        <v>42.10619449615479</v>
       </c>
     </row>
     <row r="22">
@@ -1185,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>49.15558266639709</v>
+        <v>49.9791853427887</v>
       </c>
     </row>
     <row r="23">
@@ -1219,7 +1219,7 @@
         <v>0.001121076233183856</v>
       </c>
       <c r="J23" t="n">
-        <v>43.26976871490479</v>
+        <v>43.81666541099548</v>
       </c>
     </row>
     <row r="24">
@@ -1229,31 +1229,31 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>3245</v>
+        <v>3244</v>
       </c>
       <c r="C24" t="n">
         <v>3245</v>
       </c>
       <c r="D24" t="n">
-        <v>3244</v>
+        <v>3243</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>100</v>
+        <v>99.9691738594328</v>
       </c>
       <c r="H24" t="n">
         <v>100</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>0.0003081664098613251</v>
       </c>
       <c r="J24" t="n">
-        <v>33.49357557296753</v>
+        <v>33.93024754524231</v>
       </c>
     </row>
     <row r="25">
@@ -1287,7 +1287,7 @@
         <v>0.0004302925989672978</v>
       </c>
       <c r="J25" t="n">
-        <v>43.17362904548645</v>
+        <v>43.75181579589844</v>
       </c>
     </row>
     <row r="26">
@@ -1321,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>43.25995492935181</v>
+        <v>43.86422967910767</v>
       </c>
     </row>
     <row r="27">
@@ -1331,7 +1331,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2587</v>
+        <v>2585</v>
       </c>
       <c r="C27" t="n">
         <v>2584</v>
@@ -1340,7 +1340,7 @@
         <v>2583</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1349,13 +1349,13 @@
         <v>100</v>
       </c>
       <c r="H27" t="n">
-        <v>99.88399071925754</v>
+        <v>99.96130030959752</v>
       </c>
       <c r="I27" t="n">
-        <v>0.001160990712074303</v>
+        <v>0.0003869969040247678</v>
       </c>
       <c r="J27" t="n">
-        <v>42.09691071510315</v>
+        <v>42.79960870742798</v>
       </c>
     </row>
     <row r="28">
@@ -1365,31 +1365,31 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2451</v>
+        <v>2442</v>
       </c>
       <c r="C28" t="n">
         <v>2472</v>
       </c>
       <c r="D28" t="n">
-        <v>2448</v>
+        <v>2440</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G28" t="n">
-        <v>99.0692027519223</v>
+        <v>98.74544718737353</v>
       </c>
       <c r="H28" t="n">
-        <v>99.91836734693878</v>
+        <v>99.95903318312168</v>
       </c>
       <c r="I28" t="n">
-        <v>0.01011326860841424</v>
+        <v>0.01294498381877023</v>
       </c>
       <c r="J28" t="n">
-        <v>36.36382722854614</v>
+        <v>37.19225168228149</v>
       </c>
     </row>
     <row r="29">
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>42.59109139442444</v>
+        <v>43.03028607368469</v>
       </c>
     </row>
     <row r="30">
@@ -1433,31 +1433,31 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2368</v>
+        <v>2352</v>
       </c>
       <c r="C30" t="n">
         <v>2376</v>
       </c>
       <c r="D30" t="n">
-        <v>2366</v>
+        <v>2350</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="G30" t="n">
-        <v>99.62105263157895</v>
+        <v>98.94736842105263</v>
       </c>
       <c r="H30" t="n">
-        <v>99.95775242923531</v>
+        <v>99.95746490854955</v>
       </c>
       <c r="I30" t="n">
-        <v>0.004208754208754209</v>
+        <v>0.01094276094276094</v>
       </c>
       <c r="J30" t="n">
-        <v>39.60499286651611</v>
+        <v>39.49511885643005</v>
       </c>
     </row>
     <row r="31">
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>42.3595449924469</v>
+        <v>43.17696166038513</v>
       </c>
     </row>
     <row r="32">
@@ -1525,7 +1525,7 @@
         <v>0.0004428697962798937</v>
       </c>
       <c r="J32" t="n">
-        <v>36.50954580307007</v>
+        <v>37.1533465385437</v>
       </c>
     </row>
     <row r="33">
@@ -1535,31 +1535,31 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="C33" t="n">
         <v>1452</v>
       </c>
       <c r="D33" t="n">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G33" t="n">
-        <v>99.65541006202619</v>
+        <v>99.51757408683666</v>
       </c>
       <c r="H33" t="n">
-        <v>99.31318681318682</v>
+        <v>99.44903581267218</v>
       </c>
       <c r="I33" t="n">
         <v>0.01033057851239669</v>
       </c>
       <c r="J33" t="n">
-        <v>49.96272349357605</v>
+        <v>50.75745844841003</v>
       </c>
     </row>
     <row r="34">
@@ -1569,31 +1569,31 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1941</v>
+        <v>1836</v>
       </c>
       <c r="C34" t="n">
         <v>1947</v>
       </c>
       <c r="D34" t="n">
-        <v>1940</v>
+        <v>1835</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="G34" t="n">
-        <v>99.69167523124358</v>
+        <v>94.29599177800617</v>
       </c>
       <c r="H34" t="n">
         <v>100</v>
       </c>
       <c r="I34" t="n">
-        <v>0.003081664098613251</v>
+        <v>0.05701078582434515</v>
       </c>
       <c r="J34" t="n">
-        <v>40.64520740509033</v>
+        <v>38.49594283103943</v>
       </c>
     </row>
     <row r="35">
@@ -1627,7 +1627,7 @@
         <v>0.0002840909090909091</v>
       </c>
       <c r="J35" t="n">
-        <v>32.74433255195618</v>
+        <v>33.4757707118988</v>
       </c>
     </row>
     <row r="36">
@@ -1637,31 +1637,31 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1886</v>
+        <v>1879</v>
       </c>
       <c r="C36" t="n">
         <v>1878</v>
       </c>
       <c r="D36" t="n">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="E36" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>100</v>
+        <v>99.94672349493874</v>
       </c>
       <c r="H36" t="n">
-        <v>99.57559681697613</v>
+        <v>99.89350372736955</v>
       </c>
       <c r="I36" t="n">
-        <v>0.004259850905218318</v>
+        <v>0.001597444089456869</v>
       </c>
       <c r="J36" t="n">
-        <v>41.56852269172668</v>
+        <v>42.15771770477295</v>
       </c>
     </row>
     <row r="37">
@@ -1671,31 +1671,31 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="C37" t="n">
         <v>2371</v>
       </c>
       <c r="D37" t="n">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G37" t="n">
-        <v>99.87341772151899</v>
+        <v>99.83122362869199</v>
       </c>
       <c r="H37" t="n">
         <v>100</v>
       </c>
       <c r="I37" t="n">
-        <v>0.00126528890763391</v>
+        <v>0.001687051876845213</v>
       </c>
       <c r="J37" t="n">
-        <v>44.75942325592041</v>
+        <v>45.36346316337585</v>
       </c>
     </row>
     <row r="38">
@@ -1705,31 +1705,31 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2907</v>
+        <v>2904</v>
       </c>
       <c r="C38" t="n">
         <v>2907</v>
       </c>
       <c r="D38" t="n">
-        <v>2906</v>
+        <v>2903</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G38" t="n">
-        <v>100</v>
+        <v>99.89676531314522</v>
       </c>
       <c r="H38" t="n">
         <v>100</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>0.001031991744066047</v>
       </c>
       <c r="J38" t="n">
-        <v>33.52435040473938</v>
+        <v>34.13824939727783</v>
       </c>
     </row>
     <row r="39">
@@ -1739,31 +1739,31 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2204</v>
+        <v>2051</v>
       </c>
       <c r="C39" t="n">
         <v>2257</v>
       </c>
       <c r="D39" t="n">
-        <v>2202</v>
+        <v>2049</v>
       </c>
       <c r="E39" t="n">
         <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>54</v>
+        <v>207</v>
       </c>
       <c r="G39" t="n">
-        <v>97.6063829787234</v>
+        <v>90.82446808510639</v>
       </c>
       <c r="H39" t="n">
-        <v>99.95460735360872</v>
+        <v>99.95121951219512</v>
       </c>
       <c r="I39" t="n">
-        <v>0.02436863092600797</v>
+        <v>0.0921577315019938</v>
       </c>
       <c r="J39" t="n">
-        <v>34.6678581237793</v>
+        <v>35.2193329334259</v>
       </c>
     </row>
     <row r="40">
@@ -1773,31 +1773,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="C40" t="n">
         <v>2351</v>
       </c>
       <c r="D40" t="n">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>100</v>
+        <v>99.95744680851064</v>
       </c>
       <c r="H40" t="n">
         <v>100</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>0.0004253509145044662</v>
       </c>
       <c r="J40" t="n">
-        <v>42.31657028198242</v>
+        <v>42.51305055618286</v>
       </c>
     </row>
     <row r="41">
@@ -1831,7 +1831,7 @@
         <v>0.0004212299915754001</v>
       </c>
       <c r="J41" t="n">
-        <v>36.85695815086365</v>
+        <v>37.57765603065491</v>
       </c>
     </row>
     <row r="42">
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>39.94545125961304</v>
+        <v>40.10100150108337</v>
       </c>
     </row>
     <row r="43">
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>43.2958071231842</v>
+        <v>44.17168784141541</v>
       </c>
     </row>
     <row r="44">
@@ -1909,7 +1909,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2078</v>
+        <v>2071</v>
       </c>
       <c r="C44" t="n">
         <v>2068</v>
@@ -1918,7 +1918,7 @@
         <v>2066</v>
       </c>
       <c r="E44" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -1927,13 +1927,13 @@
         <v>99.95162070633769</v>
       </c>
       <c r="H44" t="n">
-        <v>99.4703899855561</v>
+        <v>99.80676328502416</v>
       </c>
       <c r="I44" t="n">
-        <v>0.005802707930367505</v>
+        <v>0.002417794970986461</v>
       </c>
       <c r="J44" t="n">
-        <v>41.93298411369324</v>
+        <v>41.17302274703979</v>
       </c>
     </row>
     <row r="45">
@@ -1943,31 +1943,31 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2922</v>
+        <v>2919</v>
       </c>
       <c r="C45" t="n">
         <v>2923</v>
       </c>
       <c r="D45" t="n">
-        <v>2921</v>
+        <v>2918</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G45" t="n">
-        <v>99.96577686516085</v>
+        <v>99.86310746064339</v>
       </c>
       <c r="H45" t="n">
         <v>100</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0003421142661648991</v>
+        <v>0.001368457064659596</v>
       </c>
       <c r="J45" t="n">
-        <v>37.44164514541626</v>
+        <v>37.91323900222778</v>
       </c>
     </row>
     <row r="46">
@@ -2001,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>44.58977437019348</v>
+        <v>44.67792892456055</v>
       </c>
     </row>
     <row r="47">
@@ -2035,7 +2035,7 @@
         <v>0.0009242144177449168</v>
       </c>
       <c r="J47" t="n">
-        <v>39.75320172309875</v>
+        <v>40.52376008033752</v>
       </c>
     </row>
     <row r="48">
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2155</v>
+        <v>2107</v>
       </c>
       <c r="C48" t="n">
         <v>2017</v>
@@ -2054,7 +2054,7 @@
         <v>2016</v>
       </c>
       <c r="E48" t="n">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -2063,13 +2063,13 @@
         <v>100</v>
       </c>
       <c r="H48" t="n">
-        <v>93.59331476323119</v>
+        <v>95.72649572649573</v>
       </c>
       <c r="I48" t="n">
-        <v>0.06841844323252355</v>
+        <v>0.04462072384729797</v>
       </c>
       <c r="J48" t="n">
-        <v>32.54594302177429</v>
+        <v>32.94357466697693</v>
       </c>
     </row>
     <row r="49">
@@ -2103,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>45.51438045501709</v>
+        <v>46.01026749610901</v>
       </c>
     </row>
     <row r="50">
@@ -2113,31 +2113,31 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1962</v>
+        <v>1953</v>
       </c>
       <c r="C50" t="n">
         <v>1953</v>
       </c>
       <c r="D50" t="n">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="E50" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" t="n">
-        <v>100</v>
+        <v>99.94877049180327</v>
       </c>
       <c r="H50" t="n">
-        <v>99.54105048444671</v>
+        <v>99.94877049180327</v>
       </c>
       <c r="I50" t="n">
-        <v>0.004608294930875576</v>
+        <v>0.001024065540194572</v>
       </c>
       <c r="J50" t="n">
-        <v>46.73506903648376</v>
+        <v>48.62780618667603</v>
       </c>
     </row>
     <row r="51">
@@ -2171,7 +2171,7 @@
         <v>0.0003706449221645663</v>
       </c>
       <c r="J51" t="n">
-        <v>40.9460244178772</v>
+        <v>41.75216603279114</v>
       </c>
     </row>
     <row r="52">
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>43.46905112266541</v>
+        <v>44.24065399169922</v>
       </c>
     </row>
     <row r="53">
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>45.77689003944397</v>
+        <v>46.80379438400269</v>
       </c>
     </row>
     <row r="54">
@@ -2249,31 +2249,31 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="C54" t="n">
         <v>2785</v>
       </c>
       <c r="D54" t="n">
-        <v>2776</v>
+        <v>2775</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G54" t="n">
-        <v>99.71264367816092</v>
+        <v>99.67672413793103</v>
       </c>
       <c r="H54" t="n">
         <v>100</v>
       </c>
       <c r="I54" t="n">
-        <v>0.002872531418312388</v>
+        <v>0.003231597845601436</v>
       </c>
       <c r="J54" t="n">
-        <v>32.6847288608551</v>
+        <v>33.94327449798584</v>
       </c>
     </row>
     <row r="55">
@@ -2307,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>44.11378479003906</v>
+        <v>45.06007599830627</v>
       </c>
     </row>
     <row r="56">
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>35.52968215942383</v>
+        <v>35.96840977668762</v>
       </c>
     </row>
     <row r="57">
@@ -2375,7 +2375,7 @@
         <v>0.0004</v>
       </c>
       <c r="J57" t="n">
-        <v>43.56386017799377</v>
+        <v>44.63901209831238</v>
       </c>
     </row>
     <row r="58">
@@ -2385,31 +2385,31 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>3289</v>
+        <v>3286</v>
       </c>
       <c r="C58" t="n">
         <v>3289</v>
       </c>
       <c r="D58" t="n">
-        <v>3288</v>
+        <v>3285</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G58" t="n">
-        <v>100</v>
+        <v>99.9087591240876</v>
       </c>
       <c r="H58" t="n">
         <v>100</v>
       </c>
       <c r="I58" t="n">
-        <v>0</v>
+        <v>0.0009121313469139556</v>
       </c>
       <c r="J58" t="n">
-        <v>35.19466376304626</v>
+        <v>35.60381054878235</v>
       </c>
     </row>
     <row r="59">
@@ -2443,7 +2443,7 @@
         <v>0.002212389380530973</v>
       </c>
       <c r="J59" t="n">
-        <v>34.22929835319519</v>
+        <v>34.63271307945251</v>
       </c>
     </row>
     <row r="60">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>47.20427298545837</v>
+        <v>47.97205924987793</v>
       </c>
     </row>
     <row r="61">
@@ -2487,7 +2487,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="C61" t="n">
         <v>2533</v>
@@ -2496,7 +2496,7 @@
         <v>2532</v>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="n">
         <v>0</v>
@@ -2505,13 +2505,13 @@
         <v>100</v>
       </c>
       <c r="H61" t="n">
-        <v>99.92107340173638</v>
+        <v>99.96052112120016</v>
       </c>
       <c r="I61" t="n">
-        <v>0.0007895775759968417</v>
+        <v>0.0003947887879984208</v>
       </c>
       <c r="J61" t="n">
-        <v>34.87859582901001</v>
+        <v>35.96317076683044</v>
       </c>
     </row>
     <row r="62">
@@ -2545,7 +2545,7 @@
         <v>0.002075765438505449</v>
       </c>
       <c r="J62" t="n">
-        <v>36.22535061836243</v>
+        <v>36.79509472846985</v>
       </c>
     </row>
     <row r="63">
@@ -2555,7 +2555,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2442</v>
+        <v>2435</v>
       </c>
       <c r="C63" t="n">
         <v>2437</v>
@@ -2564,7 +2564,7 @@
         <v>2431</v>
       </c>
       <c r="E63" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F63" t="n">
         <v>5</v>
@@ -2573,13 +2573,13 @@
         <v>99.79474548440065</v>
       </c>
       <c r="H63" t="n">
-        <v>99.59033183121672</v>
+        <v>99.87674609695974</v>
       </c>
       <c r="I63" t="n">
-        <v>0.006155108740254411</v>
+        <v>0.003282724661469019</v>
       </c>
       <c r="J63" t="n">
-        <v>42.51649332046509</v>
+        <v>40.34293580055237</v>
       </c>
     </row>
     <row r="64">
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>41.51781320571899</v>
+        <v>42.47611975669861</v>
       </c>
     </row>
     <row r="65">
@@ -2623,7 +2623,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2345</v>
+        <v>2342</v>
       </c>
       <c r="C65" t="n">
         <v>2340</v>
@@ -2632,7 +2632,7 @@
         <v>2338</v>
       </c>
       <c r="E65" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
         <v>1</v>
@@ -2641,13 +2641,13 @@
         <v>99.95724668661822</v>
       </c>
       <c r="H65" t="n">
-        <v>99.74402730375427</v>
+        <v>99.8718496369073</v>
       </c>
       <c r="I65" t="n">
-        <v>0.002991452991452992</v>
+        <v>0.001709401709401709</v>
       </c>
       <c r="J65" t="n">
-        <v>38.65426015853882</v>
+        <v>38.54847145080566</v>
       </c>
     </row>
     <row r="66">
@@ -2681,7 +2681,7 @@
         <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>41.5362913608551</v>
+        <v>42.24662804603577</v>
       </c>
     </row>
     <row r="67">
@@ -2715,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="J67" t="n">
-        <v>42.67780494689941</v>
+        <v>43.17126870155334</v>
       </c>
     </row>
     <row r="68">
@@ -2749,7 +2749,7 @@
         <v>0.001711351968054763</v>
       </c>
       <c r="J68" t="n">
-        <v>44.7093551158905</v>
+        <v>45.12745213508606</v>
       </c>
     </row>
     <row r="69">
@@ -2783,7 +2783,7 @@
         <v>0.002741603838245374</v>
       </c>
       <c r="J69" t="n">
-        <v>47.57292461395264</v>
+        <v>47.94099235534668</v>
       </c>
     </row>
     <row r="70">
@@ -2793,31 +2793,31 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1771</v>
+        <v>1767</v>
       </c>
       <c r="C70" t="n">
         <v>1787</v>
       </c>
       <c r="D70" t="n">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G70" t="n">
-        <v>98.76888640179071</v>
+        <v>98.60100727476217</v>
       </c>
       <c r="H70" t="n">
-        <v>99.71751412429379</v>
+        <v>99.77349943374858</v>
       </c>
       <c r="I70" t="n">
-        <v>0.01510912143256855</v>
+        <v>0.01622831561275881</v>
       </c>
       <c r="J70" t="n">
-        <v>35.72090625762939</v>
+        <v>36.04430747032166</v>
       </c>
     </row>
     <row r="71">
@@ -2851,7 +2851,7 @@
         <v>0.01021059349074665</v>
       </c>
       <c r="J71" t="n">
-        <v>36.45135927200317</v>
+        <v>37.35191130638123</v>
       </c>
     </row>
     <row r="72">
@@ -2861,31 +2861,31 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C72" t="n">
         <v>920</v>
       </c>
       <c r="D72" t="n">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E72" t="n">
         <v>1</v>
       </c>
       <c r="F72" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G72" t="n">
-        <v>99.56474428726877</v>
+        <v>99.34711643090316</v>
       </c>
       <c r="H72" t="n">
-        <v>99.89082969432314</v>
+        <v>99.89059080962801</v>
       </c>
       <c r="I72" t="n">
-        <v>0.005434782608695652</v>
+        <v>0.007608695652173913</v>
       </c>
       <c r="J72" t="n">
-        <v>44.91983652114868</v>
+        <v>45.81126403808594</v>
       </c>
     </row>
     <row r="73">
@@ -2895,31 +2895,31 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1171</v>
+        <v>1165</v>
       </c>
       <c r="C73" t="n">
         <v>1143</v>
       </c>
       <c r="D73" t="n">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="E73" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F73" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G73" t="n">
-        <v>98.59894921190893</v>
+        <v>98.33625218914186</v>
       </c>
       <c r="H73" t="n">
-        <v>96.23931623931624</v>
+        <v>96.47766323024055</v>
       </c>
       <c r="I73" t="n">
         <v>0.05249343832020997</v>
       </c>
       <c r="J73" t="n">
-        <v>39.71299982070923</v>
+        <v>40.22099614143372</v>
       </c>
     </row>
     <row r="74">
@@ -2929,31 +2929,31 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1342</v>
+        <v>1250</v>
       </c>
       <c r="C74" t="n">
         <v>1356</v>
       </c>
       <c r="D74" t="n">
-        <v>1325</v>
+        <v>1247</v>
       </c>
       <c r="E74" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="G74" t="n">
-        <v>97.7859778597786</v>
+        <v>92.02952029520296</v>
       </c>
       <c r="H74" t="n">
-        <v>98.806860551827</v>
+        <v>99.83987189751801</v>
       </c>
       <c r="I74" t="n">
-        <v>0.03392330383480826</v>
+        <v>0.08112094395280237</v>
       </c>
       <c r="J74" t="n">
-        <v>41.83043575286865</v>
+        <v>42.86761617660522</v>
       </c>
     </row>
     <row r="75">
@@ -2963,31 +2963,31 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C75" t="n">
         <v>543</v>
       </c>
       <c r="D75" t="n">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G75" t="n">
-        <v>99.07749077490774</v>
+        <v>98.70848708487085</v>
       </c>
       <c r="H75" t="n">
         <v>100</v>
       </c>
       <c r="I75" t="n">
-        <v>0.009208103130755065</v>
+        <v>0.01289134438305709</v>
       </c>
       <c r="J75" t="n">
-        <v>45.27727079391479</v>
+        <v>46.21938848495483</v>
       </c>
     </row>
     <row r="76">
@@ -2997,31 +2997,31 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="C76" t="n">
         <v>2025</v>
       </c>
       <c r="D76" t="n">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G76" t="n">
-        <v>97.4802371541502</v>
+        <v>97.38142292490119</v>
       </c>
       <c r="H76" t="n">
         <v>100</v>
       </c>
       <c r="I76" t="n">
-        <v>0.02518518518518519</v>
+        <v>0.02617283950617284</v>
       </c>
       <c r="J76" t="n">
-        <v>38.05605459213257</v>
+        <v>38.40941786766052</v>
       </c>
     </row>
     <row r="77">
@@ -3055,7 +3055,7 @@
         <v>0.0004662004662004662</v>
       </c>
       <c r="J77" t="n">
-        <v>41.29235649108887</v>
+        <v>41.5780668258667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding low pass filter to MIT and changing cutoff frequency of low pass to 37.5Hz to suit 113
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/AHA_database.xlsx
+++ b/R peak detection/beatdetection/AHA_database.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="gscgwuc" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="gcgdcd" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,31 +447,31 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1643</v>
+        <v>1649</v>
       </c>
       <c r="C1" t="n">
         <v>1622</v>
       </c>
       <c r="D1" t="n">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="E1" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" t="n">
-        <v>100</v>
+        <v>99.93830968537939</v>
       </c>
       <c r="H1" t="n">
-        <v>98.721071863581</v>
+        <v>98.30097087378641</v>
       </c>
       <c r="I1" t="n">
-        <v>0.01294697903822441</v>
+        <v>0.01787916152897657</v>
       </c>
       <c r="J1" t="n">
-        <v>52.9605758190155</v>
+        <v>51.80201888084412</v>
       </c>
     </row>
     <row r="2">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2595</v>
+        <v>2596</v>
       </c>
       <c r="C2" t="n">
         <v>2595</v>
@@ -490,7 +490,7 @@
         <v>2594</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -499,13 +499,13 @@
         <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>99.96146435452793</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.0003853564547206166</v>
       </c>
       <c r="J2" t="n">
-        <v>36.99648785591125</v>
+        <v>36.14297819137573</v>
       </c>
     </row>
     <row r="3">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2182</v>
+        <v>2184</v>
       </c>
       <c r="C3" t="n">
         <v>2181</v>
@@ -524,7 +524,7 @@
         <v>2180</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -533,13 +533,13 @@
         <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>99.95414947271894</v>
+        <v>99.86257443884563</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0004585052728106373</v>
+        <v>0.001375515818431912</v>
       </c>
       <c r="J3" t="n">
-        <v>44.56078028678894</v>
+        <v>43.53279399871826</v>
       </c>
     </row>
     <row r="4">
@@ -549,31 +549,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2939</v>
+        <v>2942</v>
       </c>
       <c r="C4" t="n">
         <v>2974</v>
       </c>
       <c r="D4" t="n">
-        <v>2936</v>
+        <v>2940</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G4" t="n">
-        <v>98.75546585940128</v>
+        <v>98.89001009081736</v>
       </c>
       <c r="H4" t="n">
-        <v>99.93192648059905</v>
+        <v>99.9659979598776</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01311365164761264</v>
+        <v>0.01143241425689307</v>
       </c>
       <c r="J4" t="n">
-        <v>38.42226243019104</v>
+        <v>37.08592486381531</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>44.00360679626465</v>
+        <v>42.92649984359741</v>
       </c>
     </row>
     <row r="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2122</v>
+        <v>2123</v>
       </c>
       <c r="C6" t="n">
         <v>2122</v>
@@ -626,7 +626,7 @@
         <v>2121</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -635,13 +635,13 @@
         <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>100</v>
+        <v>99.95287464655985</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>0.000471253534401508</v>
       </c>
       <c r="J6" t="n">
-        <v>42.20387578010559</v>
+        <v>40.64820408821106</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>42.274169921875</v>
+        <v>41.25562477111816</v>
       </c>
     </row>
     <row r="8">
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>40.643310546875</v>
+        <v>38.93723320960999</v>
       </c>
     </row>
     <row r="9">
@@ -719,7 +719,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3583</v>
+        <v>3584</v>
       </c>
       <c r="C9" t="n">
         <v>3582</v>
@@ -728,7 +728,7 @@
         <v>3581</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -737,13 +737,13 @@
         <v>100</v>
       </c>
       <c r="H9" t="n">
-        <v>99.97208263539922</v>
+        <v>99.94418085403294</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0002791736460078169</v>
+        <v>0.0005583472920156337</v>
       </c>
       <c r="J9" t="n">
-        <v>31.53788757324219</v>
+        <v>29.80377221107483</v>
       </c>
     </row>
     <row r="10">
@@ -753,7 +753,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2045</v>
+        <v>2093</v>
       </c>
       <c r="C10" t="n">
         <v>1997</v>
@@ -762,7 +762,7 @@
         <v>1991</v>
       </c>
       <c r="E10" t="n">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="F10" t="n">
         <v>5</v>
@@ -771,13 +771,13 @@
         <v>99.74949899799599</v>
       </c>
       <c r="H10" t="n">
-        <v>97.40704500978474</v>
+        <v>95.17208413001912</v>
       </c>
       <c r="I10" t="n">
-        <v>0.02904356534802203</v>
+        <v>0.05307961942914372</v>
       </c>
       <c r="J10" t="n">
-        <v>48.92391967773438</v>
+        <v>48.99442291259766</v>
       </c>
     </row>
     <row r="11">
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>32.3477954864502</v>
+        <v>31.32786560058594</v>
       </c>
     </row>
     <row r="12">
@@ -845,7 +845,7 @@
         <v>0.0004142502071251035</v>
       </c>
       <c r="J12" t="n">
-        <v>42.63553929328918</v>
+        <v>41.34808969497681</v>
       </c>
     </row>
     <row r="13">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1638</v>
+        <v>1644</v>
       </c>
       <c r="C13" t="n">
         <v>1628</v>
@@ -864,7 +864,7 @@
         <v>1627</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -873,13 +873,13 @@
         <v>100</v>
       </c>
       <c r="H13" t="n">
-        <v>99.38912645082468</v>
+        <v>99.02617163724894</v>
       </c>
       <c r="I13" t="n">
-        <v>0.006142506142506142</v>
+        <v>0.009828009828009828</v>
       </c>
       <c r="J13" t="n">
-        <v>40.82839941978455</v>
+        <v>38.94654536247253</v>
       </c>
     </row>
     <row r="14">
@@ -913,7 +913,7 @@
         <v>0.0006199628022318661</v>
       </c>
       <c r="J14" t="n">
-        <v>49.46972990036011</v>
+        <v>46.78748941421509</v>
       </c>
     </row>
     <row r="15">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>35.96109127998352</v>
+        <v>34.60554480552673</v>
       </c>
     </row>
     <row r="16">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>38.06334471702576</v>
+        <v>34.0259096622467</v>
       </c>
     </row>
     <row r="17">
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>40.34566068649292</v>
+        <v>38.52973246574402</v>
       </c>
     </row>
     <row r="18">
@@ -1025,31 +1025,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2536</v>
+        <v>2545</v>
       </c>
       <c r="C18" t="n">
         <v>2537</v>
       </c>
       <c r="D18" t="n">
-        <v>2533</v>
+        <v>2534</v>
       </c>
       <c r="E18" t="n">
+        <v>10</v>
+      </c>
+      <c r="F18" t="n">
         <v>2</v>
       </c>
-      <c r="F18" t="n">
-        <v>3</v>
-      </c>
       <c r="G18" t="n">
-        <v>99.88170347003154</v>
+        <v>99.9211356466877</v>
       </c>
       <c r="H18" t="n">
-        <v>99.92110453648915</v>
+        <v>99.60691823899371</v>
       </c>
       <c r="I18" t="n">
-        <v>0.001970831690973591</v>
+        <v>0.004729996058336618</v>
       </c>
       <c r="J18" t="n">
-        <v>50.3194305896759</v>
+        <v>48.39543032646179</v>
       </c>
     </row>
     <row r="19">
@@ -1059,31 +1059,31 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2172</v>
+        <v>2174</v>
       </c>
       <c r="C19" t="n">
         <v>2177</v>
       </c>
       <c r="D19" t="n">
-        <v>2171</v>
+        <v>2172</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G19" t="n">
-        <v>99.77022058823529</v>
+        <v>99.81617647058823</v>
       </c>
       <c r="H19" t="n">
-        <v>100</v>
+        <v>99.95398067188219</v>
       </c>
       <c r="I19" t="n">
         <v>0.002296738631143776</v>
       </c>
       <c r="J19" t="n">
-        <v>46.8381724357605</v>
+        <v>45.08687710762024</v>
       </c>
     </row>
     <row r="20">
@@ -1117,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>43.31258606910706</v>
+        <v>41.07108497619629</v>
       </c>
     </row>
     <row r="21">
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1952</v>
+        <v>1956</v>
       </c>
       <c r="C21" t="n">
         <v>1950</v>
@@ -1136,7 +1136,7 @@
         <v>1949</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -1145,13 +1145,13 @@
         <v>100</v>
       </c>
       <c r="H21" t="n">
-        <v>99.89748846745259</v>
+        <v>99.69309462915601</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001025641025641026</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="J21" t="n">
-        <v>42.10619449615479</v>
+        <v>40.2023823261261</v>
       </c>
     </row>
     <row r="22">
@@ -1185,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>49.9791853427887</v>
+        <v>47.81577086448669</v>
       </c>
     </row>
     <row r="23">
@@ -1195,7 +1195,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1782</v>
+        <v>1784</v>
       </c>
       <c r="C23" t="n">
         <v>1784</v>
@@ -1204,7 +1204,7 @@
         <v>1781</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>2</v>
@@ -1213,13 +1213,13 @@
         <v>99.88782950084128</v>
       </c>
       <c r="H23" t="n">
-        <v>100</v>
+        <v>99.88782950084128</v>
       </c>
       <c r="I23" t="n">
-        <v>0.001121076233183856</v>
+        <v>0.002242152466367713</v>
       </c>
       <c r="J23" t="n">
-        <v>43.81666541099548</v>
+        <v>41.88349318504333</v>
       </c>
     </row>
     <row r="24">
@@ -1229,31 +1229,31 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>3244</v>
+        <v>3245</v>
       </c>
       <c r="C24" t="n">
         <v>3245</v>
       </c>
       <c r="D24" t="n">
-        <v>3243</v>
+        <v>3244</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>99.9691738594328</v>
+        <v>100</v>
       </c>
       <c r="H24" t="n">
         <v>100</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0003081664098613251</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>33.93024754524231</v>
+        <v>32.68469858169556</v>
       </c>
     </row>
     <row r="25">
@@ -1287,7 +1287,7 @@
         <v>0.0004302925989672978</v>
       </c>
       <c r="J25" t="n">
-        <v>43.75181579589844</v>
+        <v>42.26104235649109</v>
       </c>
     </row>
     <row r="26">
@@ -1321,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>43.86422967910767</v>
+        <v>41.69298315048218</v>
       </c>
     </row>
     <row r="27">
@@ -1331,7 +1331,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2585</v>
+        <v>2587</v>
       </c>
       <c r="C27" t="n">
         <v>2584</v>
@@ -1340,7 +1340,7 @@
         <v>2583</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1349,13 +1349,13 @@
         <v>100</v>
       </c>
       <c r="H27" t="n">
-        <v>99.96130030959752</v>
+        <v>99.88399071925754</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0003869969040247678</v>
+        <v>0.001160990712074303</v>
       </c>
       <c r="J27" t="n">
-        <v>42.79960870742798</v>
+        <v>40.94000577926636</v>
       </c>
     </row>
     <row r="28">
@@ -1365,31 +1365,31 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2442</v>
+        <v>2449</v>
       </c>
       <c r="C28" t="n">
         <v>2472</v>
       </c>
       <c r="D28" t="n">
-        <v>2440</v>
+        <v>2447</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G28" t="n">
-        <v>98.74544718737353</v>
+        <v>99.0287333063537</v>
       </c>
       <c r="H28" t="n">
-        <v>99.95903318312168</v>
+        <v>99.95915032679738</v>
       </c>
       <c r="I28" t="n">
-        <v>0.01294498381877023</v>
+        <v>0.01011326860841424</v>
       </c>
       <c r="J28" t="n">
-        <v>37.19225168228149</v>
+        <v>35.63106942176819</v>
       </c>
     </row>
     <row r="29">
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>43.03028607368469</v>
+        <v>41.40298676490784</v>
       </c>
     </row>
     <row r="30">
@@ -1433,31 +1433,31 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2352</v>
+        <v>2368</v>
       </c>
       <c r="C30" t="n">
         <v>2376</v>
       </c>
       <c r="D30" t="n">
-        <v>2350</v>
+        <v>2366</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G30" t="n">
-        <v>98.94736842105263</v>
+        <v>99.62105263157895</v>
       </c>
       <c r="H30" t="n">
-        <v>99.95746490854955</v>
+        <v>99.95775242923531</v>
       </c>
       <c r="I30" t="n">
-        <v>0.01094276094276094</v>
+        <v>0.004208754208754209</v>
       </c>
       <c r="J30" t="n">
-        <v>39.49511885643005</v>
+        <v>38.32140374183655</v>
       </c>
     </row>
     <row r="31">
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>43.17696166038513</v>
+        <v>41.7340190410614</v>
       </c>
     </row>
     <row r="32">
@@ -1525,7 +1525,7 @@
         <v>0.0004428697962798937</v>
       </c>
       <c r="J32" t="n">
-        <v>37.1533465385437</v>
+        <v>35.86098217964172</v>
       </c>
     </row>
     <row r="33">
@@ -1535,31 +1535,31 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="C33" t="n">
         <v>1452</v>
       </c>
       <c r="D33" t="n">
-        <v>1444</v>
+        <v>1441</v>
       </c>
       <c r="E33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G33" t="n">
-        <v>99.51757408683666</v>
+        <v>99.31082012405238</v>
       </c>
       <c r="H33" t="n">
-        <v>99.44903581267218</v>
+        <v>99.51657458563535</v>
       </c>
       <c r="I33" t="n">
-        <v>0.01033057851239669</v>
+        <v>0.01170798898071625</v>
       </c>
       <c r="J33" t="n">
-        <v>50.75745844841003</v>
+        <v>48.61842823028564</v>
       </c>
     </row>
     <row r="34">
@@ -1569,31 +1569,31 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1836</v>
+        <v>1942</v>
       </c>
       <c r="C34" t="n">
         <v>1947</v>
       </c>
       <c r="D34" t="n">
-        <v>1835</v>
+        <v>1940</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="G34" t="n">
-        <v>94.29599177800617</v>
+        <v>99.69167523124358</v>
       </c>
       <c r="H34" t="n">
-        <v>100</v>
+        <v>99.94848016486347</v>
       </c>
       <c r="I34" t="n">
-        <v>0.05701078582434515</v>
+        <v>0.00359527478171546</v>
       </c>
       <c r="J34" t="n">
-        <v>38.49594283103943</v>
+        <v>37.76836824417114</v>
       </c>
     </row>
     <row r="35">
@@ -1603,7 +1603,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3521</v>
+        <v>3520</v>
       </c>
       <c r="C35" t="n">
         <v>3520</v>
@@ -1612,7 +1612,7 @@
         <v>3519</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1621,13 +1621,13 @@
         <v>100</v>
       </c>
       <c r="H35" t="n">
-        <v>99.97159090909091</v>
+        <v>100</v>
       </c>
       <c r="I35" t="n">
-        <v>0.0002840909090909091</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>33.4757707118988</v>
+        <v>31.67954182624817</v>
       </c>
     </row>
     <row r="36">
@@ -1637,31 +1637,31 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1879</v>
+        <v>1885</v>
       </c>
       <c r="C36" t="n">
         <v>1878</v>
       </c>
       <c r="D36" t="n">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>99.94672349493874</v>
+        <v>100</v>
       </c>
       <c r="H36" t="n">
-        <v>99.89350372736955</v>
+        <v>99.62845010615712</v>
       </c>
       <c r="I36" t="n">
-        <v>0.001597444089456869</v>
+        <v>0.003727369542066028</v>
       </c>
       <c r="J36" t="n">
-        <v>42.15771770477295</v>
+        <v>40.97533845901489</v>
       </c>
     </row>
     <row r="37">
@@ -1671,31 +1671,31 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2367</v>
+        <v>2368</v>
       </c>
       <c r="C37" t="n">
         <v>2371</v>
       </c>
       <c r="D37" t="n">
-        <v>2366</v>
+        <v>2367</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G37" t="n">
-        <v>99.83122362869199</v>
+        <v>99.87341772151899</v>
       </c>
       <c r="H37" t="n">
         <v>100</v>
       </c>
       <c r="I37" t="n">
-        <v>0.001687051876845213</v>
+        <v>0.00126528890763391</v>
       </c>
       <c r="J37" t="n">
-        <v>45.36346316337585</v>
+        <v>43.59290957450867</v>
       </c>
     </row>
     <row r="38">
@@ -1705,31 +1705,31 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2904</v>
+        <v>2907</v>
       </c>
       <c r="C38" t="n">
         <v>2907</v>
       </c>
       <c r="D38" t="n">
-        <v>2903</v>
+        <v>2906</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>99.89676531314522</v>
+        <v>100</v>
       </c>
       <c r="H38" t="n">
         <v>100</v>
       </c>
       <c r="I38" t="n">
-        <v>0.001031991744066047</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>34.13824939727783</v>
+        <v>32.67426729202271</v>
       </c>
     </row>
     <row r="39">
@@ -1739,31 +1739,31 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2051</v>
+        <v>2116</v>
       </c>
       <c r="C39" t="n">
         <v>2257</v>
       </c>
       <c r="D39" t="n">
-        <v>2049</v>
+        <v>2115</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>207</v>
+        <v>141</v>
       </c>
       <c r="G39" t="n">
-        <v>90.82446808510639</v>
+        <v>93.75</v>
       </c>
       <c r="H39" t="n">
-        <v>99.95121951219512</v>
+        <v>100</v>
       </c>
       <c r="I39" t="n">
-        <v>0.0921577315019938</v>
+        <v>0.06247230837394772</v>
       </c>
       <c r="J39" t="n">
-        <v>35.2193329334259</v>
+        <v>33.7508430480957</v>
       </c>
     </row>
     <row r="40">
@@ -1773,31 +1773,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2350</v>
+        <v>2351</v>
       </c>
       <c r="C40" t="n">
         <v>2351</v>
       </c>
       <c r="D40" t="n">
-        <v>2349</v>
+        <v>2350</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>99.95744680851064</v>
+        <v>100</v>
       </c>
       <c r="H40" t="n">
         <v>100</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0004253509145044662</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>42.51305055618286</v>
+        <v>42.74280428886414</v>
       </c>
     </row>
     <row r="41">
@@ -1831,7 +1831,7 @@
         <v>0.0004212299915754001</v>
       </c>
       <c r="J41" t="n">
-        <v>37.57765603065491</v>
+        <v>36.05034017562866</v>
       </c>
     </row>
     <row r="42">
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>40.10100150108337</v>
+        <v>38.995760679245</v>
       </c>
     </row>
     <row r="43">
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>44.17168784141541</v>
+        <v>42.68702483177185</v>
       </c>
     </row>
     <row r="44">
@@ -1909,7 +1909,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2071</v>
+        <v>2080</v>
       </c>
       <c r="C44" t="n">
         <v>2068</v>
@@ -1918,7 +1918,7 @@
         <v>2066</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -1927,13 +1927,13 @@
         <v>99.95162070633769</v>
       </c>
       <c r="H44" t="n">
-        <v>99.80676328502416</v>
+        <v>99.37469937469938</v>
       </c>
       <c r="I44" t="n">
-        <v>0.002417794970986461</v>
+        <v>0.006769825918762089</v>
       </c>
       <c r="J44" t="n">
-        <v>41.17302274703979</v>
+        <v>41.12486505508423</v>
       </c>
     </row>
     <row r="45">
@@ -1943,31 +1943,31 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>2919</v>
+        <v>2922</v>
       </c>
       <c r="C45" t="n">
         <v>2923</v>
       </c>
       <c r="D45" t="n">
-        <v>2918</v>
+        <v>2921</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G45" t="n">
-        <v>99.86310746064339</v>
+        <v>99.96577686516085</v>
       </c>
       <c r="H45" t="n">
         <v>100</v>
       </c>
       <c r="I45" t="n">
-        <v>0.001368457064659596</v>
+        <v>0.0003421142661648991</v>
       </c>
       <c r="J45" t="n">
-        <v>37.91323900222778</v>
+        <v>36.41609668731689</v>
       </c>
     </row>
     <row r="46">
@@ -2001,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>44.67792892456055</v>
+        <v>43.96787643432617</v>
       </c>
     </row>
     <row r="47">
@@ -2035,7 +2035,7 @@
         <v>0.0009242144177449168</v>
       </c>
       <c r="J47" t="n">
-        <v>40.52376008033752</v>
+        <v>39.30252909660339</v>
       </c>
     </row>
     <row r="48">
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2107</v>
+        <v>2170</v>
       </c>
       <c r="C48" t="n">
         <v>2017</v>
@@ -2054,7 +2054,7 @@
         <v>2016</v>
       </c>
       <c r="E48" t="n">
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -2063,13 +2063,13 @@
         <v>100</v>
       </c>
       <c r="H48" t="n">
-        <v>95.72649572649573</v>
+        <v>92.9460580912863</v>
       </c>
       <c r="I48" t="n">
-        <v>0.04462072384729797</v>
+        <v>0.07585523054040655</v>
       </c>
       <c r="J48" t="n">
-        <v>32.94357466697693</v>
+        <v>31.46282005310059</v>
       </c>
     </row>
     <row r="49">
@@ -2103,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>46.01026749610901</v>
+        <v>44.69621133804321</v>
       </c>
     </row>
     <row r="50">
@@ -2113,31 +2113,31 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1953</v>
+        <v>1959</v>
       </c>
       <c r="C50" t="n">
         <v>1953</v>
       </c>
       <c r="D50" t="n">
-        <v>1951</v>
+        <v>1952</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>99.94877049180327</v>
+        <v>100</v>
       </c>
       <c r="H50" t="n">
-        <v>99.94877049180327</v>
+        <v>99.69356486210418</v>
       </c>
       <c r="I50" t="n">
-        <v>0.001024065540194572</v>
+        <v>0.003072196620583717</v>
       </c>
       <c r="J50" t="n">
-        <v>48.62780618667603</v>
+        <v>45.97582197189331</v>
       </c>
     </row>
     <row r="51">
@@ -2171,7 +2171,7 @@
         <v>0.0003706449221645663</v>
       </c>
       <c r="J51" t="n">
-        <v>41.75216603279114</v>
+        <v>39.76867842674255</v>
       </c>
     </row>
     <row r="52">
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>44.24065399169922</v>
+        <v>42.46607255935669</v>
       </c>
     </row>
     <row r="53">
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>46.80379438400269</v>
+        <v>45.16241669654846</v>
       </c>
     </row>
     <row r="54">
@@ -2249,31 +2249,31 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2776</v>
+        <v>2778</v>
       </c>
       <c r="C54" t="n">
         <v>2785</v>
       </c>
       <c r="D54" t="n">
-        <v>2775</v>
+        <v>2777</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G54" t="n">
-        <v>99.67672413793103</v>
+        <v>99.7485632183908</v>
       </c>
       <c r="H54" t="n">
         <v>100</v>
       </c>
       <c r="I54" t="n">
-        <v>0.003231597845601436</v>
+        <v>0.002513464991023339</v>
       </c>
       <c r="J54" t="n">
-        <v>33.94327449798584</v>
+        <v>32.17860245704651</v>
       </c>
     </row>
     <row r="55">
@@ -2307,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>45.06007599830627</v>
+        <v>43.16459894180298</v>
       </c>
     </row>
     <row r="56">
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>35.96840977668762</v>
+        <v>34.59283804893494</v>
       </c>
     </row>
     <row r="57">
@@ -2375,7 +2375,7 @@
         <v>0.0004</v>
       </c>
       <c r="J57" t="n">
-        <v>44.63901209831238</v>
+        <v>42.58084058761597</v>
       </c>
     </row>
     <row r="58">
@@ -2385,31 +2385,31 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>3286</v>
+        <v>3289</v>
       </c>
       <c r="C58" t="n">
         <v>3289</v>
       </c>
       <c r="D58" t="n">
-        <v>3285</v>
+        <v>3288</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>99.9087591240876</v>
+        <v>100</v>
       </c>
       <c r="H58" t="n">
         <v>100</v>
       </c>
       <c r="I58" t="n">
-        <v>0.0009121313469139556</v>
+        <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>35.60381054878235</v>
+        <v>34.45736837387085</v>
       </c>
     </row>
     <row r="59">
@@ -2419,31 +2419,31 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>3157</v>
+        <v>3156</v>
       </c>
       <c r="C59" t="n">
         <v>3164</v>
       </c>
       <c r="D59" t="n">
-        <v>3156</v>
+        <v>3155</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G59" t="n">
-        <v>99.77869111602908</v>
+        <v>99.7470755611761</v>
       </c>
       <c r="H59" t="n">
         <v>100</v>
       </c>
       <c r="I59" t="n">
-        <v>0.002212389380530973</v>
+        <v>0.002528445006321113</v>
       </c>
       <c r="J59" t="n">
-        <v>34.63271307945251</v>
+        <v>33.02324151992798</v>
       </c>
     </row>
     <row r="60">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>47.97205924987793</v>
+        <v>45.9486289024353</v>
       </c>
     </row>
     <row r="61">
@@ -2487,7 +2487,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2534</v>
+        <v>2535</v>
       </c>
       <c r="C61" t="n">
         <v>2533</v>
@@ -2496,7 +2496,7 @@
         <v>2532</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
         <v>0</v>
@@ -2505,13 +2505,13 @@
         <v>100</v>
       </c>
       <c r="H61" t="n">
-        <v>99.96052112120016</v>
+        <v>99.92107340173638</v>
       </c>
       <c r="I61" t="n">
-        <v>0.0003947887879984208</v>
+        <v>0.0007895775759968417</v>
       </c>
       <c r="J61" t="n">
-        <v>35.96317076683044</v>
+        <v>33.84360384941101</v>
       </c>
     </row>
     <row r="62">
@@ -2545,7 +2545,7 @@
         <v>0.002075765438505449</v>
       </c>
       <c r="J62" t="n">
-        <v>36.79509472846985</v>
+        <v>35.12916111946106</v>
       </c>
     </row>
     <row r="63">
@@ -2555,31 +2555,31 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2435</v>
+        <v>2450</v>
       </c>
       <c r="C63" t="n">
         <v>2437</v>
       </c>
       <c r="D63" t="n">
-        <v>2431</v>
+        <v>2432</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G63" t="n">
-        <v>99.79474548440065</v>
+        <v>99.83579638752053</v>
       </c>
       <c r="H63" t="n">
-        <v>99.87674609695974</v>
+        <v>99.30583911800736</v>
       </c>
       <c r="I63" t="n">
-        <v>0.003282724661469019</v>
+        <v>0.008617152236356175</v>
       </c>
       <c r="J63" t="n">
-        <v>40.34293580055237</v>
+        <v>40.15875959396362</v>
       </c>
     </row>
     <row r="64">
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>42.47611975669861</v>
+        <v>40.16179823875427</v>
       </c>
     </row>
     <row r="65">
@@ -2623,7 +2623,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2342</v>
+        <v>2347</v>
       </c>
       <c r="C65" t="n">
         <v>2340</v>
@@ -2632,7 +2632,7 @@
         <v>2338</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
         <v>1</v>
@@ -2641,13 +2641,13 @@
         <v>99.95724668661822</v>
       </c>
       <c r="H65" t="n">
-        <v>99.8718496369073</v>
+        <v>99.65899403239557</v>
       </c>
       <c r="I65" t="n">
-        <v>0.001709401709401709</v>
+        <v>0.003846153846153846</v>
       </c>
       <c r="J65" t="n">
-        <v>38.54847145080566</v>
+        <v>37.89919781684875</v>
       </c>
     </row>
     <row r="66">
@@ -2681,7 +2681,7 @@
         <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>42.24662804603577</v>
+        <v>40.45603013038635</v>
       </c>
     </row>
     <row r="67">
@@ -2715,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="J67" t="n">
-        <v>43.17126870155334</v>
+        <v>41.56116914749146</v>
       </c>
     </row>
     <row r="68">
@@ -2725,31 +2725,31 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="C68" t="n">
         <v>1753</v>
       </c>
       <c r="D68" t="n">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="E68" t="n">
         <v>2</v>
       </c>
       <c r="F68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>99.94292237442923</v>
+        <v>100</v>
       </c>
       <c r="H68" t="n">
-        <v>99.88590986879635</v>
+        <v>99.88597491448118</v>
       </c>
       <c r="I68" t="n">
-        <v>0.001711351968054763</v>
+        <v>0.001140901312036509</v>
       </c>
       <c r="J68" t="n">
-        <v>45.12745213508606</v>
+        <v>43.40285158157349</v>
       </c>
     </row>
     <row r="69">
@@ -2783,7 +2783,7 @@
         <v>0.002741603838245374</v>
       </c>
       <c r="J69" t="n">
-        <v>47.94099235534668</v>
+        <v>46.06160736083984</v>
       </c>
     </row>
     <row r="70">
@@ -2793,31 +2793,31 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1767</v>
+        <v>1774</v>
       </c>
       <c r="C70" t="n">
         <v>1787</v>
       </c>
       <c r="D70" t="n">
-        <v>1762</v>
+        <v>1764</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G70" t="n">
-        <v>98.60100727476217</v>
+        <v>98.7129266927812</v>
       </c>
       <c r="H70" t="n">
-        <v>99.77349943374858</v>
+        <v>99.49238578680203</v>
       </c>
       <c r="I70" t="n">
-        <v>0.01622831561275881</v>
+        <v>0.01790710688304421</v>
       </c>
       <c r="J70" t="n">
-        <v>36.04430747032166</v>
+        <v>34.2352511882782</v>
       </c>
     </row>
     <row r="71">
@@ -2851,7 +2851,7 @@
         <v>0.01021059349074665</v>
       </c>
       <c r="J71" t="n">
-        <v>37.35191130638123</v>
+        <v>35.51220679283142</v>
       </c>
     </row>
     <row r="72">
@@ -2861,31 +2861,31 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="C72" t="n">
         <v>920</v>
       </c>
       <c r="D72" t="n">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="E72" t="n">
         <v>1</v>
       </c>
       <c r="F72" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G72" t="n">
-        <v>99.34711643090316</v>
+        <v>99.67355821545158</v>
       </c>
       <c r="H72" t="n">
-        <v>99.89059080962801</v>
+        <v>99.89094874591058</v>
       </c>
       <c r="I72" t="n">
-        <v>0.007608695652173913</v>
+        <v>0.004347826086956522</v>
       </c>
       <c r="J72" t="n">
-        <v>45.81126403808594</v>
+        <v>43.70300555229187</v>
       </c>
     </row>
     <row r="73">
@@ -2895,31 +2895,31 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1165</v>
+        <v>1174</v>
       </c>
       <c r="C73" t="n">
         <v>1143</v>
       </c>
       <c r="D73" t="n">
-        <v>1123</v>
+        <v>1126</v>
       </c>
       <c r="E73" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F73" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G73" t="n">
-        <v>98.33625218914186</v>
+        <v>98.59894921190893</v>
       </c>
       <c r="H73" t="n">
-        <v>96.47766323024055</v>
+        <v>95.99317988064792</v>
       </c>
       <c r="I73" t="n">
-        <v>0.05249343832020997</v>
+        <v>0.05511811023622047</v>
       </c>
       <c r="J73" t="n">
-        <v>40.22099614143372</v>
+        <v>38.77855539321899</v>
       </c>
     </row>
     <row r="74">
@@ -2929,31 +2929,31 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1250</v>
+        <v>1354</v>
       </c>
       <c r="C74" t="n">
         <v>1356</v>
       </c>
       <c r="D74" t="n">
-        <v>1247</v>
+        <v>1337</v>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F74" t="n">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="G74" t="n">
-        <v>92.02952029520296</v>
+        <v>98.67158671586716</v>
       </c>
       <c r="H74" t="n">
-        <v>99.83987189751801</v>
+        <v>98.81744271988174</v>
       </c>
       <c r="I74" t="n">
-        <v>0.08112094395280237</v>
+        <v>0.02507374631268437</v>
       </c>
       <c r="J74" t="n">
-        <v>42.86761617660522</v>
+        <v>40.76824235916138</v>
       </c>
     </row>
     <row r="75">
@@ -2963,31 +2963,31 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="C75" t="n">
         <v>543</v>
       </c>
       <c r="D75" t="n">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G75" t="n">
-        <v>98.70848708487085</v>
+        <v>99.2619926199262</v>
       </c>
       <c r="H75" t="n">
         <v>100</v>
       </c>
       <c r="I75" t="n">
-        <v>0.01289134438305709</v>
+        <v>0.007366482504604052</v>
       </c>
       <c r="J75" t="n">
-        <v>46.21938848495483</v>
+        <v>44.08605766296387</v>
       </c>
     </row>
     <row r="76">
@@ -2997,31 +2997,31 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1972</v>
+        <v>1974</v>
       </c>
       <c r="C76" t="n">
         <v>2025</v>
       </c>
       <c r="D76" t="n">
-        <v>1971</v>
+        <v>1973</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G76" t="n">
-        <v>97.38142292490119</v>
+        <v>97.4802371541502</v>
       </c>
       <c r="H76" t="n">
         <v>100</v>
       </c>
       <c r="I76" t="n">
-        <v>0.02617283950617284</v>
+        <v>0.02518518518518519</v>
       </c>
       <c r="J76" t="n">
-        <v>38.40941786766052</v>
+        <v>36.9289391040802</v>
       </c>
     </row>
     <row r="77">
@@ -3055,7 +3055,7 @@
         <v>0.0004662004662004662</v>
       </c>
       <c r="J77" t="n">
-        <v>41.5780668258667</v>
+        <v>40.01207065582275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
considering the absolute values of the slopes when eliminating T waves
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/AHA_database.xlsx
+++ b/R peak detection/beatdetection/AHA_database.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="gcgdcd" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="dhfsdf" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1649</v>
+        <v>1695</v>
       </c>
       <c r="C1" t="n">
         <v>1622</v>
@@ -456,7 +456,7 @@
         <v>1620</v>
       </c>
       <c r="E1" t="n">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="F1" t="n">
         <v>1</v>
@@ -465,13 +465,13 @@
         <v>99.93830968537939</v>
       </c>
       <c r="H1" t="n">
-        <v>98.30097087378641</v>
+        <v>95.63164108618655</v>
       </c>
       <c r="I1" t="n">
-        <v>0.01787916152897657</v>
+        <v>0.04623921085080148</v>
       </c>
       <c r="J1" t="n">
-        <v>51.80201888084412</v>
+        <v>51.17394638061523</v>
       </c>
     </row>
     <row r="2">
@@ -505,7 +505,7 @@
         <v>0.0003853564547206166</v>
       </c>
       <c r="J2" t="n">
-        <v>36.14297819137573</v>
+        <v>37.53673219680786</v>
       </c>
     </row>
     <row r="3">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2184</v>
+        <v>2183</v>
       </c>
       <c r="C3" t="n">
         <v>2181</v>
@@ -524,7 +524,7 @@
         <v>2180</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -533,13 +533,13 @@
         <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>99.86257443884563</v>
+        <v>99.9083409715857</v>
       </c>
       <c r="I3" t="n">
-        <v>0.001375515818431912</v>
+        <v>0.0009170105456212746</v>
       </c>
       <c r="J3" t="n">
-        <v>43.53279399871826</v>
+        <v>44.39185690879822</v>
       </c>
     </row>
     <row r="4">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2942</v>
+        <v>2943</v>
       </c>
       <c r="C4" t="n">
         <v>2974</v>
@@ -558,7 +558,7 @@
         <v>2940</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>33</v>
@@ -567,13 +567,13 @@
         <v>98.89001009081736</v>
       </c>
       <c r="H4" t="n">
-        <v>99.9659979598776</v>
+        <v>99.93201903467029</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01143241425689307</v>
+        <v>0.01176866173503699</v>
       </c>
       <c r="J4" t="n">
-        <v>37.08592486381531</v>
+        <v>38.31153011322021</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>42.92649984359741</v>
+        <v>44.37205862998962</v>
       </c>
     </row>
     <row r="6">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="C6" t="n">
         <v>2122</v>
@@ -626,7 +626,7 @@
         <v>2121</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -635,13 +635,13 @@
         <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>99.95287464655985</v>
+        <v>100</v>
       </c>
       <c r="I6" t="n">
-        <v>0.000471253534401508</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>40.64820408821106</v>
+        <v>42.59914469718933</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>41.25562477111816</v>
+        <v>41.48567795753479</v>
       </c>
     </row>
     <row r="8">
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>38.93723320960999</v>
+        <v>39.05715894699097</v>
       </c>
     </row>
     <row r="9">
@@ -743,7 +743,7 @@
         <v>0.0005583472920156337</v>
       </c>
       <c r="J9" t="n">
-        <v>29.80377221107483</v>
+        <v>30.62437701225281</v>
       </c>
     </row>
     <row r="10">
@@ -753,7 +753,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2093</v>
+        <v>2072</v>
       </c>
       <c r="C10" t="n">
         <v>1997</v>
@@ -762,7 +762,7 @@
         <v>1991</v>
       </c>
       <c r="E10" t="n">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="F10" t="n">
         <v>5</v>
@@ -771,13 +771,13 @@
         <v>99.74949899799599</v>
       </c>
       <c r="H10" t="n">
-        <v>95.17208413001912</v>
+        <v>96.13713182037662</v>
       </c>
       <c r="I10" t="n">
-        <v>0.05307961942914372</v>
+        <v>0.04256384576865298</v>
       </c>
       <c r="J10" t="n">
-        <v>48.99442291259766</v>
+        <v>49.68859601020813</v>
       </c>
     </row>
     <row r="11">
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>31.32786560058594</v>
+        <v>31.48810243606567</v>
       </c>
     </row>
     <row r="12">
@@ -845,7 +845,7 @@
         <v>0.0004142502071251035</v>
       </c>
       <c r="J12" t="n">
-        <v>41.34808969497681</v>
+        <v>41.30621552467346</v>
       </c>
     </row>
     <row r="13">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1644</v>
+        <v>1646</v>
       </c>
       <c r="C13" t="n">
         <v>1628</v>
@@ -864,7 +864,7 @@
         <v>1627</v>
       </c>
       <c r="E13" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -873,13 +873,13 @@
         <v>100</v>
       </c>
       <c r="H13" t="n">
-        <v>99.02617163724894</v>
+        <v>98.90577507598785</v>
       </c>
       <c r="I13" t="n">
-        <v>0.009828009828009828</v>
+        <v>0.01105651105651106</v>
       </c>
       <c r="J13" t="n">
-        <v>38.94654536247253</v>
+        <v>38.97719073295593</v>
       </c>
     </row>
     <row r="14">
@@ -889,7 +889,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="C14" t="n">
         <v>1613</v>
@@ -898,7 +898,7 @@
         <v>1612</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -907,13 +907,13 @@
         <v>100</v>
       </c>
       <c r="H14" t="n">
-        <v>99.93800371977682</v>
+        <v>99.87608426270137</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0006199628022318661</v>
+        <v>0.001239925604463732</v>
       </c>
       <c r="J14" t="n">
-        <v>46.78748941421509</v>
+        <v>47.19957232475281</v>
       </c>
     </row>
     <row r="15">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>34.60554480552673</v>
+        <v>35.22078013420105</v>
       </c>
     </row>
     <row r="16">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>34.0259096622467</v>
+        <v>36.49293518066406</v>
       </c>
     </row>
     <row r="17">
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>38.52973246574402</v>
+        <v>38.84084963798523</v>
       </c>
     </row>
     <row r="18">
@@ -1025,31 +1025,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2545</v>
+        <v>2540</v>
       </c>
       <c r="C18" t="n">
         <v>2537</v>
       </c>
       <c r="D18" t="n">
-        <v>2534</v>
+        <v>2532</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F18" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G18" t="n">
-        <v>99.9211356466877</v>
+        <v>99.84227129337539</v>
       </c>
       <c r="H18" t="n">
-        <v>99.60691823899371</v>
+        <v>99.72430090586845</v>
       </c>
       <c r="I18" t="n">
-        <v>0.004729996058336618</v>
+        <v>0.004335829720141899</v>
       </c>
       <c r="J18" t="n">
-        <v>48.39543032646179</v>
+        <v>49.98954153060913</v>
       </c>
     </row>
     <row r="19">
@@ -1083,7 +1083,7 @@
         <v>0.002296738631143776</v>
       </c>
       <c r="J19" t="n">
-        <v>45.08687710762024</v>
+        <v>46.18350005149841</v>
       </c>
     </row>
     <row r="20">
@@ -1093,31 +1093,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="C20" t="n">
         <v>2943</v>
       </c>
       <c r="D20" t="n">
-        <v>2942</v>
+        <v>2941</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>100</v>
+        <v>99.96600951733515</v>
       </c>
       <c r="H20" t="n">
         <v>100</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>0.0003397893306150187</v>
       </c>
       <c r="J20" t="n">
-        <v>41.07108497619629</v>
+        <v>41.71847486495972</v>
       </c>
     </row>
     <row r="21">
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="C21" t="n">
         <v>1950</v>
@@ -1136,7 +1136,7 @@
         <v>1949</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -1145,13 +1145,13 @@
         <v>100</v>
       </c>
       <c r="H21" t="n">
-        <v>99.69309462915601</v>
+        <v>99.79518689196108</v>
       </c>
       <c r="I21" t="n">
-        <v>0.003076923076923077</v>
+        <v>0.002051282051282051</v>
       </c>
       <c r="J21" t="n">
-        <v>40.2023823261261</v>
+        <v>41.29077005386353</v>
       </c>
     </row>
     <row r="22">
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1878</v>
+        <v>1879</v>
       </c>
       <c r="C22" t="n">
         <v>1878</v>
@@ -1170,7 +1170,7 @@
         <v>1877</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1179,13 +1179,13 @@
         <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>100</v>
+        <v>99.94675186368477</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>0.0005324813631522897</v>
       </c>
       <c r="J22" t="n">
-        <v>47.81577086448669</v>
+        <v>48.27675914764404</v>
       </c>
     </row>
     <row r="23">
@@ -1195,7 +1195,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1784</v>
+        <v>1782</v>
       </c>
       <c r="C23" t="n">
         <v>1784</v>
@@ -1204,7 +1204,7 @@
         <v>1781</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
         <v>2</v>
@@ -1213,13 +1213,13 @@
         <v>99.88782950084128</v>
       </c>
       <c r="H23" t="n">
-        <v>99.88782950084128</v>
+        <v>100</v>
       </c>
       <c r="I23" t="n">
-        <v>0.002242152466367713</v>
+        <v>0.001121076233183856</v>
       </c>
       <c r="J23" t="n">
-        <v>41.88349318504333</v>
+        <v>42.45736384391785</v>
       </c>
     </row>
     <row r="24">
@@ -1235,25 +1235,25 @@
         <v>3245</v>
       </c>
       <c r="D24" t="n">
-        <v>3244</v>
+        <v>3243</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>100</v>
+        <v>99.9691738594328</v>
       </c>
       <c r="H24" t="n">
-        <v>100</v>
+        <v>99.9691738594328</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>0.0006163328197226503</v>
       </c>
       <c r="J24" t="n">
-        <v>32.68469858169556</v>
+        <v>32.96350383758545</v>
       </c>
     </row>
     <row r="25">
@@ -1287,7 +1287,7 @@
         <v>0.0004302925989672978</v>
       </c>
       <c r="J25" t="n">
-        <v>42.26104235649109</v>
+        <v>42.97075223922729</v>
       </c>
     </row>
     <row r="26">
@@ -1321,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>41.69298315048218</v>
+        <v>42.29809617996216</v>
       </c>
     </row>
     <row r="27">
@@ -1331,7 +1331,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="C27" t="n">
         <v>2584</v>
@@ -1340,7 +1340,7 @@
         <v>2583</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1349,13 +1349,13 @@
         <v>100</v>
       </c>
       <c r="H27" t="n">
-        <v>99.88399071925754</v>
+        <v>99.92263056092844</v>
       </c>
       <c r="I27" t="n">
-        <v>0.001160990712074303</v>
+        <v>0.0007739938080495357</v>
       </c>
       <c r="J27" t="n">
-        <v>40.94000577926636</v>
+        <v>41.33864736557007</v>
       </c>
     </row>
     <row r="28">
@@ -1371,25 +1371,25 @@
         <v>2472</v>
       </c>
       <c r="D28" t="n">
-        <v>2447</v>
+        <v>2448</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G28" t="n">
-        <v>99.0287333063537</v>
+        <v>99.0692027519223</v>
       </c>
       <c r="H28" t="n">
-        <v>99.95915032679738</v>
+        <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>0.01011326860841424</v>
+        <v>0.009304207119741101</v>
       </c>
       <c r="J28" t="n">
-        <v>35.63106942176819</v>
+        <v>35.59612011909485</v>
       </c>
     </row>
     <row r="29">
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>41.40298676490784</v>
+        <v>41.66688370704651</v>
       </c>
     </row>
     <row r="30">
@@ -1433,31 +1433,31 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2368</v>
+        <v>2371</v>
       </c>
       <c r="C30" t="n">
         <v>2376</v>
       </c>
       <c r="D30" t="n">
-        <v>2366</v>
+        <v>2369</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G30" t="n">
-        <v>99.62105263157895</v>
+        <v>99.74736842105263</v>
       </c>
       <c r="H30" t="n">
-        <v>99.95775242923531</v>
+        <v>99.957805907173</v>
       </c>
       <c r="I30" t="n">
-        <v>0.004208754208754209</v>
+        <v>0.002946127946127946</v>
       </c>
       <c r="J30" t="n">
-        <v>38.32140374183655</v>
+        <v>39.39181303977966</v>
       </c>
     </row>
     <row r="31">
@@ -1467,31 +1467,31 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="C31" t="n">
         <v>2582</v>
       </c>
       <c r="D31" t="n">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" t="n">
-        <v>100</v>
+        <v>99.96125532739248</v>
       </c>
       <c r="H31" t="n">
         <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>0.0003872966692486445</v>
       </c>
       <c r="J31" t="n">
-        <v>41.7340190410614</v>
+        <v>42.0978901386261</v>
       </c>
     </row>
     <row r="32">
@@ -1525,7 +1525,7 @@
         <v>0.0004428697962798937</v>
       </c>
       <c r="J32" t="n">
-        <v>35.86098217964172</v>
+        <v>35.74618697166443</v>
       </c>
     </row>
     <row r="33">
@@ -1541,25 +1541,25 @@
         <v>1452</v>
       </c>
       <c r="D33" t="n">
-        <v>1441</v>
+        <v>1445</v>
       </c>
       <c r="E33" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F33" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G33" t="n">
-        <v>99.31082012405238</v>
+        <v>99.58649207443143</v>
       </c>
       <c r="H33" t="n">
-        <v>99.51657458563535</v>
+        <v>99.79281767955801</v>
       </c>
       <c r="I33" t="n">
-        <v>0.01170798898071625</v>
+        <v>0.006198347107438017</v>
       </c>
       <c r="J33" t="n">
-        <v>48.61842823028564</v>
+        <v>49.61659455299377</v>
       </c>
     </row>
     <row r="34">
@@ -1569,31 +1569,31 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1942</v>
+        <v>1945</v>
       </c>
       <c r="C34" t="n">
         <v>1947</v>
       </c>
       <c r="D34" t="n">
-        <v>1940</v>
+        <v>1944</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G34" t="n">
-        <v>99.69167523124358</v>
+        <v>99.89722507708119</v>
       </c>
       <c r="H34" t="n">
-        <v>99.94848016486347</v>
+        <v>100</v>
       </c>
       <c r="I34" t="n">
-        <v>0.00359527478171546</v>
+        <v>0.001027221366204417</v>
       </c>
       <c r="J34" t="n">
-        <v>37.76836824417114</v>
+        <v>38.15952491760254</v>
       </c>
     </row>
     <row r="35">
@@ -1603,31 +1603,31 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3520</v>
+        <v>3518</v>
       </c>
       <c r="C35" t="n">
         <v>3520</v>
       </c>
       <c r="D35" t="n">
-        <v>3519</v>
+        <v>3515</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G35" t="n">
-        <v>100</v>
+        <v>99.88633134413186</v>
       </c>
       <c r="H35" t="n">
-        <v>100</v>
+        <v>99.94313335228888</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>0.001704545454545454</v>
       </c>
       <c r="J35" t="n">
-        <v>31.67954182624817</v>
+        <v>32.81579232215881</v>
       </c>
     </row>
     <row r="36">
@@ -1661,7 +1661,7 @@
         <v>0.003727369542066028</v>
       </c>
       <c r="J36" t="n">
-        <v>40.97533845901489</v>
+        <v>41.41860818862915</v>
       </c>
     </row>
     <row r="37">
@@ -1671,7 +1671,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2368</v>
+        <v>2370</v>
       </c>
       <c r="C37" t="n">
         <v>2371</v>
@@ -1680,7 +1680,7 @@
         <v>2367</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37" t="n">
         <v>3</v>
@@ -1689,13 +1689,13 @@
         <v>99.87341772151899</v>
       </c>
       <c r="H37" t="n">
-        <v>100</v>
+        <v>99.91557619248628</v>
       </c>
       <c r="I37" t="n">
-        <v>0.00126528890763391</v>
+        <v>0.002108814846056516</v>
       </c>
       <c r="J37" t="n">
-        <v>43.59290957450867</v>
+        <v>44.667724609375</v>
       </c>
     </row>
     <row r="38">
@@ -1729,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>32.67426729202271</v>
+        <v>32.82728481292725</v>
       </c>
     </row>
     <row r="39">
@@ -1739,31 +1739,31 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2116</v>
+        <v>2145</v>
       </c>
       <c r="C39" t="n">
         <v>2257</v>
       </c>
       <c r="D39" t="n">
-        <v>2115</v>
+        <v>2144</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="G39" t="n">
-        <v>93.75</v>
+        <v>95.0354609929078</v>
       </c>
       <c r="H39" t="n">
         <v>100</v>
       </c>
       <c r="I39" t="n">
-        <v>0.06247230837394772</v>
+        <v>0.04962339388568897</v>
       </c>
       <c r="J39" t="n">
-        <v>33.7508430480957</v>
+        <v>34.57963824272156</v>
       </c>
     </row>
     <row r="40">
@@ -1773,31 +1773,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="C40" t="n">
         <v>2351</v>
       </c>
       <c r="D40" t="n">
-        <v>2350</v>
+        <v>2319</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="G40" t="n">
-        <v>100</v>
+        <v>98.68085106382979</v>
       </c>
       <c r="H40" t="n">
-        <v>100</v>
+        <v>98.72286079182631</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>0.02594640578477244</v>
       </c>
       <c r="J40" t="n">
-        <v>42.74280428886414</v>
+        <v>41.59917092323303</v>
       </c>
     </row>
     <row r="41">
@@ -1831,7 +1831,7 @@
         <v>0.0004212299915754001</v>
       </c>
       <c r="J41" t="n">
-        <v>36.05034017562866</v>
+        <v>36.25950264930725</v>
       </c>
     </row>
     <row r="42">
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>38.995760679245</v>
+        <v>39.14421129226685</v>
       </c>
     </row>
     <row r="43">
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>42.68702483177185</v>
+        <v>42.84071111679077</v>
       </c>
     </row>
     <row r="44">
@@ -1909,7 +1909,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2080</v>
+        <v>2077</v>
       </c>
       <c r="C44" t="n">
         <v>2068</v>
@@ -1918,7 +1918,7 @@
         <v>2066</v>
       </c>
       <c r="E44" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -1927,13 +1927,13 @@
         <v>99.95162070633769</v>
       </c>
       <c r="H44" t="n">
-        <v>99.37469937469938</v>
+        <v>99.51830443159923</v>
       </c>
       <c r="I44" t="n">
-        <v>0.006769825918762089</v>
+        <v>0.005319148936170213</v>
       </c>
       <c r="J44" t="n">
-        <v>41.12486505508423</v>
+        <v>40.99813055992126</v>
       </c>
     </row>
     <row r="45">
@@ -1967,7 +1967,7 @@
         <v>0.0003421142661648991</v>
       </c>
       <c r="J45" t="n">
-        <v>36.41609668731689</v>
+        <v>35.97954940795898</v>
       </c>
     </row>
     <row r="46">
@@ -2001,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>43.96787643432617</v>
+        <v>43.88580989837646</v>
       </c>
     </row>
     <row r="47">
@@ -2035,7 +2035,7 @@
         <v>0.0009242144177449168</v>
       </c>
       <c r="J47" t="n">
-        <v>39.30252909660339</v>
+        <v>38.74785161018372</v>
       </c>
     </row>
     <row r="48">
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2170</v>
+        <v>2295</v>
       </c>
       <c r="C48" t="n">
         <v>2017</v>
@@ -2054,7 +2054,7 @@
         <v>2016</v>
       </c>
       <c r="E48" t="n">
-        <v>153</v>
+        <v>278</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -2063,13 +2063,13 @@
         <v>100</v>
       </c>
       <c r="H48" t="n">
-        <v>92.9460580912863</v>
+        <v>87.88142981691369</v>
       </c>
       <c r="I48" t="n">
-        <v>0.07585523054040655</v>
+        <v>0.1378284581060982</v>
       </c>
       <c r="J48" t="n">
-        <v>31.46282005310059</v>
+        <v>45.12385416030884</v>
       </c>
     </row>
     <row r="49">
@@ -2103,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>44.69621133804321</v>
+        <v>45.06470918655396</v>
       </c>
     </row>
     <row r="50">
@@ -2113,7 +2113,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1959</v>
+        <v>1953</v>
       </c>
       <c r="C50" t="n">
         <v>1953</v>
@@ -2122,7 +2122,7 @@
         <v>1952</v>
       </c>
       <c r="E50" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
@@ -2131,13 +2131,13 @@
         <v>100</v>
       </c>
       <c r="H50" t="n">
-        <v>99.69356486210418</v>
+        <v>100</v>
       </c>
       <c r="I50" t="n">
-        <v>0.003072196620583717</v>
+        <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>45.97582197189331</v>
+        <v>45.72856020927429</v>
       </c>
     </row>
     <row r="51">
@@ -2171,7 +2171,7 @@
         <v>0.0003706449221645663</v>
       </c>
       <c r="J51" t="n">
-        <v>39.76867842674255</v>
+        <v>39.43454504013062</v>
       </c>
     </row>
     <row r="52">
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>42.46607255935669</v>
+        <v>42.29803681373596</v>
       </c>
     </row>
     <row r="53">
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>45.16241669654846</v>
+        <v>44.70084118843079</v>
       </c>
     </row>
     <row r="54">
@@ -2249,7 +2249,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2778</v>
+        <v>2779</v>
       </c>
       <c r="C54" t="n">
         <v>2785</v>
@@ -2258,7 +2258,7 @@
         <v>2777</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
         <v>7</v>
@@ -2267,13 +2267,13 @@
         <v>99.7485632183908</v>
       </c>
       <c r="H54" t="n">
-        <v>100</v>
+        <v>99.96400287976962</v>
       </c>
       <c r="I54" t="n">
-        <v>0.002513464991023339</v>
+        <v>0.002872531418312388</v>
       </c>
       <c r="J54" t="n">
-        <v>32.17860245704651</v>
+        <v>32.08808016777039</v>
       </c>
     </row>
     <row r="55">
@@ -2307,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>43.16459894180298</v>
+        <v>43.1470582485199</v>
       </c>
     </row>
     <row r="56">
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>34.59283804893494</v>
+        <v>35.02522039413452</v>
       </c>
     </row>
     <row r="57">
@@ -2351,7 +2351,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2501</v>
+        <v>2502</v>
       </c>
       <c r="C57" t="n">
         <v>2500</v>
@@ -2360,7 +2360,7 @@
         <v>2499</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -2369,13 +2369,13 @@
         <v>100</v>
       </c>
       <c r="H57" t="n">
-        <v>99.95999999999999</v>
+        <v>99.92003198720512</v>
       </c>
       <c r="I57" t="n">
-        <v>0.0004</v>
+        <v>0.0008</v>
       </c>
       <c r="J57" t="n">
-        <v>42.58084058761597</v>
+        <v>42.72607159614563</v>
       </c>
     </row>
     <row r="58">
@@ -2385,31 +2385,31 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>3289</v>
+        <v>3284</v>
       </c>
       <c r="C58" t="n">
         <v>3289</v>
       </c>
       <c r="D58" t="n">
-        <v>3288</v>
+        <v>3283</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G58" t="n">
-        <v>100</v>
+        <v>99.84793187347933</v>
       </c>
       <c r="H58" t="n">
         <v>100</v>
       </c>
       <c r="I58" t="n">
-        <v>0</v>
+        <v>0.001520218911523259</v>
       </c>
       <c r="J58" t="n">
-        <v>34.45736837387085</v>
+        <v>34.31363940238953</v>
       </c>
     </row>
     <row r="59">
@@ -2419,31 +2419,31 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>3156</v>
+        <v>3157</v>
       </c>
       <c r="C59" t="n">
         <v>3164</v>
       </c>
       <c r="D59" t="n">
-        <v>3155</v>
+        <v>3156</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G59" t="n">
-        <v>99.7470755611761</v>
+        <v>99.77869111602908</v>
       </c>
       <c r="H59" t="n">
         <v>100</v>
       </c>
       <c r="I59" t="n">
-        <v>0.002528445006321113</v>
+        <v>0.002212389380530973</v>
       </c>
       <c r="J59" t="n">
-        <v>33.02324151992798</v>
+        <v>33.50030660629272</v>
       </c>
     </row>
     <row r="60">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>45.9486289024353</v>
+        <v>45.99365711212158</v>
       </c>
     </row>
     <row r="61">
@@ -2511,7 +2511,7 @@
         <v>0.0007895775759968417</v>
       </c>
       <c r="J61" t="n">
-        <v>33.84360384941101</v>
+        <v>34.21698999404907</v>
       </c>
     </row>
     <row r="62">
@@ -2521,31 +2521,31 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>1927</v>
+        <v>1924</v>
       </c>
       <c r="C62" t="n">
         <v>1927</v>
       </c>
       <c r="D62" t="n">
-        <v>1924</v>
+        <v>1922</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G62" t="n">
-        <v>99.89615784008308</v>
+        <v>99.79231568016614</v>
       </c>
       <c r="H62" t="n">
-        <v>99.89615784008308</v>
+        <v>99.9479979199168</v>
       </c>
       <c r="I62" t="n">
-        <v>0.002075765438505449</v>
+        <v>0.002594706798131811</v>
       </c>
       <c r="J62" t="n">
-        <v>35.12916111946106</v>
+        <v>35.28152418136597</v>
       </c>
     </row>
     <row r="63">
@@ -2555,31 +2555,31 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2450</v>
+        <v>2437</v>
       </c>
       <c r="C63" t="n">
         <v>2437</v>
       </c>
       <c r="D63" t="n">
-        <v>2432</v>
+        <v>2428</v>
       </c>
       <c r="E63" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F63" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G63" t="n">
-        <v>99.83579638752053</v>
+        <v>99.67159277504105</v>
       </c>
       <c r="H63" t="n">
-        <v>99.30583911800736</v>
+        <v>99.67159277504105</v>
       </c>
       <c r="I63" t="n">
-        <v>0.008617152236356175</v>
+        <v>0.006565449322938038</v>
       </c>
       <c r="J63" t="n">
-        <v>40.15875959396362</v>
+        <v>40.38345837593079</v>
       </c>
     </row>
     <row r="64">
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>40.16179823875427</v>
+        <v>40.36891484260559</v>
       </c>
     </row>
     <row r="65">
@@ -2623,31 +2623,31 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="C65" t="n">
         <v>2340</v>
       </c>
       <c r="D65" t="n">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="E65" t="n">
         <v>8</v>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G65" t="n">
-        <v>99.95724668661822</v>
+        <v>99.91449337323643</v>
       </c>
       <c r="H65" t="n">
-        <v>99.65899403239557</v>
+        <v>99.6588486140725</v>
       </c>
       <c r="I65" t="n">
-        <v>0.003846153846153846</v>
+        <v>0.004273504273504274</v>
       </c>
       <c r="J65" t="n">
-        <v>37.89919781684875</v>
+        <v>37.35435438156128</v>
       </c>
     </row>
     <row r="66">
@@ -2681,7 +2681,7 @@
         <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>40.45603013038635</v>
+        <v>40.55513024330139</v>
       </c>
     </row>
     <row r="67">
@@ -2691,31 +2691,31 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>2897</v>
+        <v>2894</v>
       </c>
       <c r="C67" t="n">
         <v>2897</v>
       </c>
       <c r="D67" t="n">
-        <v>2896</v>
+        <v>2889</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G67" t="n">
-        <v>100</v>
+        <v>99.75828729281768</v>
       </c>
       <c r="H67" t="n">
-        <v>100</v>
+        <v>99.86173522295195</v>
       </c>
       <c r="I67" t="n">
-        <v>0</v>
+        <v>0.003797031411805316</v>
       </c>
       <c r="J67" t="n">
-        <v>41.56116914749146</v>
+        <v>42.77412223815918</v>
       </c>
     </row>
     <row r="68">
@@ -2749,7 +2749,7 @@
         <v>0.001140901312036509</v>
       </c>
       <c r="J68" t="n">
-        <v>43.40285158157349</v>
+        <v>43.3324453830719</v>
       </c>
     </row>
     <row r="69">
@@ -2783,7 +2783,7 @@
         <v>0.002741603838245374</v>
       </c>
       <c r="J69" t="n">
-        <v>46.06160736083984</v>
+        <v>45.2323796749115</v>
       </c>
     </row>
     <row r="70">
@@ -2793,31 +2793,31 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>1774</v>
+        <v>1768</v>
       </c>
       <c r="C70" t="n">
         <v>1787</v>
       </c>
       <c r="D70" t="n">
-        <v>1764</v>
+        <v>1761</v>
       </c>
       <c r="E70" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F70" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G70" t="n">
-        <v>98.7129266927812</v>
+        <v>98.54504756575265</v>
       </c>
       <c r="H70" t="n">
-        <v>99.49238578680203</v>
+        <v>99.66044142614601</v>
       </c>
       <c r="I70" t="n">
         <v>0.01790710688304421</v>
       </c>
       <c r="J70" t="n">
-        <v>34.2352511882782</v>
+        <v>34.29248356819153</v>
       </c>
     </row>
     <row r="71">
@@ -2827,31 +2827,31 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1551</v>
+        <v>1536</v>
       </c>
       <c r="C71" t="n">
         <v>1567</v>
       </c>
       <c r="D71" t="n">
-        <v>1550</v>
+        <v>1535</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G71" t="n">
-        <v>98.97828863346105</v>
+        <v>98.02043422733078</v>
       </c>
       <c r="H71" t="n">
         <v>100</v>
       </c>
       <c r="I71" t="n">
-        <v>0.01021059349074665</v>
+        <v>0.01978302488832163</v>
       </c>
       <c r="J71" t="n">
-        <v>35.51220679283142</v>
+        <v>37.75248789787292</v>
       </c>
     </row>
     <row r="72">
@@ -2861,31 +2861,31 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="C72" t="n">
         <v>920</v>
       </c>
       <c r="D72" t="n">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="E72" t="n">
         <v>1</v>
       </c>
       <c r="F72" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G72" t="n">
-        <v>99.67355821545158</v>
+        <v>99.34711643090316</v>
       </c>
       <c r="H72" t="n">
-        <v>99.89094874591058</v>
+        <v>99.89059080962801</v>
       </c>
       <c r="I72" t="n">
-        <v>0.004347826086956522</v>
+        <v>0.007608695652173913</v>
       </c>
       <c r="J72" t="n">
-        <v>43.70300555229187</v>
+        <v>43.48759746551514</v>
       </c>
     </row>
     <row r="73">
@@ -2895,31 +2895,31 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1174</v>
+        <v>1178</v>
       </c>
       <c r="C73" t="n">
         <v>1143</v>
       </c>
       <c r="D73" t="n">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="E73" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F73" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G73" t="n">
-        <v>98.59894921190893</v>
+        <v>98.77408056042032</v>
       </c>
       <c r="H73" t="n">
-        <v>95.99317988064792</v>
+        <v>95.83687340696686</v>
       </c>
       <c r="I73" t="n">
         <v>0.05511811023622047</v>
       </c>
       <c r="J73" t="n">
-        <v>38.77855539321899</v>
+        <v>37.92223191261292</v>
       </c>
     </row>
     <row r="74">
@@ -2929,31 +2929,31 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1354</v>
+        <v>1339</v>
       </c>
       <c r="C74" t="n">
         <v>1356</v>
       </c>
       <c r="D74" t="n">
-        <v>1337</v>
+        <v>1321</v>
       </c>
       <c r="E74" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F74" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G74" t="n">
-        <v>98.67158671586716</v>
+        <v>97.49077490774907</v>
       </c>
       <c r="H74" t="n">
-        <v>98.81744271988174</v>
+        <v>98.72944693572497</v>
       </c>
       <c r="I74" t="n">
-        <v>0.02507374631268437</v>
+        <v>0.03761061946902655</v>
       </c>
       <c r="J74" t="n">
-        <v>40.76824235916138</v>
+        <v>41.73047757148743</v>
       </c>
     </row>
     <row r="75">
@@ -2987,7 +2987,7 @@
         <v>0.007366482504604052</v>
       </c>
       <c r="J75" t="n">
-        <v>44.08605766296387</v>
+        <v>43.8138279914856</v>
       </c>
     </row>
     <row r="76">
@@ -2997,31 +2997,31 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="C76" t="n">
         <v>2025</v>
       </c>
       <c r="D76" t="n">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G76" t="n">
-        <v>97.4802371541502</v>
+        <v>97.38142292490119</v>
       </c>
       <c r="H76" t="n">
         <v>100</v>
       </c>
       <c r="I76" t="n">
-        <v>0.02518518518518519</v>
+        <v>0.02617283950617284</v>
       </c>
       <c r="J76" t="n">
-        <v>36.9289391040802</v>
+        <v>38.53585410118103</v>
       </c>
     </row>
     <row r="77">
@@ -3055,7 +3055,7 @@
         <v>0.0004662004662004662</v>
       </c>
       <c r="J77" t="n">
-        <v>40.01207065582275</v>
+        <v>41.14851832389832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the slope comparison threshold to 1/3 and the RT interval to 380 ms
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/AHA_database.xlsx
+++ b/R peak detection/beatdetection/AHA_database.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="dhfsdf" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="swfwewfd" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1695</v>
+        <v>1691</v>
       </c>
       <c r="C1" t="n">
         <v>1622</v>
@@ -456,7 +456,7 @@
         <v>1620</v>
       </c>
       <c r="E1" t="n">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F1" t="n">
         <v>1</v>
@@ -465,13 +465,13 @@
         <v>99.93830968537939</v>
       </c>
       <c r="H1" t="n">
-        <v>95.63164108618655</v>
+        <v>95.85798816568047</v>
       </c>
       <c r="I1" t="n">
-        <v>0.04623921085080148</v>
+        <v>0.0437731196054254</v>
       </c>
       <c r="J1" t="n">
-        <v>51.17394638061523</v>
+        <v>51.03661918640137</v>
       </c>
     </row>
     <row r="2">
@@ -505,7 +505,7 @@
         <v>0.0003853564547206166</v>
       </c>
       <c r="J2" t="n">
-        <v>37.53673219680786</v>
+        <v>36.93914771080017</v>
       </c>
     </row>
     <row r="3">
@@ -539,7 +539,7 @@
         <v>0.0009170105456212746</v>
       </c>
       <c r="J3" t="n">
-        <v>44.39185690879822</v>
+        <v>44.37130188941956</v>
       </c>
     </row>
     <row r="4">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="C4" t="n">
         <v>2974</v>
@@ -558,7 +558,7 @@
         <v>2940</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>33</v>
@@ -567,13 +567,13 @@
         <v>98.89001009081736</v>
       </c>
       <c r="H4" t="n">
-        <v>99.93201903467029</v>
+        <v>99.9659979598776</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01176866173503699</v>
+        <v>0.01143241425689307</v>
       </c>
       <c r="J4" t="n">
-        <v>38.31153011322021</v>
+        <v>41.87565040588379</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>44.37205862998962</v>
+        <v>44.60436964035034</v>
       </c>
     </row>
     <row r="6">
@@ -641,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>42.59914469718933</v>
+        <v>43.40618181228638</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>41.48567795753479</v>
+        <v>42.04231452941895</v>
       </c>
     </row>
     <row r="8">
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>39.05715894699097</v>
+        <v>40.21286225318909</v>
       </c>
     </row>
     <row r="9">
@@ -743,7 +743,7 @@
         <v>0.0005583472920156337</v>
       </c>
       <c r="J9" t="n">
-        <v>30.62437701225281</v>
+        <v>30.53034400939941</v>
       </c>
     </row>
     <row r="10">
@@ -753,7 +753,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2072</v>
+        <v>2073</v>
       </c>
       <c r="C10" t="n">
         <v>1997</v>
@@ -762,7 +762,7 @@
         <v>1991</v>
       </c>
       <c r="E10" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F10" t="n">
         <v>5</v>
@@ -771,13 +771,13 @@
         <v>99.74949899799599</v>
       </c>
       <c r="H10" t="n">
-        <v>96.13713182037662</v>
+        <v>96.09073359073359</v>
       </c>
       <c r="I10" t="n">
-        <v>0.04256384576865298</v>
+        <v>0.04306459689534301</v>
       </c>
       <c r="J10" t="n">
-        <v>49.68859601020813</v>
+        <v>50.57822561264038</v>
       </c>
     </row>
     <row r="11">
@@ -787,31 +787,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2875</v>
+        <v>2874</v>
       </c>
       <c r="C11" t="n">
         <v>2875</v>
       </c>
       <c r="D11" t="n">
-        <v>2874</v>
+        <v>2873</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>100</v>
+        <v>99.9652052887961</v>
       </c>
       <c r="H11" t="n">
         <v>100</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>0.0003478260869565218</v>
       </c>
       <c r="J11" t="n">
-        <v>31.48810243606567</v>
+        <v>31.41887331008911</v>
       </c>
     </row>
     <row r="12">
@@ -845,7 +845,7 @@
         <v>0.0004142502071251035</v>
       </c>
       <c r="J12" t="n">
-        <v>41.30621552467346</v>
+        <v>41.96691012382507</v>
       </c>
     </row>
     <row r="13">
@@ -879,7 +879,7 @@
         <v>0.01105651105651106</v>
       </c>
       <c r="J13" t="n">
-        <v>38.97719073295593</v>
+        <v>39.74461460113525</v>
       </c>
     </row>
     <row r="14">
@@ -913,7 +913,7 @@
         <v>0.001239925604463732</v>
       </c>
       <c r="J14" t="n">
-        <v>47.19957232475281</v>
+        <v>49.02508592605591</v>
       </c>
     </row>
     <row r="15">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>35.22078013420105</v>
+        <v>36.06474256515503</v>
       </c>
     </row>
     <row r="16">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>36.49293518066406</v>
+        <v>37.9193913936615</v>
       </c>
     </row>
     <row r="17">
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>38.84084963798523</v>
+        <v>39.61196422576904</v>
       </c>
     </row>
     <row r="18">
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="C18" t="n">
         <v>2537</v>
@@ -1034,7 +1034,7 @@
         <v>2532</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>4</v>
@@ -1043,13 +1043,13 @@
         <v>99.84227129337539</v>
       </c>
       <c r="H18" t="n">
-        <v>99.72430090586845</v>
+        <v>99.76359338061465</v>
       </c>
       <c r="I18" t="n">
-        <v>0.004335829720141899</v>
+        <v>0.003941663381947182</v>
       </c>
       <c r="J18" t="n">
-        <v>49.98954153060913</v>
+        <v>50.16433310508728</v>
       </c>
     </row>
     <row r="19">
@@ -1083,7 +1083,7 @@
         <v>0.002296738631143776</v>
       </c>
       <c r="J19" t="n">
-        <v>46.18350005149841</v>
+        <v>46.6275806427002</v>
       </c>
     </row>
     <row r="20">
@@ -1093,31 +1093,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2942</v>
+        <v>2940</v>
       </c>
       <c r="C20" t="n">
         <v>2943</v>
       </c>
       <c r="D20" t="n">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G20" t="n">
-        <v>99.96600951733515</v>
+        <v>99.89802855200544</v>
       </c>
       <c r="H20" t="n">
         <v>100</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0003397893306150187</v>
+        <v>0.001019367991845056</v>
       </c>
       <c r="J20" t="n">
-        <v>41.71847486495972</v>
+        <v>42.57859110832214</v>
       </c>
     </row>
     <row r="21">
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1954</v>
+        <v>1955</v>
       </c>
       <c r="C21" t="n">
         <v>1950</v>
@@ -1136,7 +1136,7 @@
         <v>1949</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -1145,13 +1145,13 @@
         <v>100</v>
       </c>
       <c r="H21" t="n">
-        <v>99.79518689196108</v>
+        <v>99.74411463664278</v>
       </c>
       <c r="I21" t="n">
-        <v>0.002051282051282051</v>
+        <v>0.002564102564102564</v>
       </c>
       <c r="J21" t="n">
-        <v>41.29077005386353</v>
+        <v>41.69644474983215</v>
       </c>
     </row>
     <row r="22">
@@ -1185,7 +1185,7 @@
         <v>0.0005324813631522897</v>
       </c>
       <c r="J22" t="n">
-        <v>48.27675914764404</v>
+        <v>49.18008327484131</v>
       </c>
     </row>
     <row r="23">
@@ -1219,7 +1219,7 @@
         <v>0.001121076233183856</v>
       </c>
       <c r="J23" t="n">
-        <v>42.45736384391785</v>
+        <v>43.51635003089905</v>
       </c>
     </row>
     <row r="24">
@@ -1253,7 +1253,7 @@
         <v>0.0006163328197226503</v>
       </c>
       <c r="J24" t="n">
-        <v>32.96350383758545</v>
+        <v>33.82432150840759</v>
       </c>
     </row>
     <row r="25">
@@ -1287,7 +1287,7 @@
         <v>0.0004302925989672978</v>
       </c>
       <c r="J25" t="n">
-        <v>42.97075223922729</v>
+        <v>44.04618239402771</v>
       </c>
     </row>
     <row r="26">
@@ -1321,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>42.29809617996216</v>
+        <v>42.39572930335999</v>
       </c>
     </row>
     <row r="27">
@@ -1331,7 +1331,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2586</v>
+        <v>2587</v>
       </c>
       <c r="C27" t="n">
         <v>2584</v>
@@ -1340,7 +1340,7 @@
         <v>2583</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1349,13 +1349,13 @@
         <v>100</v>
       </c>
       <c r="H27" t="n">
-        <v>99.92263056092844</v>
+        <v>99.88399071925754</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0007739938080495357</v>
+        <v>0.001160990712074303</v>
       </c>
       <c r="J27" t="n">
-        <v>41.33864736557007</v>
+        <v>42.55039668083191</v>
       </c>
     </row>
     <row r="28">
@@ -1389,7 +1389,7 @@
         <v>0.009304207119741101</v>
       </c>
       <c r="J28" t="n">
-        <v>35.59612011909485</v>
+        <v>36.57597899436951</v>
       </c>
     </row>
     <row r="29">
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>41.66688370704651</v>
+        <v>42.62749004364014</v>
       </c>
     </row>
     <row r="30">
@@ -1457,7 +1457,7 @@
         <v>0.002946127946127946</v>
       </c>
       <c r="J30" t="n">
-        <v>39.39181303977966</v>
+        <v>40.26213145256042</v>
       </c>
     </row>
     <row r="31">
@@ -1491,7 +1491,7 @@
         <v>0.0003872966692486445</v>
       </c>
       <c r="J31" t="n">
-        <v>42.0978901386261</v>
+        <v>43.9177393913269</v>
       </c>
     </row>
     <row r="32">
@@ -1525,7 +1525,7 @@
         <v>0.0004428697962798937</v>
       </c>
       <c r="J32" t="n">
-        <v>35.74618697166443</v>
+        <v>36.42376589775085</v>
       </c>
     </row>
     <row r="33">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="C33" t="n">
         <v>1452</v>
@@ -1544,7 +1544,7 @@
         <v>1445</v>
       </c>
       <c r="E33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" t="n">
         <v>6</v>
@@ -1553,13 +1553,13 @@
         <v>99.58649207443143</v>
       </c>
       <c r="H33" t="n">
-        <v>99.79281767955801</v>
+        <v>99.86178299930891</v>
       </c>
       <c r="I33" t="n">
-        <v>0.006198347107438017</v>
+        <v>0.005509641873278237</v>
       </c>
       <c r="J33" t="n">
-        <v>49.61659455299377</v>
+        <v>50.54662680625916</v>
       </c>
     </row>
     <row r="34">
@@ -1593,7 +1593,7 @@
         <v>0.001027221366204417</v>
       </c>
       <c r="J34" t="n">
-        <v>38.15952491760254</v>
+        <v>39.48422980308533</v>
       </c>
     </row>
     <row r="35">
@@ -1603,31 +1603,31 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3518</v>
+        <v>3500</v>
       </c>
       <c r="C35" t="n">
         <v>3520</v>
       </c>
       <c r="D35" t="n">
-        <v>3515</v>
+        <v>3497</v>
       </c>
       <c r="E35" t="n">
         <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G35" t="n">
-        <v>99.88633134413186</v>
+        <v>99.37482239272521</v>
       </c>
       <c r="H35" t="n">
-        <v>99.94313335228888</v>
+        <v>99.94284081166047</v>
       </c>
       <c r="I35" t="n">
-        <v>0.001704545454545454</v>
+        <v>0.006818181818181818</v>
       </c>
       <c r="J35" t="n">
-        <v>32.81579232215881</v>
+        <v>32.82644605636597</v>
       </c>
     </row>
     <row r="36">
@@ -1661,7 +1661,7 @@
         <v>0.003727369542066028</v>
       </c>
       <c r="J36" t="n">
-        <v>41.41860818862915</v>
+        <v>42.92876696586609</v>
       </c>
     </row>
     <row r="37">
@@ -1695,7 +1695,7 @@
         <v>0.002108814846056516</v>
       </c>
       <c r="J37" t="n">
-        <v>44.667724609375</v>
+        <v>46.87474322319031</v>
       </c>
     </row>
     <row r="38">
@@ -1729,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>32.82728481292725</v>
+        <v>33.8890917301178</v>
       </c>
     </row>
     <row r="39">
@@ -1739,31 +1739,31 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2145</v>
+        <v>2070</v>
       </c>
       <c r="C39" t="n">
         <v>2257</v>
       </c>
       <c r="D39" t="n">
-        <v>2144</v>
+        <v>2069</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>112</v>
+        <v>187</v>
       </c>
       <c r="G39" t="n">
-        <v>95.0354609929078</v>
+        <v>91.71099290780141</v>
       </c>
       <c r="H39" t="n">
         <v>100</v>
       </c>
       <c r="I39" t="n">
-        <v>0.04962339388568897</v>
+        <v>0.08285334514842711</v>
       </c>
       <c r="J39" t="n">
-        <v>34.57963824272156</v>
+        <v>34.50550580024719</v>
       </c>
     </row>
     <row r="40">
@@ -1773,31 +1773,31 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2350</v>
+        <v>2279</v>
       </c>
       <c r="C40" t="n">
         <v>2351</v>
       </c>
       <c r="D40" t="n">
-        <v>2319</v>
+        <v>2248</v>
       </c>
       <c r="E40" t="n">
         <v>30</v>
       </c>
       <c r="F40" t="n">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="G40" t="n">
-        <v>98.68085106382979</v>
+        <v>95.65957446808511</v>
       </c>
       <c r="H40" t="n">
-        <v>98.72286079182631</v>
+        <v>98.68305531167691</v>
       </c>
       <c r="I40" t="n">
-        <v>0.02594640578477244</v>
+        <v>0.05614632071458953</v>
       </c>
       <c r="J40" t="n">
-        <v>41.59917092323303</v>
+        <v>39.72537088394165</v>
       </c>
     </row>
     <row r="41">
@@ -1831,7 +1831,7 @@
         <v>0.0004212299915754001</v>
       </c>
       <c r="J41" t="n">
-        <v>36.25950264930725</v>
+        <v>37.52414703369141</v>
       </c>
     </row>
     <row r="42">
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>39.14421129226685</v>
+        <v>39.75350856781006</v>
       </c>
     </row>
     <row r="43">
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>42.84071111679077</v>
+        <v>44.16143321990967</v>
       </c>
     </row>
     <row r="44">
@@ -1933,7 +1933,7 @@
         <v>0.005319148936170213</v>
       </c>
       <c r="J44" t="n">
-        <v>40.99813055992126</v>
+        <v>41.80450344085693</v>
       </c>
     </row>
     <row r="45">
@@ -1967,7 +1967,7 @@
         <v>0.0003421142661648991</v>
       </c>
       <c r="J45" t="n">
-        <v>35.97954940795898</v>
+        <v>37.31579780578613</v>
       </c>
     </row>
     <row r="46">
@@ -2001,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>43.88580989837646</v>
+        <v>47.26611304283142</v>
       </c>
     </row>
     <row r="47">
@@ -2035,7 +2035,7 @@
         <v>0.0009242144177449168</v>
       </c>
       <c r="J47" t="n">
-        <v>38.74785161018372</v>
+        <v>40.74874758720398</v>
       </c>
     </row>
     <row r="48">
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2295</v>
+        <v>2299</v>
       </c>
       <c r="C48" t="n">
         <v>2017</v>
@@ -2054,7 +2054,7 @@
         <v>2016</v>
       </c>
       <c r="E48" t="n">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -2063,13 +2063,13 @@
         <v>100</v>
       </c>
       <c r="H48" t="n">
-        <v>87.88142981691369</v>
+        <v>87.72845953002611</v>
       </c>
       <c r="I48" t="n">
-        <v>0.1378284581060982</v>
+        <v>0.1398116013882003</v>
       </c>
       <c r="J48" t="n">
-        <v>45.12385416030884</v>
+        <v>45.77669382095337</v>
       </c>
     </row>
     <row r="49">
@@ -2103,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>45.06470918655396</v>
+        <v>45.7607364654541</v>
       </c>
     </row>
     <row r="50">
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>45.72856020927429</v>
+        <v>47.01032614707947</v>
       </c>
     </row>
     <row r="51">
@@ -2171,7 +2171,7 @@
         <v>0.0003706449221645663</v>
       </c>
       <c r="J51" t="n">
-        <v>39.43454504013062</v>
+        <v>40.75990319252014</v>
       </c>
     </row>
     <row r="52">
@@ -2181,31 +2181,31 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2251</v>
+        <v>2250</v>
       </c>
       <c r="C52" t="n">
         <v>2251</v>
       </c>
       <c r="D52" t="n">
-        <v>2250</v>
+        <v>2249</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" t="n">
-        <v>100</v>
+        <v>99.95555555555555</v>
       </c>
       <c r="H52" t="n">
         <v>100</v>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>0.000444247001332741</v>
       </c>
       <c r="J52" t="n">
-        <v>42.29803681373596</v>
+        <v>43.28269004821777</v>
       </c>
     </row>
     <row r="53">
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>44.70084118843079</v>
+        <v>45.92657160758972</v>
       </c>
     </row>
     <row r="54">
@@ -2273,7 +2273,7 @@
         <v>0.002872531418312388</v>
       </c>
       <c r="J54" t="n">
-        <v>32.08808016777039</v>
+        <v>32.86650705337524</v>
       </c>
     </row>
     <row r="55">
@@ -2307,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>43.1470582485199</v>
+        <v>44.45862507820129</v>
       </c>
     </row>
     <row r="56">
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>35.02522039413452</v>
+        <v>36.32990980148315</v>
       </c>
     </row>
     <row r="57">
@@ -2375,7 +2375,7 @@
         <v>0.0008</v>
       </c>
       <c r="J57" t="n">
-        <v>42.72607159614563</v>
+        <v>45.01442265510559</v>
       </c>
     </row>
     <row r="58">
@@ -2409,7 +2409,7 @@
         <v>0.001520218911523259</v>
       </c>
       <c r="J58" t="n">
-        <v>34.31363940238953</v>
+        <v>35.28443479537964</v>
       </c>
     </row>
     <row r="59">
@@ -2443,7 +2443,7 @@
         <v>0.002212389380530973</v>
       </c>
       <c r="J59" t="n">
-        <v>33.50030660629272</v>
+        <v>34.69120335578918</v>
       </c>
     </row>
     <row r="60">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>45.99365711212158</v>
+        <v>48.14723420143127</v>
       </c>
     </row>
     <row r="61">
@@ -2511,7 +2511,7 @@
         <v>0.0007895775759968417</v>
       </c>
       <c r="J61" t="n">
-        <v>34.21698999404907</v>
+        <v>35.66426277160645</v>
       </c>
     </row>
     <row r="62">
@@ -2545,7 +2545,7 @@
         <v>0.002594706798131811</v>
       </c>
       <c r="J62" t="n">
-        <v>35.28152418136597</v>
+        <v>36.78492569923401</v>
       </c>
     </row>
     <row r="63">
@@ -2555,31 +2555,31 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2437</v>
+        <v>2438</v>
       </c>
       <c r="C63" t="n">
         <v>2437</v>
       </c>
       <c r="D63" t="n">
-        <v>2428</v>
+        <v>2429</v>
       </c>
       <c r="E63" t="n">
         <v>8</v>
       </c>
       <c r="F63" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G63" t="n">
-        <v>99.67159277504105</v>
+        <v>99.71264367816092</v>
       </c>
       <c r="H63" t="n">
-        <v>99.67159277504105</v>
+        <v>99.6717275338531</v>
       </c>
       <c r="I63" t="n">
-        <v>0.006565449322938038</v>
+        <v>0.006155108740254411</v>
       </c>
       <c r="J63" t="n">
-        <v>40.38345837593079</v>
+        <v>42.70380425453186</v>
       </c>
     </row>
     <row r="64">
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>40.36891484260559</v>
+        <v>42.12425804138184</v>
       </c>
     </row>
     <row r="65">
@@ -2647,7 +2647,7 @@
         <v>0.004273504273504274</v>
       </c>
       <c r="J65" t="n">
-        <v>37.35435438156128</v>
+        <v>38.60061264038086</v>
       </c>
     </row>
     <row r="66">
@@ -2681,7 +2681,7 @@
         <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>40.55513024330139</v>
+        <v>42.69251680374146</v>
       </c>
     </row>
     <row r="67">
@@ -2691,31 +2691,31 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>2894</v>
+        <v>2808</v>
       </c>
       <c r="C67" t="n">
         <v>2897</v>
       </c>
       <c r="D67" t="n">
-        <v>2889</v>
+        <v>2803</v>
       </c>
       <c r="E67" t="n">
         <v>4</v>
       </c>
       <c r="F67" t="n">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="G67" t="n">
-        <v>99.75828729281768</v>
+        <v>96.78867403314918</v>
       </c>
       <c r="H67" t="n">
-        <v>99.86173522295195</v>
+        <v>99.85749910936943</v>
       </c>
       <c r="I67" t="n">
-        <v>0.003797031411805316</v>
+        <v>0.03348291335864688</v>
       </c>
       <c r="J67" t="n">
-        <v>42.77412223815918</v>
+        <v>43.98487067222595</v>
       </c>
     </row>
     <row r="68">
@@ -2749,7 +2749,7 @@
         <v>0.001140901312036509</v>
       </c>
       <c r="J68" t="n">
-        <v>43.3324453830719</v>
+        <v>44.83152866363525</v>
       </c>
     </row>
     <row r="69">
@@ -2783,7 +2783,7 @@
         <v>0.002741603838245374</v>
       </c>
       <c r="J69" t="n">
-        <v>45.2323796749115</v>
+        <v>47.04738140106201</v>
       </c>
     </row>
     <row r="70">
@@ -2817,7 +2817,7 @@
         <v>0.01790710688304421</v>
       </c>
       <c r="J70" t="n">
-        <v>34.29248356819153</v>
+        <v>35.28760194778442</v>
       </c>
     </row>
     <row r="71">
@@ -2827,31 +2827,31 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1536</v>
+        <v>1530</v>
       </c>
       <c r="C71" t="n">
         <v>1567</v>
       </c>
       <c r="D71" t="n">
-        <v>1535</v>
+        <v>1529</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G71" t="n">
-        <v>98.02043422733078</v>
+        <v>97.63729246487867</v>
       </c>
       <c r="H71" t="n">
         <v>100</v>
       </c>
       <c r="I71" t="n">
-        <v>0.01978302488832163</v>
+        <v>0.02361199744735163</v>
       </c>
       <c r="J71" t="n">
-        <v>37.75248789787292</v>
+        <v>37.71228075027466</v>
       </c>
     </row>
     <row r="72">
@@ -2885,7 +2885,7 @@
         <v>0.007608695652173913</v>
       </c>
       <c r="J72" t="n">
-        <v>43.48759746551514</v>
+        <v>43.83773565292358</v>
       </c>
     </row>
     <row r="73">
@@ -2895,7 +2895,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C73" t="n">
         <v>1143</v>
@@ -2904,7 +2904,7 @@
         <v>1128</v>
       </c>
       <c r="E73" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F73" t="n">
         <v>14</v>
@@ -2913,13 +2913,13 @@
         <v>98.77408056042032</v>
       </c>
       <c r="H73" t="n">
-        <v>95.83687340696686</v>
+        <v>95.91836734693878</v>
       </c>
       <c r="I73" t="n">
-        <v>0.05511811023622047</v>
+        <v>0.0542432195975503</v>
       </c>
       <c r="J73" t="n">
-        <v>37.92223191261292</v>
+        <v>39.01833724975586</v>
       </c>
     </row>
     <row r="74">
@@ -2929,31 +2929,31 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1339</v>
+        <v>1327</v>
       </c>
       <c r="C74" t="n">
         <v>1356</v>
       </c>
       <c r="D74" t="n">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="E74" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F74" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G74" t="n">
-        <v>97.49077490774907</v>
+        <v>97.26937269372694</v>
       </c>
       <c r="H74" t="n">
-        <v>98.72944693572497</v>
+        <v>99.39668174962293</v>
       </c>
       <c r="I74" t="n">
-        <v>0.03761061946902655</v>
+        <v>0.0331858407079646</v>
       </c>
       <c r="J74" t="n">
-        <v>41.73047757148743</v>
+        <v>42.16090941429138</v>
       </c>
     </row>
     <row r="75">
@@ -2987,7 +2987,7 @@
         <v>0.007366482504604052</v>
       </c>
       <c r="J75" t="n">
-        <v>43.8138279914856</v>
+        <v>43.33949518203735</v>
       </c>
     </row>
     <row r="76">
@@ -2997,31 +2997,31 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="C76" t="n">
         <v>2025</v>
       </c>
       <c r="D76" t="n">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G76" t="n">
-        <v>97.38142292490119</v>
+        <v>97.33201581027669</v>
       </c>
       <c r="H76" t="n">
         <v>100</v>
       </c>
       <c r="I76" t="n">
-        <v>0.02617283950617284</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="J76" t="n">
-        <v>38.53585410118103</v>
+        <v>37.36109828948975</v>
       </c>
     </row>
     <row r="77">
@@ -3055,7 +3055,7 @@
         <v>0.0004662004662004662</v>
       </c>
       <c r="J77" t="n">
-        <v>41.14851832389832</v>
+        <v>40.39943909645081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>